<commit_message>
spring has on average more carbon than summer ??????????????????????????????????????
</commit_message>
<xml_diff>
--- a/Bed_Carbon/Carbon_Sediment_Samples.xlsx
+++ b/Bed_Carbon/Carbon_Sediment_Samples.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\huck4481\Documents\GitHub\La_Jara\Bed_Carbon\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F059A83B-46B5-45E4-A507-6BBC6374BAA9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCE6C479-6D5C-4962-AD0C-3E479EC01D7C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{797E201D-8F44-4DD9-9B42-7B8F6976B830}"/>
+    <workbookView xWindow="-25320" yWindow="195" windowWidth="25440" windowHeight="15390" activeTab="3" xr2:uid="{797E201D-8F44-4DD9-9B42-7B8F6976B830}"/>
   </bookViews>
   <sheets>
     <sheet name="All Samples" sheetId="1" r:id="rId1"/>
     <sheet name="Composite Samples" sheetId="2" r:id="rId2"/>
     <sheet name="Seasonal" sheetId="3" r:id="rId3"/>
+    <sheet name="Sheet1" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="715" uniqueCount="138">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="762" uniqueCount="142">
   <si>
     <t>Name</t>
   </si>
@@ -453,6 +454,18 @@
   <si>
     <t>Spring</t>
   </si>
+  <si>
+    <t>Down SP</t>
+  </si>
+  <si>
+    <t>Up SP</t>
+  </si>
+  <si>
+    <t>Up SM</t>
+  </si>
+  <si>
+    <t>Down SM</t>
+  </si>
 </sst>
 </file>
 
@@ -462,7 +475,7 @@
     <numFmt numFmtId="164" formatCode="0.0000"/>
     <numFmt numFmtId="165" formatCode="0.000"/>
   </numFmts>
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="9">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -807,7 +820,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="325">
+  <cellXfs count="331">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -1775,6 +1788,22 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="13" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -32278,20 +32307,20 @@
       <selection activeCell="O51" sqref="O51"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="18.7109375" customWidth="1"/>
-    <col min="2" max="2" width="14.85546875" customWidth="1"/>
-    <col min="9" max="9" width="13.42578125" customWidth="1"/>
-    <col min="10" max="10" width="16.42578125" style="32" customWidth="1"/>
-    <col min="11" max="11" width="15.85546875" customWidth="1"/>
-    <col min="12" max="12" width="10.28515625" customWidth="1"/>
-    <col min="13" max="13" width="17.7109375" customWidth="1"/>
-    <col min="14" max="14" width="16.7109375" customWidth="1"/>
-    <col min="15" max="15" width="11.5703125" customWidth="1"/>
+    <col min="1" max="1" width="18.75" customWidth="1"/>
+    <col min="2" max="2" width="14.875" customWidth="1"/>
+    <col min="9" max="9" width="13.375" customWidth="1"/>
+    <col min="10" max="10" width="16.375" style="32" customWidth="1"/>
+    <col min="11" max="11" width="15.875" customWidth="1"/>
+    <col min="12" max="12" width="10.25" customWidth="1"/>
+    <col min="13" max="13" width="17.75" customWidth="1"/>
+    <col min="14" max="14" width="16.75" customWidth="1"/>
+    <col min="15" max="15" width="11.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" ht="15">
       <c r="A1" s="20" t="s">
         <v>0</v>
       </c>
@@ -32329,7 +32358,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" ht="15">
       <c r="A2" s="2" t="s">
         <v>15</v>
       </c>
@@ -32369,7 +32398,7 @@
         <v>-7.7465857446808476E-4</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" ht="15">
       <c r="A3" s="2" t="s">
         <v>16</v>
       </c>
@@ -32409,7 +32438,7 @@
         <v>1.0369328240675921E-3</v>
       </c>
     </row>
-    <row r="4" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12" ht="15.75" thickBot="1">
       <c r="A4" s="104" t="s">
         <v>17</v>
       </c>
@@ -32449,7 +32478,7 @@
         <v>-1.8794106280126401E-3</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" ht="15">
       <c r="A5" s="113" t="s">
         <v>11</v>
       </c>
@@ -32489,7 +32518,7 @@
         <v>1.2061318035695877E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" ht="15">
       <c r="A6" s="51" t="s">
         <v>13</v>
       </c>
@@ -32529,7 +32558,7 @@
         <v>9.6894732532614507E-5</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" ht="15">
       <c r="A7" s="65" t="s">
         <v>10</v>
       </c>
@@ -32569,7 +32598,7 @@
         <v>1.1595263660704859E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" ht="15">
       <c r="A8" s="120" t="s">
         <v>12</v>
       </c>
@@ -32609,7 +32638,7 @@
         <v>1.7454287453069798E-3</v>
       </c>
     </row>
-    <row r="9" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:12" ht="15.75" thickBot="1">
       <c r="A9" s="139" t="s">
         <v>14</v>
       </c>
@@ -32649,7 +32678,7 @@
         <v>1.5683176995033121E-3</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" ht="15">
       <c r="A10" s="113" t="s">
         <v>20</v>
       </c>
@@ -32689,7 +32718,7 @@
         <v>1.3292377521363417E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" ht="15">
       <c r="A11" s="51" t="s">
         <v>18</v>
       </c>
@@ -32729,7 +32758,7 @@
         <v>1.0369517155732347E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" ht="15">
       <c r="A12" s="65" t="s">
         <v>21</v>
       </c>
@@ -32769,7 +32798,7 @@
         <v>6.8922560718681701E-4</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12" ht="15">
       <c r="A13" s="122" t="s">
         <v>19</v>
       </c>
@@ -32809,7 +32838,7 @@
         <v>1.0901794040645514E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12" ht="15">
       <c r="A14" s="120" t="s">
         <v>23</v>
       </c>
@@ -32849,7 +32878,7 @@
         <v>9.3291047016118983E-4</v>
       </c>
     </row>
-    <row r="15" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:12" ht="15.75" thickBot="1">
       <c r="A15" s="139" t="s">
         <v>22</v>
       </c>
@@ -32889,7 +32918,7 @@
         <v>1.9023096757851137E-3</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12" ht="15">
       <c r="A16" s="113" t="s">
         <v>25</v>
       </c>
@@ -32929,7 +32958,7 @@
         <v>2.5853732185710876E-3</v>
       </c>
     </row>
-    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:18" ht="15">
       <c r="A17" s="51" t="s">
         <v>26</v>
       </c>
@@ -32972,7 +33001,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="18" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:18" ht="15">
       <c r="A18" s="65" t="s">
         <v>27</v>
       </c>
@@ -33012,7 +33041,7 @@
         <v>1.6796037884212729E-3</v>
       </c>
     </row>
-    <row r="19" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:18" ht="15">
       <c r="A19" s="122" t="s">
         <v>24</v>
       </c>
@@ -33052,7 +33081,7 @@
         <v>7.1540883650046531E-4</v>
       </c>
     </row>
-    <row r="20" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:18" ht="15">
       <c r="A20" s="120" t="s">
         <v>29</v>
       </c>
@@ -33092,7 +33121,7 @@
         <v>-1.8964228261324385E-3</v>
       </c>
     </row>
-    <row r="21" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:18" ht="15.75" thickBot="1">
       <c r="A21" s="139" t="s">
         <v>28</v>
       </c>
@@ -33132,7 +33161,7 @@
         <v>-1.6027230326546356E-6</v>
       </c>
     </row>
-    <row r="22" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:18" ht="15">
       <c r="A22" s="57" t="s">
         <v>71</v>
       </c>
@@ -33172,7 +33201,7 @@
         <v>7.9439062617902049E-4</v>
       </c>
     </row>
-    <row r="23" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:18" ht="15">
       <c r="A23" s="22" t="s">
         <v>72</v>
       </c>
@@ -33212,7 +33241,7 @@
         <v>3.1474946120986233E-3</v>
       </c>
     </row>
-    <row r="24" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:18" ht="15">
       <c r="A24" s="124" t="s">
         <v>41</v>
       </c>
@@ -33252,7 +33281,7 @@
         <v>3.5392455522788207E-3</v>
       </c>
     </row>
-    <row r="25" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:18" ht="15.75" thickBot="1">
       <c r="A25" s="148" t="s">
         <v>42</v>
       </c>
@@ -33292,7 +33321,7 @@
         <v>2.1982702913497338E-3</v>
       </c>
     </row>
-    <row r="26" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:18" ht="15">
       <c r="A26" s="57" t="s">
         <v>48</v>
       </c>
@@ -33332,7 +33361,7 @@
         <v>3.9499744289269913E-3</v>
       </c>
     </row>
-    <row r="27" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:18" ht="15">
       <c r="A27" s="127" t="s">
         <v>53</v>
       </c>
@@ -33372,7 +33401,7 @@
         <v>1.2083477356246732E-3</v>
       </c>
     </row>
-    <row r="28" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:18" ht="15">
       <c r="A28" s="124" t="s">
         <v>46</v>
       </c>
@@ -33412,7 +33441,7 @@
         <v>2.3639572792721517E-3</v>
       </c>
     </row>
-    <row r="29" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:18" ht="15.75" thickBot="1">
       <c r="A29" s="148" t="s">
         <v>47</v>
       </c>
@@ -33452,7 +33481,7 @@
         <v>6.526587407184186E-3</v>
       </c>
     </row>
-    <row r="30" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:18" ht="15">
       <c r="A30" s="57" t="s">
         <v>49</v>
       </c>
@@ -33492,7 +33521,7 @@
         <v>2.6479190306808779E-3</v>
       </c>
     </row>
-    <row r="31" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:18" ht="15">
       <c r="A31" s="124" t="s">
         <v>50</v>
       </c>
@@ -33532,7 +33561,7 @@
         <v>3.6101488052774963E-3</v>
       </c>
     </row>
-    <row r="32" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:18" ht="15.75" thickBot="1">
       <c r="A32" s="148" t="s">
         <v>81</v>
       </c>
@@ -33572,7 +33601,7 @@
         <v>1.4840236413115042E-3</v>
       </c>
     </row>
-    <row r="33" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:19" ht="15">
       <c r="A33" s="57" t="s">
         <v>51</v>
       </c>
@@ -33612,7 +33641,7 @@
         <v>2.5049740815024095E-3</v>
       </c>
     </row>
-    <row r="34" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:19" ht="15">
       <c r="A34" s="124" t="s">
         <v>52</v>
       </c>
@@ -33652,7 +33681,7 @@
         <v>2.2584131632020919E-3</v>
       </c>
     </row>
-    <row r="35" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:19" ht="15">
       <c r="A35" s="156" t="s">
         <v>69</v>
       </c>
@@ -33713,7 +33742,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="36" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:19" ht="15.75" thickBot="1">
       <c r="A36" s="148" t="s">
         <v>70</v>
       </c>
@@ -33774,7 +33803,7 @@
         <v>1.2061318035695876</v>
       </c>
     </row>
-    <row r="37" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:19" ht="15">
       <c r="A37" s="39" t="s">
         <v>30</v>
       </c>
@@ -33835,7 +33864,7 @@
         <v>1.3292377521363417</v>
       </c>
     </row>
-    <row r="38" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:19" ht="15">
       <c r="A38" s="22" t="s">
         <v>33</v>
       </c>
@@ -33896,7 +33925,7 @@
         <v>0.25853732185710876</v>
       </c>
     </row>
-    <row r="39" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:19" ht="15">
       <c r="A39" s="127" t="s">
         <v>31</v>
       </c>
@@ -33957,7 +33986,7 @@
         <v>0.31264785061813194</v>
       </c>
     </row>
-    <row r="40" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:19" ht="15">
       <c r="A40" s="124" t="s">
         <v>32</v>
       </c>
@@ -34018,7 +34047,7 @@
         <v>0.43677241122731852</v>
       </c>
     </row>
-    <row r="41" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:19" ht="15.75" thickBot="1">
       <c r="A41" s="148" t="s">
         <v>34</v>
       </c>
@@ -34079,7 +34108,7 @@
         <v>0.21059542617589286</v>
       </c>
     </row>
-    <row r="42" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:19" ht="15">
       <c r="A42" s="39" t="s">
         <v>35</v>
       </c>
@@ -34140,7 +34169,7 @@
         <v>0.57748225761286209</v>
       </c>
     </row>
-    <row r="43" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:19" ht="15">
       <c r="A43" s="21" t="s">
         <v>36</v>
       </c>
@@ -34201,7 +34230,7 @@
         <v>0.36104776822195289</v>
       </c>
     </row>
-    <row r="44" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:19" ht="15">
       <c r="A44" s="22" t="s">
         <v>37</v>
       </c>
@@ -34262,7 +34291,7 @@
         <v>0.20694510467987184</v>
       </c>
     </row>
-    <row r="45" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:19" ht="15">
       <c r="A45" s="127" t="s">
         <v>38</v>
       </c>
@@ -34323,7 +34352,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="46" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:19" ht="15">
       <c r="A46" s="124" t="s">
         <v>39</v>
       </c>
@@ -34384,7 +34413,7 @@
         <v>9.6894732532614505E-3</v>
       </c>
     </row>
-    <row r="47" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:19" ht="15.75" thickBot="1">
       <c r="A47" s="148" t="s">
         <v>40</v>
       </c>
@@ -34445,7 +34474,7 @@
         <v>1.0369517155732346</v>
       </c>
     </row>
-    <row r="48" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:19" ht="15">
       <c r="A48" s="39" t="s">
         <v>54</v>
       </c>
@@ -34506,7 +34535,7 @@
         <v>0.17001195690658247</v>
       </c>
     </row>
-    <row r="49" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:19" ht="15">
       <c r="A49" s="21" t="s">
         <v>55</v>
       </c>
@@ -34567,7 +34596,7 @@
         <v>7.9439062617902054E-2</v>
       </c>
     </row>
-    <row r="50" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:19" ht="15">
       <c r="A50" s="22" t="s">
         <v>56</v>
       </c>
@@ -34628,7 +34657,7 @@
         <v>0.39499744289269911</v>
       </c>
     </row>
-    <row r="51" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:19" ht="15">
       <c r="A51" s="127" t="s">
         <v>57</v>
       </c>
@@ -34689,7 +34718,7 @@
         <v>0.26479190306808781</v>
       </c>
     </row>
-    <row r="52" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:19" ht="15">
       <c r="A52" s="124" t="s">
         <v>58</v>
       </c>
@@ -34750,7 +34779,7 @@
         <v>0.25049740815024096</v>
       </c>
     </row>
-    <row r="53" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:19" ht="15.75" thickBot="1">
       <c r="A53" s="148" t="s">
         <v>59</v>
       </c>
@@ -34811,7 +34840,7 @@
         <v>0.46536260865740742</v>
       </c>
     </row>
-    <row r="54" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:19" ht="15">
       <c r="A54" s="39" t="s">
         <v>63</v>
       </c>
@@ -34872,7 +34901,7 @@
         <v>0.19472956344905759</v>
       </c>
     </row>
-    <row r="55" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:19" ht="15">
       <c r="A55" s="21" t="s">
         <v>64</v>
       </c>
@@ -34933,7 +34962,7 @@
         <v>0.65076974205508487</v>
       </c>
     </row>
-    <row r="56" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:19" ht="15">
       <c r="A56" s="22" t="s">
         <v>65</v>
       </c>
@@ -34994,7 +35023,7 @@
         <v>0.44548279685085013</v>
       </c>
     </row>
-    <row r="57" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:19" ht="15">
       <c r="A57" s="127" t="s">
         <v>66</v>
       </c>
@@ -35055,7 +35084,7 @@
         <v>0.2271080936932702</v>
       </c>
     </row>
-    <row r="58" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:19" ht="15">
       <c r="A58" s="124" t="s">
         <v>67</v>
       </c>
@@ -35116,7 +35145,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="59" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:19" ht="15.75" thickBot="1">
       <c r="A59" s="148" t="s">
         <v>68</v>
       </c>
@@ -35177,7 +35206,7 @@
         <v>1.1595263660704858</v>
       </c>
     </row>
-    <row r="60" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:19" ht="15">
       <c r="A60" s="39" t="s">
         <v>60</v>
       </c>
@@ -35238,7 +35267,7 @@
         <v>6.8922560718681705E-2</v>
       </c>
     </row>
-    <row r="61" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:19" ht="15">
       <c r="A61" s="21" t="s">
         <v>61</v>
       </c>
@@ -35299,7 +35328,7 @@
         <v>0.16796037884212731</v>
       </c>
     </row>
-    <row r="62" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:19" ht="15">
       <c r="A62" s="22" t="s">
         <v>43</v>
       </c>
@@ -35360,7 +35389,7 @@
         <v>0.31474946120986236</v>
       </c>
     </row>
-    <row r="63" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:19" ht="15">
       <c r="A63" s="127" t="s">
         <v>62</v>
       </c>
@@ -35421,7 +35450,7 @@
         <v>0.7353482955121704</v>
       </c>
     </row>
-    <row r="64" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:19" ht="15">
       <c r="A64" s="124" t="s">
         <v>44</v>
       </c>
@@ -35482,7 +35511,7 @@
         <v>0.49469332371144475</v>
       </c>
     </row>
-    <row r="65" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:19" ht="15.75" thickBot="1">
       <c r="A65" s="148" t="s">
         <v>45</v>
       </c>
@@ -35543,7 +35572,7 @@
         <v>0.35001434001298215</v>
       </c>
     </row>
-    <row r="66" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:19" ht="15">
       <c r="A66" s="39" t="s">
         <v>76</v>
       </c>
@@ -35604,7 +35633,7 @@
         <v>0.65937849482304212</v>
       </c>
     </row>
-    <row r="67" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:19" ht="15">
       <c r="A67" s="21" t="s">
         <v>80</v>
       </c>
@@ -35665,7 +35694,7 @@
         <v>0.32405367652189609</v>
       </c>
     </row>
-    <row r="68" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:19" ht="15">
       <c r="A68" s="22" t="s">
         <v>77</v>
       </c>
@@ -35724,7 +35753,7 @@
         <v>0.80972320884986226</v>
       </c>
     </row>
-    <row r="69" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:19" ht="15">
       <c r="A69" s="127" t="s">
         <v>78</v>
       </c>
@@ -35764,7 +35793,7 @@
         <v>1.6948198261392141E-3</v>
       </c>
     </row>
-    <row r="70" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:19" ht="15.75" thickBot="1">
       <c r="A70" s="131" t="s">
         <v>79</v>
       </c>
@@ -35825,7 +35854,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="71" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:19" ht="15">
       <c r="M71" s="75" t="s">
         <v>19</v>
       </c>
@@ -35848,7 +35877,7 @@
         <v>1.0901794040645514</v>
       </c>
     </row>
-    <row r="72" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:19" ht="15">
       <c r="M72" s="84" t="s">
         <v>53</v>
       </c>
@@ -35871,7 +35900,7 @@
         <v>0.12083477356246732</v>
       </c>
     </row>
-    <row r="73" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:19" ht="15">
       <c r="M73" s="84" t="s">
         <v>31</v>
       </c>
@@ -35894,7 +35923,7 @@
         <v>0.57716289500423379</v>
       </c>
     </row>
-    <row r="74" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:19" ht="15">
       <c r="M74" s="84" t="s">
         <v>38</v>
       </c>
@@ -35917,7 +35946,7 @@
         <v>0.4188589299167082</v>
       </c>
     </row>
-    <row r="75" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:19" ht="15">
       <c r="M75" s="84" t="s">
         <v>57</v>
       </c>
@@ -35940,7 +35969,7 @@
         <v>0.33340865272307069</v>
       </c>
     </row>
-    <row r="76" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:19" ht="15">
       <c r="M76" s="84" t="s">
         <v>66</v>
       </c>
@@ -35963,7 +35992,7 @@
         <v>0.37687971199087078</v>
       </c>
     </row>
-    <row r="77" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:19" ht="15">
       <c r="M77" s="84" t="s">
         <v>62</v>
       </c>
@@ -35986,7 +36015,7 @@
         <v>0.19279147674361641</v>
       </c>
     </row>
-    <row r="78" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:19" ht="15">
       <c r="M78" s="84" t="s">
         <v>78</v>
       </c>
@@ -36009,7 +36038,7 @@
         <v>0.16948198261392142</v>
       </c>
     </row>
-    <row r="79" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:19" ht="15">
       <c r="M79" s="1" t="s">
         <v>0</v>
       </c>
@@ -36032,7 +36061,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="80" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:19" ht="15">
       <c r="M80" s="90" t="s">
         <v>12</v>
       </c>
@@ -36055,7 +36084,7 @@
         <v>0.17454287453069797</v>
       </c>
     </row>
-    <row r="81" spans="13:19" x14ac:dyDescent="0.25">
+    <row r="81" spans="13:19" ht="15">
       <c r="M81" s="90" t="s">
         <v>23</v>
       </c>
@@ -36078,7 +36107,7 @@
         <v>9.3291047016118983E-2</v>
       </c>
     </row>
-    <row r="82" spans="13:19" x14ac:dyDescent="0.25">
+    <row r="82" spans="13:19" ht="15">
       <c r="M82" s="90" t="s">
         <v>29</v>
       </c>
@@ -36101,7 +36130,7 @@
         <v>-0.18964228261324384</v>
       </c>
     </row>
-    <row r="83" spans="13:19" x14ac:dyDescent="0.25">
+    <row r="83" spans="13:19" ht="15">
       <c r="M83" s="99" t="s">
         <v>41</v>
       </c>
@@ -36124,7 +36153,7 @@
         <v>0.35392455522788208</v>
       </c>
     </row>
-    <row r="84" spans="13:19" x14ac:dyDescent="0.25">
+    <row r="84" spans="13:19" ht="15">
       <c r="M84" s="99" t="s">
         <v>46</v>
       </c>
@@ -36147,7 +36176,7 @@
         <v>0.23639572792721517</v>
       </c>
     </row>
-    <row r="85" spans="13:19" x14ac:dyDescent="0.25">
+    <row r="85" spans="13:19" ht="15">
       <c r="M85" s="99" t="s">
         <v>50</v>
       </c>
@@ -36170,7 +36199,7 @@
         <v>0.3610148805277496</v>
       </c>
     </row>
-    <row r="86" spans="13:19" x14ac:dyDescent="0.25">
+    <row r="86" spans="13:19" ht="15">
       <c r="M86" s="99" t="s">
         <v>52</v>
       </c>
@@ -36193,7 +36222,7 @@
         <v>0.22584131632020921</v>
       </c>
     </row>
-    <row r="87" spans="13:19" x14ac:dyDescent="0.25">
+    <row r="87" spans="13:19" ht="15">
       <c r="M87" s="99" t="s">
         <v>32</v>
       </c>
@@ -36216,7 +36245,7 @@
         <v>0.17044564966222317</v>
       </c>
     </row>
-    <row r="88" spans="13:19" x14ac:dyDescent="0.25">
+    <row r="88" spans="13:19" ht="15">
       <c r="M88" s="99" t="s">
         <v>39</v>
       </c>
@@ -36239,7 +36268,7 @@
         <v>0.28067760361842103</v>
       </c>
     </row>
-    <row r="89" spans="13:19" x14ac:dyDescent="0.25">
+    <row r="89" spans="13:19" ht="15">
       <c r="M89" s="99" t="s">
         <v>58</v>
       </c>
@@ -36262,7 +36291,7 @@
         <v>0.64814216875848041</v>
       </c>
     </row>
-    <row r="90" spans="13:19" x14ac:dyDescent="0.25">
+    <row r="90" spans="13:19" ht="15">
       <c r="M90" s="99" t="s">
         <v>67</v>
       </c>
@@ -36285,7 +36314,7 @@
         <v>0.27153190842331631</v>
       </c>
     </row>
-    <row r="91" spans="13:19" x14ac:dyDescent="0.25">
+    <row r="91" spans="13:19" ht="15">
       <c r="M91" s="99" t="s">
         <v>44</v>
       </c>
@@ -36308,7 +36337,7 @@
         <v>0.39384541446935828</v>
       </c>
     </row>
-    <row r="92" spans="13:19" x14ac:dyDescent="0.25">
+    <row r="92" spans="13:19" ht="15">
       <c r="M92" s="99" t="s">
         <v>79</v>
       </c>
@@ -36331,7 +36360,7 @@
         <v>0.36305354438579657</v>
       </c>
     </row>
-    <row r="93" spans="13:19" x14ac:dyDescent="0.25">
+    <row r="93" spans="13:19" ht="15">
       <c r="M93" s="1" t="s">
         <v>0</v>
       </c>
@@ -36354,7 +36383,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="94" spans="13:19" x14ac:dyDescent="0.25">
+    <row r="94" spans="13:19" ht="15">
       <c r="M94" s="165" t="s">
         <v>14</v>
       </c>
@@ -36377,7 +36406,7 @@
         <v>0.15683176995033121</v>
       </c>
     </row>
-    <row r="95" spans="13:19" x14ac:dyDescent="0.25">
+    <row r="95" spans="13:19" ht="15">
       <c r="M95" s="165" t="s">
         <v>22</v>
       </c>
@@ -36400,7 +36429,7 @@
         <v>0.19023096757851138</v>
       </c>
     </row>
-    <row r="96" spans="13:19" x14ac:dyDescent="0.25">
+    <row r="96" spans="13:19" ht="15">
       <c r="M96" s="165" t="s">
         <v>28</v>
       </c>
@@ -36423,7 +36452,7 @@
         <v>-1.6027230326546356E-4</v>
       </c>
     </row>
-    <row r="97" spans="13:19" x14ac:dyDescent="0.25">
+    <row r="97" spans="13:19" ht="15">
       <c r="M97" s="157" t="s">
         <v>42</v>
       </c>
@@ -36446,7 +36475,7 @@
         <v>0.21982702913497337</v>
       </c>
     </row>
-    <row r="98" spans="13:19" x14ac:dyDescent="0.25">
+    <row r="98" spans="13:19" ht="15">
       <c r="M98" s="157" t="s">
         <v>47</v>
       </c>
@@ -36469,7 +36498,7 @@
         <v>0.65265874071841856</v>
       </c>
     </row>
-    <row r="99" spans="13:19" x14ac:dyDescent="0.25">
+    <row r="99" spans="13:19" ht="15">
       <c r="M99" s="157" t="s">
         <v>81</v>
       </c>
@@ -36492,7 +36521,7 @@
         <v>0.14840236413115043</v>
       </c>
     </row>
-    <row r="100" spans="13:19" x14ac:dyDescent="0.25">
+    <row r="100" spans="13:19" ht="15">
       <c r="M100" s="157" t="s">
         <v>70</v>
       </c>
@@ -36515,7 +36544,7 @@
         <v>0.28898223577701382</v>
       </c>
     </row>
-    <row r="101" spans="13:19" x14ac:dyDescent="0.25">
+    <row r="101" spans="13:19" ht="15">
       <c r="M101" s="157" t="s">
         <v>34</v>
       </c>
@@ -36538,7 +36567,7 @@
         <v>0.64241861616104012</v>
       </c>
     </row>
-    <row r="102" spans="13:19" x14ac:dyDescent="0.25">
+    <row r="102" spans="13:19" ht="15">
       <c r="M102" s="157" t="s">
         <v>40</v>
       </c>
@@ -36561,7 +36590,7 @@
         <v>0.52116159026022513</v>
       </c>
     </row>
-    <row r="103" spans="13:19" x14ac:dyDescent="0.25">
+    <row r="103" spans="13:19" ht="15">
       <c r="M103" s="157" t="s">
         <v>59</v>
       </c>
@@ -36584,7 +36613,7 @@
         <v>0.17366525812700745</v>
       </c>
     </row>
-    <row r="104" spans="13:19" x14ac:dyDescent="0.25">
+    <row r="104" spans="13:19" ht="15">
       <c r="M104" s="157" t="s">
         <v>68</v>
       </c>
@@ -36607,7 +36636,7 @@
         <v>0.29535755831295851</v>
       </c>
     </row>
-    <row r="105" spans="13:19" x14ac:dyDescent="0.25">
+    <row r="105" spans="13:19" ht="15">
       <c r="M105" s="157" t="s">
         <v>45</v>
       </c>
@@ -36640,30 +36669,30 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{83E4E41D-CCD8-4B95-AB4C-B35F3B4D4374}">
   <dimension ref="A1:AA149"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A39" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I42" sqref="I42"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K1" sqref="A1:K1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="15.42578125" customWidth="1"/>
+    <col min="1" max="1" width="15.375" customWidth="1"/>
     <col min="2" max="2" width="13" customWidth="1"/>
-    <col min="9" max="9" width="11.7109375" customWidth="1"/>
+    <col min="9" max="9" width="11.75" customWidth="1"/>
     <col min="10" max="10" width="11" customWidth="1"/>
-    <col min="13" max="13" width="17.85546875" customWidth="1"/>
-    <col min="14" max="14" width="14.5703125" customWidth="1"/>
-    <col min="15" max="15" width="14.42578125" customWidth="1"/>
-    <col min="16" max="16" width="18.5703125" customWidth="1"/>
-    <col min="17" max="17" width="14.5703125" customWidth="1"/>
+    <col min="13" max="13" width="17.875" customWidth="1"/>
+    <col min="14" max="14" width="14.625" customWidth="1"/>
+    <col min="15" max="15" width="14.375" customWidth="1"/>
+    <col min="16" max="16" width="18.625" customWidth="1"/>
+    <col min="17" max="17" width="14.625" customWidth="1"/>
     <col min="18" max="18" width="16" customWidth="1"/>
-    <col min="19" max="20" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="14.85546875" customWidth="1"/>
-    <col min="23" max="23" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="11.7109375" customWidth="1"/>
+    <col min="19" max="20" width="12.625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="13.75" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="14.875" customWidth="1"/>
+    <col min="23" max="23" width="12.625" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="11.75" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:27" ht="15.75" thickBot="1">
       <c r="A1" s="20" t="s">
         <v>0</v>
       </c>
@@ -36740,7 +36769,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="2" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:27" ht="15">
       <c r="A2" s="202" t="s">
         <v>15</v>
       </c>
@@ -36821,7 +36850,7 @@
         <v>2.6810543211950755E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:27" ht="15.75" thickBot="1">
       <c r="A3" s="202" t="s">
         <v>16</v>
       </c>
@@ -36902,7 +36931,7 @@
         <v>2.5087848786925868E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:27" ht="15.75" thickBot="1">
       <c r="A4" s="211" t="s">
         <v>17</v>
       </c>
@@ -36991,7 +37020,7 @@
         <v>2.7589641746197054E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:27" ht="15.75" thickBot="1">
       <c r="A5" s="220" t="s">
         <v>11</v>
       </c>
@@ -37080,7 +37109,7 @@
         <v>2.4637775821349121E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:27" ht="15">
       <c r="A6" s="229" t="s">
         <v>13</v>
       </c>
@@ -37169,7 +37198,7 @@
         <v>2.6974532065504243E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:27" ht="15.75" thickBot="1">
       <c r="A7" s="229" t="s">
         <v>10</v>
       </c>
@@ -37258,7 +37287,7 @@
         <v>2.8407410650292033E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:27" ht="15">
       <c r="A8" s="229" t="s">
         <v>12</v>
       </c>
@@ -37347,7 +37376,7 @@
         <v>2.0469845020203995E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:27" ht="15.75" thickBot="1">
       <c r="A9" s="231" t="s">
         <v>14</v>
       </c>
@@ -37436,7 +37465,7 @@
         <v>2.3365366492794606E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:27" ht="15">
       <c r="A10" s="220" t="s">
         <v>20</v>
       </c>
@@ -37525,7 +37554,7 @@
         <v>2.9533151051345578E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:27" ht="15.75" thickBot="1">
       <c r="A11" s="229" t="s">
         <v>18</v>
       </c>
@@ -37614,7 +37643,7 @@
         <v>3.8957908141007642E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:27" ht="15">
       <c r="A12" s="229" t="s">
         <v>21</v>
       </c>
@@ -37694,7 +37723,7 @@
         <v>3.3632050133964565E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:27" ht="15.75" thickBot="1">
       <c r="A13" s="229" t="s">
         <v>19</v>
       </c>
@@ -37783,7 +37812,7 @@
         <v>1.9225430592985922E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:27" ht="15">
       <c r="A14" s="229" t="s">
         <v>23</v>
       </c>
@@ -37872,7 +37901,7 @@
         <v>3.9939712575804961E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:27" ht="15.75" thickBot="1">
       <c r="A15" s="231" t="s">
         <v>22</v>
       </c>
@@ -37961,7 +37990,7 @@
         <v>5.6832110467934065E-2</v>
       </c>
     </row>
-    <row r="16" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:27" ht="15">
       <c r="A16" s="220" t="s">
         <v>25</v>
       </c>
@@ -38035,7 +38064,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:24" ht="15.75" thickBot="1">
       <c r="A17" s="229" t="s">
         <v>26</v>
       </c>
@@ -38117,7 +38146,7 @@
         <v>7.419796104849565E-3</v>
       </c>
     </row>
-    <row r="18" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:24" ht="15">
       <c r="A18" s="229" t="s">
         <v>27</v>
       </c>
@@ -38199,7 +38228,7 @@
         <v>3.1760739180964181E-3</v>
       </c>
     </row>
-    <row r="19" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:24" ht="15.75" thickBot="1">
       <c r="A19" s="229" t="s">
         <v>24</v>
       </c>
@@ -38281,7 +38310,7 @@
         <v>8.8091237429136163E-3</v>
       </c>
     </row>
-    <row r="20" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:24" ht="15">
       <c r="A20" s="229" t="s">
         <v>29</v>
       </c>
@@ -38363,7 +38392,7 @@
         <v>7.9155125466650669E-3</v>
       </c>
     </row>
-    <row r="21" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:24" ht="15.75" thickBot="1">
       <c r="A21" s="231" t="s">
         <v>28</v>
       </c>
@@ -38449,7 +38478,7 @@
         <v>1.5190107460238357E-2</v>
       </c>
     </row>
-    <row r="22" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:24" ht="15">
       <c r="A22" s="196" t="s">
         <v>71</v>
       </c>
@@ -38531,7 +38560,7 @@
         <v>8.5172697020779974E-3</v>
       </c>
     </row>
-    <row r="23" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:24" ht="15.75" thickBot="1">
       <c r="A23" s="197" t="s">
         <v>72</v>
       </c>
@@ -38613,7 +38642,7 @@
         <v>1.1244076834432943E-2</v>
       </c>
     </row>
-    <row r="24" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:24" ht="15">
       <c r="A24" s="197" t="s">
         <v>41</v>
       </c>
@@ -38695,7 +38724,7 @@
         <v>1.0190569249542262E-3</v>
       </c>
     </row>
-    <row r="25" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:24" ht="15.75" thickBot="1">
       <c r="A25" s="251" t="s">
         <v>42</v>
       </c>
@@ -38777,7 +38806,7 @@
         <v>1.8142230281456069E-2</v>
       </c>
     </row>
-    <row r="26" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:24" ht="15">
       <c r="A26" s="196" t="s">
         <v>48</v>
       </c>
@@ -38859,7 +38888,7 @@
         <v>1.8595564800486377E-2</v>
       </c>
     </row>
-    <row r="27" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:24" ht="15.75" thickBot="1">
       <c r="A27" s="197" t="s">
         <v>53</v>
       </c>
@@ -38941,7 +38970,7 @@
         <v>1.9352588601638779E-3</v>
       </c>
     </row>
-    <row r="28" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:24" ht="15">
       <c r="A28" s="197" t="s">
         <v>46</v>
       </c>
@@ -39023,7 +39052,7 @@
         <v>4.5788300238872891E-2</v>
       </c>
     </row>
-    <row r="29" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:24" ht="15.75" thickBot="1">
       <c r="A29" s="251" t="s">
         <v>47</v>
       </c>
@@ -39105,7 +39134,7 @@
         <v>5.2922756712115923E-4</v>
       </c>
     </row>
-    <row r="30" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:24" ht="15">
       <c r="A30" s="196" t="s">
         <v>49</v>
       </c>
@@ -39141,7 +39170,7 @@
         <v>1.0290745463990066E-2</v>
       </c>
     </row>
-    <row r="31" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:24" ht="15">
       <c r="A31" s="197" t="s">
         <v>50</v>
       </c>
@@ -39191,7 +39220,7 @@
       <c r="W31" s="324"/>
       <c r="X31" s="324"/>
     </row>
-    <row r="32" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:24" ht="15.75" thickBot="1">
       <c r="A32" s="251" t="s">
         <v>81</v>
       </c>
@@ -39263,7 +39292,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="33" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:25" ht="15">
       <c r="A33" s="196" t="s">
         <v>51</v>
       </c>
@@ -39339,7 +39368,7 @@
         <v>2.3207130322112076E-2</v>
       </c>
     </row>
-    <row r="34" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:25" ht="15">
       <c r="A34" s="197" t="s">
         <v>52</v>
       </c>
@@ -39411,7 +39440,7 @@
         <v>1.121686533888791E-3</v>
       </c>
     </row>
-    <row r="35" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:25" ht="15">
       <c r="A35" s="197" t="s">
         <v>69</v>
       </c>
@@ -39483,7 +39512,7 @@
         <v>8.5165958681662733E-3</v>
       </c>
     </row>
-    <row r="36" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:25" ht="15.75" thickBot="1">
       <c r="A36" s="251" t="s">
         <v>70</v>
       </c>
@@ -39559,7 +39588,7 @@
         <v>3.3014809854020766E-3</v>
       </c>
     </row>
-    <row r="37" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:25" ht="15">
       <c r="A37" s="271" t="s">
         <v>30</v>
       </c>
@@ -39635,7 +39664,7 @@
         <v>2.8242659754160279E-2</v>
       </c>
     </row>
-    <row r="38" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:25" ht="15">
       <c r="A38" s="279" t="s">
         <v>33</v>
       </c>
@@ -39707,7 +39736,7 @@
         <v>8.7222176349643753E-3</v>
       </c>
     </row>
-    <row r="39" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:25" ht="15">
       <c r="A39" s="279" t="s">
         <v>31</v>
       </c>
@@ -39779,7 +39808,7 @@
         <v>1.1308432645602742E-3</v>
       </c>
     </row>
-    <row r="40" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:25" ht="15">
       <c r="A40" s="279" t="s">
         <v>32</v>
       </c>
@@ -39851,7 +39880,7 @@
         <v>7.419796104849565E-3</v>
       </c>
     </row>
-    <row r="41" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:25" ht="15.75" thickBot="1">
       <c r="A41" s="289" t="s">
         <v>34</v>
       </c>
@@ -39927,7 +39956,7 @@
         <v>3.2022646854353055E-2</v>
       </c>
     </row>
-    <row r="42" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:25" ht="15">
       <c r="A42" s="271" t="s">
         <v>35</v>
       </c>
@@ -39999,7 +40028,7 @@
         <v>1.5190107460238357E-2</v>
       </c>
     </row>
-    <row r="43" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:25" ht="15">
       <c r="A43" s="279" t="s">
         <v>36</v>
       </c>
@@ -40075,7 +40104,7 @@
         <v>3.2923666943971711E-2</v>
       </c>
     </row>
-    <row r="44" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:25" ht="15">
       <c r="A44" s="279" t="s">
         <v>37</v>
       </c>
@@ -40147,7 +40176,7 @@
         <v>1.8142230281456069E-2</v>
       </c>
     </row>
-    <row r="45" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:25" ht="15">
       <c r="A45" s="279" t="s">
         <v>38</v>
       </c>
@@ -40219,7 +40248,7 @@
         <v>1.9352588601638779E-3</v>
       </c>
     </row>
-    <row r="46" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:25" ht="15">
       <c r="A46" s="279" t="s">
         <v>39</v>
       </c>
@@ -40295,7 +40324,7 @@
         <v>5.2922756712115923E-4</v>
       </c>
     </row>
-    <row r="47" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:25" ht="15.75" thickBot="1">
       <c r="A47" s="289" t="s">
         <v>40</v>
       </c>
@@ -40335,7 +40364,7 @@
         <v>3.5104139147676995E-2</v>
       </c>
     </row>
-    <row r="48" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:25" ht="15">
       <c r="A48" s="57" t="s">
         <v>54</v>
       </c>
@@ -40385,7 +40414,7 @@
       <c r="W48" s="324"/>
       <c r="X48" s="324"/>
     </row>
-    <row r="49" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:25" ht="15">
       <c r="A49" s="21" t="s">
         <v>55</v>
       </c>
@@ -40457,7 +40486,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="50" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:25" ht="15">
       <c r="A50" s="21" t="s">
         <v>56</v>
       </c>
@@ -40533,7 +40562,7 @@
         <v>2.8855774461099319E-2</v>
       </c>
     </row>
-    <row r="51" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:25" ht="15">
       <c r="A51" s="21" t="s">
         <v>57</v>
       </c>
@@ -40605,7 +40634,7 @@
         <v>1.1678798493635017E-2</v>
       </c>
     </row>
-    <row r="52" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:25" ht="15">
       <c r="A52" s="21" t="s">
         <v>58</v>
       </c>
@@ -40677,7 +40706,7 @@
         <v>1.0921211596456464E-2</v>
       </c>
     </row>
-    <row r="53" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:25" ht="15.75" thickBot="1">
       <c r="A53" s="297" t="s">
         <v>59</v>
       </c>
@@ -40749,7 +40778,7 @@
         <v>5.843412719900771E-3</v>
       </c>
     </row>
-    <row r="54" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:25" ht="15">
       <c r="A54" s="57" t="s">
         <v>63</v>
       </c>
@@ -40825,7 +40854,7 @@
         <v>2.1365917360237147E-2</v>
       </c>
     </row>
-    <row r="55" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:25" ht="15">
       <c r="A55" s="21" t="s">
         <v>64</v>
       </c>
@@ -40897,7 +40926,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:25" ht="15">
       <c r="A56" s="21" t="s">
         <v>65</v>
       </c>
@@ -40969,7 +40998,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:25" ht="15">
       <c r="A57" s="21" t="s">
         <v>66</v>
       </c>
@@ -41041,7 +41070,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:25" ht="15">
       <c r="A58" s="21" t="s">
         <v>67</v>
       </c>
@@ -41117,7 +41146,7 @@
         <v>3.6468412338000161E-2</v>
       </c>
     </row>
-    <row r="59" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:25" ht="15.75" thickBot="1">
       <c r="A59" s="297" t="s">
         <v>68</v>
       </c>
@@ -41189,7 +41218,7 @@
         <v>7.9155125466650669E-3</v>
       </c>
     </row>
-    <row r="60" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:25" ht="15">
       <c r="A60" s="57" t="s">
         <v>60</v>
       </c>
@@ -41265,7 +41294,7 @@
         <v>4.1890984941373041E-2</v>
       </c>
     </row>
-    <row r="61" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:25" ht="15">
       <c r="A61" s="21" t="s">
         <v>61</v>
       </c>
@@ -41337,7 +41366,7 @@
         <v>1.0190569249542262E-3</v>
       </c>
     </row>
-    <row r="62" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:25" ht="15">
       <c r="A62" s="21" t="s">
         <v>43</v>
       </c>
@@ -41409,7 +41438,7 @@
         <v>1.8595564800486377E-2</v>
       </c>
     </row>
-    <row r="63" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:25" ht="15">
       <c r="A63" s="21" t="s">
         <v>62</v>
       </c>
@@ -41481,7 +41510,7 @@
         <v>4.5788300238872891E-2</v>
       </c>
     </row>
-    <row r="64" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:25" ht="15">
       <c r="A64" s="21" t="s">
         <v>44</v>
       </c>
@@ -41517,7 +41546,7 @@
         <v>3.8038774552472371E-2</v>
       </c>
     </row>
-    <row r="65" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:18" ht="15.75" thickBot="1">
       <c r="A65" s="297" t="s">
         <v>45</v>
       </c>
@@ -41571,7 +41600,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="66" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:18" ht="15">
       <c r="A66" s="57" t="s">
         <v>76</v>
       </c>
@@ -41629,7 +41658,7 @@
         <v>3.3537961271519E-2</v>
       </c>
     </row>
-    <row r="67" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:18" ht="15">
       <c r="A67" s="21" t="s">
         <v>80</v>
       </c>
@@ -41688,7 +41717,7 @@
         <v>4.1886053732350083E-2</v>
       </c>
     </row>
-    <row r="68" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:18" ht="15">
       <c r="A68" s="21" t="s">
         <v>77</v>
       </c>
@@ -41747,7 +41776,7 @@
         <v>1.7762821983933013E-2</v>
       </c>
     </row>
-    <row r="69" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:18" ht="15">
       <c r="A69" s="21" t="s">
         <v>78</v>
       </c>
@@ -41806,7 +41835,7 @@
         <v>4.09563578558092E-2</v>
       </c>
     </row>
-    <row r="70" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:18" ht="15.75" thickBot="1">
       <c r="A70" s="297" t="s">
         <v>79</v>
       </c>
@@ -41865,7 +41894,7 @@
         <v>3.1172376844082413E-2</v>
       </c>
     </row>
-    <row r="71" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:18">
       <c r="M71" s="317" t="s">
         <v>122</v>
       </c>
@@ -41890,7 +41919,7 @@
         <v>2.5308277245108358E-2</v>
       </c>
     </row>
-    <row r="72" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:18">
       <c r="J72" s="315">
         <f>MEDIAN(K48:K70)</f>
         <v>3.4453948702562319E-2</v>
@@ -41900,7 +41929,7 @@
         <v>3.7701373470929049E-2</v>
       </c>
     </row>
-    <row r="74" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:18">
       <c r="A74" s="323" t="s">
         <v>111</v>
       </c>
@@ -41915,7 +41944,7 @@
       <c r="J74" s="323"/>
       <c r="K74" s="323"/>
     </row>
-    <row r="75" spans="1:18" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:18" ht="17.25" customHeight="1">
       <c r="A75" s="1" t="s">
         <v>0</v>
       </c>
@@ -41950,7 +41979,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="76" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:18" ht="15">
       <c r="A76" s="202" t="s">
         <v>11</v>
       </c>
@@ -41985,7 +42014,7 @@
         <v>1.4275283509600518E-2</v>
       </c>
     </row>
-    <row r="77" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:18" ht="15">
       <c r="A77" s="202" t="s">
         <v>20</v>
       </c>
@@ -42020,7 +42049,7 @@
         <v>4.1672818488478154E-2</v>
       </c>
     </row>
-    <row r="78" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:18" ht="15">
       <c r="A78" s="202" t="s">
         <v>25</v>
       </c>
@@ -42055,7 +42084,7 @@
         <v>3.8214387509899805E-2</v>
       </c>
     </row>
-    <row r="79" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:18" ht="15">
       <c r="A79" s="287" t="s">
         <v>30</v>
       </c>
@@ -42090,7 +42119,7 @@
         <v>2.1624750611575927E-2</v>
       </c>
     </row>
-    <row r="80" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:18" ht="15">
       <c r="A80" s="287" t="s">
         <v>35</v>
       </c>
@@ -42125,7 +42154,7 @@
         <v>4.8117931554435479E-2</v>
       </c>
     </row>
-    <row r="81" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:11" ht="15">
       <c r="A81" s="13" t="s">
         <v>54</v>
       </c>
@@ -42160,7 +42189,7 @@
         <v>3.7411501977499997E-2</v>
       </c>
     </row>
-    <row r="82" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:11" ht="15">
       <c r="A82" s="13" t="s">
         <v>63</v>
       </c>
@@ -42195,7 +42224,7 @@
         <v>1.4162913918015331E-2</v>
       </c>
     </row>
-    <row r="83" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:11" ht="15">
       <c r="A83" s="13" t="s">
         <v>60</v>
       </c>
@@ -42230,7 +42259,7 @@
         <v>3.4453948702562319E-2</v>
       </c>
     </row>
-    <row r="84" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:11" ht="15">
       <c r="A84" s="13" t="s">
         <v>76</v>
       </c>
@@ -42265,7 +42294,7 @@
         <v>4.8123480487998367E-2</v>
       </c>
     </row>
-    <row r="85" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:11">
       <c r="A85" s="323" t="s">
         <v>112</v>
       </c>
@@ -42280,7 +42309,7 @@
       <c r="J85" s="323"/>
       <c r="K85" s="323"/>
     </row>
-    <row r="86" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:11" ht="14.25" customHeight="1">
       <c r="A86" s="1" t="s">
         <v>0</v>
       </c>
@@ -42315,7 +42344,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="87" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:11" ht="15">
       <c r="A87" s="202" t="s">
         <v>13</v>
       </c>
@@ -42350,7 +42379,7 @@
         <v>3.9289218981435024E-2</v>
       </c>
     </row>
-    <row r="88" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:11" ht="15">
       <c r="A88" s="202" t="s">
         <v>18</v>
       </c>
@@ -42385,7 +42414,7 @@
         <v>3.0706717222428074E-2</v>
       </c>
     </row>
-    <row r="89" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:11" ht="15">
       <c r="A89" s="202" t="s">
         <v>26</v>
       </c>
@@ -42420,7 +42449,7 @@
         <v>2.4355743821808513E-2</v>
       </c>
     </row>
-    <row r="90" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:11" ht="15">
       <c r="A90" s="198" t="s">
         <v>71</v>
       </c>
@@ -42455,7 +42484,7 @@
         <v>1.2947988089113313E-2</v>
       </c>
     </row>
-    <row r="91" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:11" ht="15">
       <c r="A91" s="198" t="s">
         <v>48</v>
       </c>
@@ -42490,7 +42519,7 @@
         <v>3.9185770295907078E-2</v>
       </c>
     </row>
-    <row r="92" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:11" ht="15">
       <c r="A92" s="198" t="s">
         <v>49</v>
       </c>
@@ -42525,7 +42554,7 @@
         <v>1.0290745463990066E-2</v>
       </c>
     </row>
-    <row r="93" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:11" ht="15">
       <c r="A93" s="198" t="s">
         <v>51</v>
       </c>
@@ -42560,7 +42589,7 @@
         <v>1.8901883746156495E-2</v>
       </c>
     </row>
-    <row r="94" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:11" ht="15">
       <c r="A94" s="287" t="s">
         <v>36</v>
       </c>
@@ -42595,7 +42624,7 @@
         <v>5.7839505209629632E-2</v>
       </c>
     </row>
-    <row r="95" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:11" ht="15">
       <c r="A95" s="13" t="s">
         <v>55</v>
       </c>
@@ -42630,7 +42659,7 @@
         <v>3.4015607951991461E-2</v>
       </c>
     </row>
-    <row r="96" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:11" ht="15">
       <c r="A96" s="13" t="s">
         <v>64</v>
       </c>
@@ -42665,7 +42694,7 @@
         <v>1.6366473070102194E-2</v>
       </c>
     </row>
-    <row r="97" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:11" ht="15">
       <c r="A97" s="13" t="s">
         <v>61</v>
       </c>
@@ -42700,7 +42729,7 @@
         <v>6.3932943295208655E-2</v>
       </c>
     </row>
-    <row r="98" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:11" ht="15">
       <c r="A98" s="13" t="s">
         <v>80</v>
       </c>
@@ -42735,7 +42764,7 @@
         <v>5.3229190612098028E-2</v>
       </c>
     </row>
-    <row r="99" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:11">
       <c r="A99" s="323" t="s">
         <v>113</v>
       </c>
@@ -42750,7 +42779,7 @@
       <c r="J99" s="323"/>
       <c r="K99" s="323"/>
     </row>
-    <row r="100" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:11" ht="15">
       <c r="A100" s="1" t="s">
         <v>0</v>
       </c>
@@ -42785,7 +42814,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="101" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:11" ht="15">
       <c r="A101" s="202" t="s">
         <v>10</v>
       </c>
@@ -42820,7 +42849,7 @@
         <v>1.4761361997822069E-2</v>
       </c>
     </row>
-    <row r="102" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:11" ht="15">
       <c r="A102" s="202" t="s">
         <v>21</v>
       </c>
@@ -42855,7 +42884,7 @@
         <v>1.5058361144762035E-2</v>
       </c>
     </row>
-    <row r="103" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:11" ht="15">
       <c r="A103" s="202" t="s">
         <v>27</v>
       </c>
@@ -42890,7 +42919,7 @@
         <v>2.8185368694723621E-2</v>
       </c>
     </row>
-    <row r="104" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:11" ht="15">
       <c r="A104" s="198" t="s">
         <v>72</v>
       </c>
@@ -42925,7 +42954,7 @@
         <v>2.1222551780676606E-2</v>
       </c>
     </row>
-    <row r="105" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:11" ht="15">
       <c r="A105" s="287" t="s">
         <v>33</v>
       </c>
@@ -42960,7 +42989,7 @@
         <v>2.7976898447768763E-2</v>
       </c>
     </row>
-    <row r="106" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:11" ht="15">
       <c r="A106" s="287" t="s">
         <v>37</v>
       </c>
@@ -42995,7 +43024,7 @@
         <v>3.8450563674918829E-2</v>
       </c>
     </row>
-    <row r="107" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:11" ht="15">
       <c r="A107" s="13" t="s">
         <v>56</v>
       </c>
@@ -43030,7 +43059,7 @@
         <v>1.7886653884458457E-2</v>
       </c>
     </row>
-    <row r="108" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:11" ht="15">
       <c r="A108" s="13" t="s">
         <v>65</v>
       </c>
@@ -43065,7 +43094,7 @@
         <v>1.6280268144578312E-2</v>
       </c>
     </row>
-    <row r="109" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:11" ht="15">
       <c r="A109" s="13" t="s">
         <v>43</v>
       </c>
@@ -43100,7 +43129,7 @@
         <v>1.9121543922762271E-2</v>
       </c>
     </row>
-    <row r="110" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:11" ht="15">
       <c r="A110" s="13" t="s">
         <v>77</v>
       </c>
@@ -43136,7 +43165,7 @@
         <v>0.1477072933292011</v>
       </c>
     </row>
-    <row r="111" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:11">
       <c r="A111" s="323" t="s">
         <v>114</v>
       </c>
@@ -43151,7 +43180,7 @@
       <c r="J111" s="323"/>
       <c r="K111" s="323"/>
     </row>
-    <row r="112" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:11" ht="15">
       <c r="A112" s="1" t="s">
         <v>0</v>
       </c>
@@ -43186,7 +43215,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="113" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:11" ht="15">
       <c r="A113" s="202" t="s">
         <v>19</v>
       </c>
@@ -43221,7 +43250,7 @@
         <v>3.4816069629649893E-2</v>
       </c>
     </row>
-    <row r="114" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:11" ht="15">
       <c r="A114" s="202" t="s">
         <v>24</v>
       </c>
@@ -43256,7 +43285,7 @@
         <v>1.4704209641736405E-2</v>
       </c>
     </row>
-    <row r="115" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:11" ht="15">
       <c r="A115" s="198" t="s">
         <v>53</v>
       </c>
@@ -43291,7 +43320,7 @@
         <v>6.4307165637578411E-3</v>
       </c>
     </row>
-    <row r="116" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:11" ht="15">
       <c r="A116" s="287" t="s">
         <v>31</v>
       </c>
@@ -43326,7 +43355,7 @@
         <v>4.5796617339119383E-2</v>
       </c>
     </row>
-    <row r="117" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:11" ht="15">
       <c r="A117" s="287" t="s">
         <v>38</v>
       </c>
@@ -43361,7 +43390,7 @@
         <v>4.792294697998508E-2</v>
       </c>
     </row>
-    <row r="118" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:11" ht="15">
       <c r="A118" s="13" t="s">
         <v>57</v>
       </c>
@@ -43396,7 +43425,7 @@
         <v>4.1712511737339225E-2</v>
       </c>
     </row>
-    <row r="119" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:11" ht="15">
       <c r="A119" s="13" t="s">
         <v>66</v>
       </c>
@@ -43431,7 +43460,7 @@
         <v>4.8377718971910101E-2</v>
       </c>
     </row>
-    <row r="120" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:11" ht="15">
       <c r="A120" s="13" t="s">
         <v>62</v>
       </c>
@@ -43466,7 +43495,7 @@
         <v>4.2561740354097384E-2</v>
       </c>
     </row>
-    <row r="121" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:11" ht="15">
       <c r="A121" s="13" t="s">
         <v>78</v>
       </c>
@@ -43501,7 +43530,7 @@
         <v>3.1173460359890111E-2</v>
       </c>
     </row>
-    <row r="122" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:11">
       <c r="A122" s="323" t="s">
         <v>115</v>
       </c>
@@ -43516,7 +43545,7 @@
       <c r="J122" s="323"/>
       <c r="K122" s="323"/>
     </row>
-    <row r="123" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:11" ht="15">
       <c r="A123" s="1" t="s">
         <v>0</v>
       </c>
@@ -43551,7 +43580,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="124" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:11" ht="15">
       <c r="A124" s="202" t="s">
         <v>12</v>
       </c>
@@ -43586,7 +43615,7 @@
         <v>2.8522095944787992E-2</v>
       </c>
     </row>
-    <row r="125" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:11" ht="15">
       <c r="A125" s="202" t="s">
         <v>23</v>
       </c>
@@ -43621,7 +43650,7 @@
         <v>1.4504291018941295E-2</v>
       </c>
     </row>
-    <row r="126" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:11" ht="15">
       <c r="A126" s="202" t="s">
         <v>29</v>
       </c>
@@ -43656,7 +43685,7 @@
         <v>2.2718415220178003E-2</v>
       </c>
     </row>
-    <row r="127" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:11" ht="15">
       <c r="A127" s="198" t="s">
         <v>41</v>
       </c>
@@ -43691,7 +43720,7 @@
         <v>2.7760354085790886E-2</v>
       </c>
     </row>
-    <row r="128" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:11" ht="15">
       <c r="A128" s="198" t="s">
         <v>46</v>
       </c>
@@ -43726,7 +43755,7 @@
         <v>1.8748977215822783E-2</v>
       </c>
     </row>
-    <row r="129" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:11" ht="15">
       <c r="A129" s="198" t="s">
         <v>50</v>
       </c>
@@ -43761,7 +43790,7 @@
         <v>3.1779787840978201E-2</v>
       </c>
     </row>
-    <row r="130" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:11" ht="15">
       <c r="A130" s="198" t="s">
         <v>52</v>
       </c>
@@ -43796,7 +43825,7 @@
         <v>1.9971370823819133E-2</v>
       </c>
     </row>
-    <row r="131" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:11" ht="15">
       <c r="A131" s="287" t="s">
         <v>32</v>
       </c>
@@ -43831,7 +43860,7 @@
         <v>3.2583484975625902E-2</v>
       </c>
     </row>
-    <row r="132" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:11" ht="15">
       <c r="A132" s="287" t="s">
         <v>39</v>
       </c>
@@ -43866,7 +43895,7 @@
         <v>1.0746867809774435E-2</v>
       </c>
     </row>
-    <row r="133" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:11" ht="15">
       <c r="A133" s="13" t="s">
         <v>58</v>
       </c>
@@ -43901,7 +43930,7 @@
         <v>4.8660426133989146E-2</v>
       </c>
     </row>
-    <row r="134" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:11" ht="15">
       <c r="A134" s="13" t="s">
         <v>67</v>
       </c>
@@ -43936,7 +43965,7 @@
         <v>7.8753014642203526E-3</v>
       </c>
     </row>
-    <row r="135" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:11" ht="15">
       <c r="A135" s="13" t="s">
         <v>44</v>
       </c>
@@ -43971,7 +44000,7 @@
         <v>3.8038774552472371E-2</v>
       </c>
     </row>
-    <row r="136" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:11" ht="15">
       <c r="A136" s="13" t="s">
         <v>79</v>
       </c>
@@ -44006,7 +44035,7 @@
         <v>3.0115005225647792E-2</v>
       </c>
     </row>
-    <row r="137" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:11">
       <c r="A137" s="323" t="s">
         <v>116</v>
       </c>
@@ -44021,7 +44050,7 @@
       <c r="J137" s="323"/>
       <c r="K137" s="323"/>
     </row>
-    <row r="138" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:11" ht="15">
       <c r="A138" s="1" t="s">
         <v>0</v>
       </c>
@@ -44056,7 +44085,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="139" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:11" ht="15">
       <c r="A139" s="202" t="s">
         <v>14</v>
       </c>
@@ -44091,7 +44120,7 @@
         <v>2.627872287701041E-2</v>
       </c>
     </row>
-    <row r="140" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:11" ht="15">
       <c r="A140" s="202" t="s">
         <v>22</v>
       </c>
@@ -44126,7 +44155,7 @@
         <v>2.8779592972922853E-2</v>
       </c>
     </row>
-    <row r="141" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:11" ht="15">
       <c r="A141" s="202" t="s">
         <v>28</v>
       </c>
@@ -44161,7 +44190,7 @@
         <v>1.9648530039748393E-2</v>
       </c>
     </row>
-    <row r="142" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:11" ht="15">
       <c r="A142" s="198" t="s">
         <v>42</v>
       </c>
@@ -44196,7 +44225,7 @@
         <v>4.5967234306436171E-2</v>
       </c>
     </row>
-    <row r="143" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:11" ht="15">
       <c r="A143" s="198" t="s">
         <v>47</v>
       </c>
@@ -44231,7 +44260,7 @@
         <v>2.7707459234450341E-2</v>
       </c>
     </row>
-    <row r="144" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:11" ht="15">
       <c r="A144" s="198" t="s">
         <v>81</v>
       </c>
@@ -44266,7 +44295,7 @@
         <v>2.9518101311857652E-2</v>
       </c>
     </row>
-    <row r="145" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:11" ht="15">
       <c r="A145" s="287" t="s">
         <v>34</v>
       </c>
@@ -44301,7 +44330,7 @@
         <v>2.4416330404311126E-2</v>
       </c>
     </row>
-    <row r="146" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:11" ht="15">
       <c r="A146" s="287" t="s">
         <v>40</v>
       </c>
@@ -44336,7 +44365,7 @@
         <v>3.0669633617302388E-2</v>
       </c>
     </row>
-    <row r="147" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:11" ht="15">
       <c r="A147" s="13" t="s">
         <v>59</v>
       </c>
@@ -44371,7 +44400,7 @@
         <v>2.2105599118509095E-2</v>
       </c>
     </row>
-    <row r="148" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:11" ht="15">
       <c r="A148" s="13" t="s">
         <v>68</v>
       </c>
@@ -44406,7 +44435,7 @@
         <v>1.2289907989089242E-2</v>
       </c>
     </row>
-    <row r="149" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:11" ht="15">
       <c r="A149" s="13" t="s">
         <v>45</v>
       </c>
@@ -44466,24 +44495,24 @@
   <dimension ref="B1:AP76"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="AS12" sqref="AS12"/>
+      <selection activeCell="G22" sqref="G22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="2" max="2" width="11.85546875" customWidth="1"/>
-    <col min="5" max="5" width="17.7109375" customWidth="1"/>
-    <col min="7" max="7" width="17.85546875" customWidth="1"/>
-    <col min="9" max="9" width="12.85546875" customWidth="1"/>
-    <col min="12" max="12" width="12.140625" customWidth="1"/>
-    <col min="16" max="16" width="14.85546875" customWidth="1"/>
-    <col min="26" max="26" width="11.42578125" customWidth="1"/>
+    <col min="2" max="2" width="11.875" customWidth="1"/>
+    <col min="5" max="5" width="17.75" customWidth="1"/>
+    <col min="7" max="7" width="17.875" customWidth="1"/>
+    <col min="9" max="9" width="12.875" customWidth="1"/>
+    <col min="12" max="12" width="12.125" customWidth="1"/>
+    <col min="16" max="16" width="14.875" customWidth="1"/>
+    <col min="26" max="26" width="11.375" customWidth="1"/>
     <col min="33" max="33" width="12" customWidth="1"/>
-    <col min="40" max="40" width="11.42578125" customWidth="1"/>
+    <col min="40" max="40" width="11.375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:42" ht="11.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="2" spans="2:42" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:42" ht="11.25" customHeight="1"/>
+    <row r="2" spans="2:42" ht="17.25" customHeight="1">
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
@@ -44593,7 +44622,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="3" spans="2:42" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:42">
       <c r="B3" s="202" t="s">
         <v>11</v>
       </c>
@@ -44718,7 +44747,7 @@
         <v>6.7686778397052075E-2</v>
       </c>
     </row>
-    <row r="4" spans="2:42" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:42">
       <c r="B4" s="202" t="s">
         <v>20</v>
       </c>
@@ -44843,7 +44872,7 @@
         <v>0.10820679894105208</v>
       </c>
     </row>
-    <row r="5" spans="2:42" ht="30" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:42" ht="30">
       <c r="B5" s="202" t="s">
         <v>25</v>
       </c>
@@ -44952,7 +44981,7 @@
         <v>0.18699078585244788</v>
       </c>
     </row>
-    <row r="6" spans="2:42" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:42">
       <c r="B6" s="287" t="s">
         <v>30</v>
       </c>
@@ -45077,7 +45106,7 @@
         <v>0.27422056534322914</v>
       </c>
     </row>
-    <row r="7" spans="2:42" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:42" ht="15.75" customHeight="1">
       <c r="B7" s="287" t="s">
         <v>35</v>
       </c>
@@ -45152,7 +45181,7 @@
         <v>0.1783715898815833</v>
       </c>
     </row>
-    <row r="8" spans="2:42" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:42" ht="15" customHeight="1">
       <c r="B8" s="13" t="s">
         <v>54</v>
       </c>
@@ -45251,7 +45280,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="9" spans="2:42" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:42">
       <c r="B9" s="13" t="s">
         <v>63</v>
       </c>
@@ -45354,7 +45383,7 @@
         <v>5.3829515218864581E-2</v>
       </c>
     </row>
-    <row r="10" spans="2:42" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:42">
       <c r="B10" s="13" t="s">
         <v>60</v>
       </c>
@@ -45445,7 +45474,7 @@
         <v>0.16107619621076041</v>
       </c>
     </row>
-    <row r="11" spans="2:42" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:42">
       <c r="B11" s="13" t="s">
         <v>76</v>
       </c>
@@ -45526,7 +45555,7 @@
         <v>0.26585933766858333</v>
       </c>
     </row>
-    <row r="12" spans="2:42" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:42">
       <c r="I12" s="32"/>
       <c r="J12" s="32"/>
       <c r="K12" s="32"/>
@@ -45555,7 +45584,7 @@
       <c r="W12" s="32"/>
       <c r="X12" s="32"/>
     </row>
-    <row r="13" spans="2:42" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:42" ht="15.75" customHeight="1">
       <c r="B13" s="1" t="s">
         <v>0</v>
       </c>
@@ -45600,7 +45629,7 @@
       <c r="T13" s="32"/>
       <c r="U13" s="32"/>
     </row>
-    <row r="14" spans="2:42" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:42">
       <c r="B14" s="202" t="s">
         <v>13</v>
       </c>
@@ -45659,7 +45688,7 @@
         <v>6.7675898294374995E-2</v>
       </c>
     </row>
-    <row r="15" spans="2:42" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:42">
       <c r="B15" s="202" t="s">
         <v>18</v>
       </c>
@@ -45718,7 +45747,7 @@
         <v>8.9115899574874993E-2</v>
       </c>
     </row>
-    <row r="16" spans="2:42" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:42">
       <c r="B16" s="202" t="s">
         <v>26</v>
       </c>
@@ -45753,7 +45782,7 @@
       <c r="T16" s="32"/>
       <c r="U16" s="32"/>
     </row>
-    <row r="17" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:21">
       <c r="B17" s="198" t="s">
         <v>71</v>
       </c>
@@ -45812,7 +45841,7 @@
         <v>5.3520596246249996E-2</v>
       </c>
     </row>
-    <row r="18" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:21">
       <c r="B18" s="198" t="s">
         <v>48</v>
       </c>
@@ -45871,7 +45900,7 @@
         <v>0.1202577189975</v>
       </c>
     </row>
-    <row r="19" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:21">
       <c r="B19" s="198" t="s">
         <v>49</v>
       </c>
@@ -45918,7 +45947,7 @@
       <c r="T19" s="32"/>
       <c r="U19" s="32"/>
     </row>
-    <row r="20" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:21">
       <c r="B20" s="198" t="s">
         <v>51</v>
       </c>
@@ -45965,7 +45994,7 @@
       <c r="T20" s="32"/>
       <c r="U20" s="32"/>
     </row>
-    <row r="21" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:21">
       <c r="B21" s="287" t="s">
         <v>36</v>
       </c>
@@ -46000,7 +46029,7 @@
       <c r="T21" s="32"/>
       <c r="U21" s="32"/>
     </row>
-    <row r="22" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:21">
       <c r="B22" s="13" t="s">
         <v>55</v>
       </c>
@@ -46047,7 +46076,7 @@
       <c r="T22" s="32"/>
       <c r="U22" s="32"/>
     </row>
-    <row r="23" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:21">
       <c r="B23" s="13" t="s">
         <v>64</v>
       </c>
@@ -46094,7 +46123,7 @@
       <c r="T23" s="32"/>
       <c r="U23" s="32"/>
     </row>
-    <row r="24" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:21">
       <c r="B24" s="13" t="s">
         <v>61</v>
       </c>
@@ -46141,7 +46170,7 @@
       <c r="T24" s="32"/>
       <c r="U24" s="32"/>
     </row>
-    <row r="25" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:21">
       <c r="B25" s="13" t="s">
         <v>80</v>
       </c>
@@ -46188,7 +46217,7 @@
       <c r="T25" s="32"/>
       <c r="U25" s="32"/>
     </row>
-    <row r="26" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:21">
       <c r="I26" s="32"/>
       <c r="J26" s="32"/>
       <c r="K26" s="32"/>
@@ -46203,7 +46232,7 @@
       <c r="T26" s="32"/>
       <c r="U26" s="32"/>
     </row>
-    <row r="27" spans="2:21" ht="30" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:21" ht="30">
       <c r="B27" s="1" t="s">
         <v>0</v>
       </c>
@@ -46248,7 +46277,7 @@
       <c r="T27" s="32"/>
       <c r="U27" s="32"/>
     </row>
-    <row r="28" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:21">
       <c r="B28" s="202" t="s">
         <v>10</v>
       </c>
@@ -46295,7 +46324,7 @@
       <c r="T28" s="32"/>
       <c r="U28" s="32"/>
     </row>
-    <row r="29" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:21">
       <c r="B29" s="202" t="s">
         <v>21</v>
       </c>
@@ -46342,7 +46371,7 @@
       <c r="T29" s="32"/>
       <c r="U29" s="32"/>
     </row>
-    <row r="30" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:21">
       <c r="B30" s="202" t="s">
         <v>27</v>
       </c>
@@ -46377,7 +46406,7 @@
       <c r="T30" s="32"/>
       <c r="U30" s="32"/>
     </row>
-    <row r="31" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:21">
       <c r="B31" s="198" t="s">
         <v>72</v>
       </c>
@@ -46412,7 +46441,7 @@
       <c r="T31" s="32"/>
       <c r="U31" s="32"/>
     </row>
-    <row r="32" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:21">
       <c r="B32" s="287" t="s">
         <v>33</v>
       </c>
@@ -46434,7 +46463,7 @@
         <v>0.22422697086037502</v>
       </c>
     </row>
-    <row r="33" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:7">
       <c r="B33" s="287" t="s">
         <v>37</v>
       </c>
@@ -46456,7 +46485,7 @@
         <v>0.29528361253162505</v>
       </c>
     </row>
-    <row r="34" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:7">
       <c r="B34" s="13" t="s">
         <v>56</v>
       </c>
@@ -46478,7 +46507,7 @@
         <v>0.33747822904506253</v>
       </c>
     </row>
-    <row r="35" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:7">
       <c r="B35" s="13" t="s">
         <v>65</v>
       </c>
@@ -46500,7 +46529,7 @@
         <v>0.36990852318906253</v>
       </c>
     </row>
-    <row r="36" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:7">
       <c r="B36" s="13" t="s">
         <v>43</v>
       </c>
@@ -46522,7 +46551,7 @@
         <v>0.40964309146056255</v>
       </c>
     </row>
-    <row r="37" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:7">
       <c r="B37" s="13" t="s">
         <v>77</v>
       </c>
@@ -46545,7 +46574,7 @@
         <v>0.7313495763315625</v>
       </c>
     </row>
-    <row r="39" spans="2:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:7" ht="30">
       <c r="B39" s="1" t="s">
         <v>0</v>
       </c>
@@ -46565,7 +46594,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="40" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:7">
       <c r="B40" s="202" t="s">
         <v>19</v>
       </c>
@@ -46587,7 +46616,7 @@
         <v>7.9554719103750005E-2</v>
       </c>
     </row>
-    <row r="41" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:7">
       <c r="B41" s="202" t="s">
         <v>24</v>
       </c>
@@ -46609,7 +46638,7 @@
         <v>0.11118347404312501</v>
       </c>
     </row>
-    <row r="42" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:7">
       <c r="B42" s="198" t="s">
         <v>53</v>
       </c>
@@ -46631,7 +46660,7 @@
         <v>0.12348543482959376</v>
       </c>
     </row>
-    <row r="43" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:7">
       <c r="B43" s="287" t="s">
         <v>31</v>
       </c>
@@ -46653,7 +46682,7 @@
         <v>0.17757123990709375</v>
       </c>
     </row>
-    <row r="44" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:7">
       <c r="B44" s="287" t="s">
         <v>38</v>
       </c>
@@ -46675,7 +46704,7 @@
         <v>0.27394428628384376</v>
       </c>
     </row>
-    <row r="45" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:7">
       <c r="B45" s="13" t="s">
         <v>57</v>
       </c>
@@ -46697,7 +46726,7 @@
         <v>0.35177983318571876</v>
       </c>
     </row>
-    <row r="46" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:7">
       <c r="B46" s="13" t="s">
         <v>66</v>
       </c>
@@ -46719,7 +46748,7 @@
         <v>0.45511464090971876</v>
       </c>
     </row>
-    <row r="47" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:7">
       <c r="B47" s="13" t="s">
         <v>62</v>
       </c>
@@ -46741,7 +46770,7 @@
         <v>0.54470710435509373</v>
       </c>
     </row>
-    <row r="48" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:7">
       <c r="B48" s="13" t="s">
         <v>78</v>
       </c>
@@ -46763,7 +46792,7 @@
         <v>0.60995315688834373</v>
       </c>
     </row>
-    <row r="50" spans="2:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="50" spans="2:7" ht="30">
       <c r="B50" s="1" t="s">
         <v>0</v>
       </c>
@@ -46783,7 +46812,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="51" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="51" spans="2:7">
       <c r="B51" s="202" t="s">
         <v>12</v>
       </c>
@@ -46805,7 +46834,7 @@
         <v>3.2287012609500003E-2</v>
       </c>
     </row>
-    <row r="52" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="52" spans="2:7">
       <c r="B52" s="202" t="s">
         <v>23</v>
       </c>
@@ -46827,7 +46856,7 @@
         <v>6.119406461025001E-2</v>
       </c>
     </row>
-    <row r="53" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="53" spans="2:7">
       <c r="B53" s="202" t="s">
         <v>29</v>
       </c>
@@ -46849,7 +46878,7 @@
         <v>0.103950122054625</v>
       </c>
     </row>
-    <row r="54" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="54" spans="2:7">
       <c r="B54" s="198" t="s">
         <v>41</v>
       </c>
@@ -46871,7 +46900,7 @@
         <v>0.15572318242462502</v>
       </c>
     </row>
-    <row r="55" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="55" spans="2:7">
       <c r="B55" s="198" t="s">
         <v>46</v>
       </c>
@@ -46893,7 +46922,7 @@
         <v>0.200158258426125</v>
       </c>
     </row>
-    <row r="56" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="56" spans="2:7">
       <c r="B56" s="198" t="s">
         <v>50</v>
       </c>
@@ -46915,7 +46944,7 @@
         <v>0.26285977983637498</v>
       </c>
     </row>
-    <row r="57" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="57" spans="2:7">
       <c r="B57" s="198" t="s">
         <v>52</v>
       </c>
@@ -46937,7 +46966,7 @@
         <v>0.30366129042943746</v>
       </c>
     </row>
-    <row r="58" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="58" spans="2:7">
       <c r="B58" s="287" t="s">
         <v>32</v>
       </c>
@@ -46959,7 +46988,7 @@
         <v>0.37133718872381244</v>
       </c>
     </row>
-    <row r="59" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="59" spans="2:7">
       <c r="B59" s="287" t="s">
         <v>39</v>
       </c>
@@ -46981,7 +47010,7 @@
         <v>0.39277719000431244</v>
       </c>
     </row>
-    <row r="60" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="60" spans="2:7">
       <c r="B60" s="13" t="s">
         <v>58</v>
       </c>
@@ -47003,7 +47032,7 @@
         <v>0.5003653921865624</v>
       </c>
     </row>
-    <row r="61" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="61" spans="2:7">
       <c r="B61" s="13" t="s">
         <v>67</v>
       </c>
@@ -47025,7 +47054,7 @@
         <v>0.51650188488674986</v>
       </c>
     </row>
-    <row r="62" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="62" spans="2:7">
       <c r="B62" s="13" t="s">
         <v>44</v>
       </c>
@@ -47047,7 +47076,7 @@
         <v>0.58881359531099986</v>
       </c>
     </row>
-    <row r="63" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="63" spans="2:7">
       <c r="B63" s="13" t="s">
         <v>79</v>
       </c>
@@ -47069,7 +47098,7 @@
         <v>0.65157326620124989</v>
       </c>
     </row>
-    <row r="65" spans="2:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="65" spans="2:7" ht="30">
       <c r="B65" s="1" t="s">
         <v>0</v>
       </c>
@@ -47089,7 +47118,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="66" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="66" spans="2:7">
       <c r="B66" s="202" t="s">
         <v>14</v>
       </c>
@@ -47111,7 +47140,7 @@
         <v>5.5553220162000004E-2</v>
       </c>
     </row>
-    <row r="67" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="67" spans="2:7">
       <c r="B67" s="202" t="s">
         <v>22</v>
       </c>
@@ -47133,7 +47162,7 @@
         <v>0.11374555715325001</v>
       </c>
     </row>
-    <row r="68" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="68" spans="2:7">
       <c r="B68" s="202" t="s">
         <v>28</v>
       </c>
@@ -47155,7 +47184,7 @@
         <v>0.15044901126750002</v>
       </c>
     </row>
-    <row r="69" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="69" spans="2:7">
       <c r="B69" s="198" t="s">
         <v>42</v>
       </c>
@@ -47177,7 +47206,7 @@
         <v>0.25847201188762503</v>
       </c>
     </row>
-    <row r="70" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="70" spans="2:7">
       <c r="B70" s="198" t="s">
         <v>47</v>
       </c>
@@ -47199,7 +47228,7 @@
         <v>0.31593728233987506</v>
       </c>
     </row>
-    <row r="71" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="71" spans="2:7">
       <c r="B71" s="198" t="s">
         <v>81</v>
       </c>
@@ -47221,7 +47250,7 @@
         <v>0.37337950749275006</v>
       </c>
     </row>
-    <row r="72" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="72" spans="2:7">
       <c r="B72" s="287" t="s">
         <v>34</v>
       </c>
@@ -47243,7 +47272,7 @@
         <v>0.42690010373900006</v>
       </c>
     </row>
-    <row r="73" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="73" spans="2:7">
       <c r="B73" s="287" t="s">
         <v>40</v>
       </c>
@@ -47265,7 +47294,7 @@
         <v>0.49363722649025005</v>
       </c>
     </row>
-    <row r="74" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="74" spans="2:7">
       <c r="B74" s="13" t="s">
         <v>59</v>
       </c>
@@ -47287,7 +47316,7 @@
         <v>0.534930485643625</v>
       </c>
     </row>
-    <row r="75" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="75" spans="2:7">
       <c r="B75" s="13" t="s">
         <v>68</v>
       </c>
@@ -47309,7 +47338,7 @@
         <v>0.56006334748131248</v>
       </c>
     </row>
-    <row r="76" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="76" spans="2:7">
       <c r="B76" s="13" t="s">
         <v>45</v>
       </c>
@@ -47335,4 +47364,1215 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C9262DC-E5B7-49F4-A43F-DEF8C5BFDEDE}">
+  <dimension ref="A1:O35"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="R8" sqref="R8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25"/>
+  <cols>
+    <col min="1" max="1" width="13.375" customWidth="1"/>
+    <col min="2" max="2" width="12.25" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:15" ht="24.75" customHeight="1" thickBot="1">
+      <c r="A1" s="20" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="20" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="20" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="20" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" s="20" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1" s="20" t="s">
+        <v>7</v>
+      </c>
+      <c r="G1" s="20" t="s">
+        <v>8</v>
+      </c>
+      <c r="H1" s="31" t="s">
+        <v>73</v>
+      </c>
+      <c r="I1" s="31" t="s">
+        <v>74</v>
+      </c>
+      <c r="L1" s="325" t="s">
+        <v>139</v>
+      </c>
+      <c r="M1" s="325" t="s">
+        <v>138</v>
+      </c>
+      <c r="N1" s="325" t="s">
+        <v>140</v>
+      </c>
+      <c r="O1" s="325" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" ht="15">
+      <c r="A2" s="271" t="s">
+        <v>30</v>
+      </c>
+      <c r="B2" s="272">
+        <v>2.0019999999999998</v>
+      </c>
+      <c r="C2" s="274">
+        <v>4.3292750724375002E-2</v>
+      </c>
+      <c r="D2" s="275">
+        <v>2.1624750611575925</v>
+      </c>
+      <c r="E2" s="276">
+        <v>6.2592099693750004E-3</v>
+      </c>
+      <c r="F2" s="275">
+        <v>0.31264785061813194</v>
+      </c>
+      <c r="G2" s="275">
+        <v>6.9166477776264639</v>
+      </c>
+      <c r="H2" s="277">
+        <v>45004</v>
+      </c>
+      <c r="I2" s="278">
+        <f>C2/B2</f>
+        <v>2.1624750611575927E-2</v>
+      </c>
+      <c r="L2" s="326">
+        <v>2.1624750611575927E-2</v>
+      </c>
+      <c r="M2" s="326">
+        <v>4.5796617339119383E-2</v>
+      </c>
+      <c r="N2" s="328">
+        <v>3.7411501977499997E-2</v>
+      </c>
+      <c r="O2" s="328">
+        <v>4.1712511737339225E-2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" ht="15">
+      <c r="A3" s="279" t="s">
+        <v>33</v>
+      </c>
+      <c r="B3" s="280">
+        <v>1.972</v>
+      </c>
+      <c r="C3" s="282">
+        <v>5.5170443739E-2</v>
+      </c>
+      <c r="D3" s="283">
+        <v>2.7976898447768761</v>
+      </c>
+      <c r="E3" s="284">
+        <v>1.4501068387500001E-2</v>
+      </c>
+      <c r="F3" s="283">
+        <v>0.7353482955121704</v>
+      </c>
+      <c r="G3" s="283">
+        <v>3.8045778603842195</v>
+      </c>
+      <c r="H3" s="285">
+        <v>45004</v>
+      </c>
+      <c r="I3" s="286">
+        <f>C3/B3</f>
+        <v>2.7976898447768763E-2</v>
+      </c>
+      <c r="L3" s="326">
+        <v>2.7976898447768763E-2</v>
+      </c>
+      <c r="M3" s="326">
+        <v>3.2583484975625902E-2</v>
+      </c>
+      <c r="N3" s="328">
+        <v>3.4015607951991461E-2</v>
+      </c>
+      <c r="O3" s="328">
+        <v>4.8660426133989146E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" ht="15">
+      <c r="A4" s="279" t="s">
+        <v>31</v>
+      </c>
+      <c r="B4" s="280">
+        <v>1.181</v>
+      </c>
+      <c r="C4" s="282">
+        <v>5.4085805077499993E-2</v>
+      </c>
+      <c r="D4" s="283">
+        <v>4.5796617339119381</v>
+      </c>
+      <c r="E4" s="284">
+        <v>6.8162937900000005E-3</v>
+      </c>
+      <c r="F4" s="283">
+        <v>0.57716289500423379</v>
+      </c>
+      <c r="G4" s="283">
+        <v>7.9347819715235586</v>
+      </c>
+      <c r="H4" s="285">
+        <v>45004</v>
+      </c>
+      <c r="I4" s="286">
+        <f>C4/B4</f>
+        <v>4.5796617339119383E-2</v>
+      </c>
+      <c r="L4" s="326">
+        <v>4.8117931554435479E-2</v>
+      </c>
+      <c r="M4" s="326">
+        <v>2.4416330404311126E-2</v>
+      </c>
+      <c r="N4" s="328">
+        <v>1.7886653884458457E-2</v>
+      </c>
+      <c r="O4" s="328">
+        <v>2.2105599118509095E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" ht="15">
+      <c r="A5" s="279" t="s">
+        <v>32</v>
+      </c>
+      <c r="B5" s="287">
+        <v>2.077</v>
+      </c>
+      <c r="C5" s="282">
+        <v>6.7675898294374995E-2</v>
+      </c>
+      <c r="D5" s="283">
+        <v>3.25834849756259</v>
+      </c>
+      <c r="E5" s="284">
+        <v>3.540156143484375E-3</v>
+      </c>
+      <c r="F5" s="283">
+        <v>0.17044564966222317</v>
+      </c>
+      <c r="G5" s="283">
+        <v>19.116642190749655</v>
+      </c>
+      <c r="H5" s="285">
+        <v>45004</v>
+      </c>
+      <c r="I5" s="286">
+        <f>C5/B5</f>
+        <v>3.2583484975625902E-2</v>
+      </c>
+      <c r="L5" s="326">
+        <v>5.7839505209629632E-2</v>
+      </c>
+      <c r="M5" s="326">
+        <v>4.792294697998508E-2</v>
+      </c>
+      <c r="N5" s="328">
+        <v>1.4162913918015331E-2</v>
+      </c>
+      <c r="O5" s="328">
+        <v>4.8377718971910101E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" ht="15.75" thickBot="1">
+      <c r="A6" s="289" t="s">
+        <v>34</v>
+      </c>
+      <c r="B6" s="290">
+        <v>2.1920000000000002</v>
+      </c>
+      <c r="C6" s="292">
+        <v>5.3520596246249996E-2</v>
+      </c>
+      <c r="D6" s="293">
+        <v>2.4416330404311126</v>
+      </c>
+      <c r="E6" s="294">
+        <v>1.4081816066250001E-2</v>
+      </c>
+      <c r="F6" s="293">
+        <v>0.64241861616104012</v>
+      </c>
+      <c r="G6" s="293">
+        <v>3.8006884903519818</v>
+      </c>
+      <c r="H6" s="295">
+        <v>45004</v>
+      </c>
+      <c r="I6" s="296">
+        <f>C6/B6</f>
+        <v>2.4416330404311126E-2</v>
+      </c>
+      <c r="L6" s="326">
+        <v>3.8450563674918829E-2</v>
+      </c>
+      <c r="M6" s="326">
+        <v>1.0746867809774435E-2</v>
+      </c>
+      <c r="N6" s="328">
+        <v>1.6366473070102194E-2</v>
+      </c>
+      <c r="O6" s="328">
+        <v>7.8753014642203526E-3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" ht="15">
+      <c r="A7" s="271" t="s">
+        <v>35</v>
+      </c>
+      <c r="B7" s="272">
+        <v>1.984</v>
+      </c>
+      <c r="C7" s="274">
+        <v>9.5465976203999992E-2</v>
+      </c>
+      <c r="D7" s="275">
+        <v>4.8117931554435476</v>
+      </c>
+      <c r="E7" s="276">
+        <v>8.6655646387499997E-3</v>
+      </c>
+      <c r="F7" s="275">
+        <v>0.43677241122731852</v>
+      </c>
+      <c r="G7" s="275">
+        <v>11.016705798616128</v>
+      </c>
+      <c r="H7" s="277">
+        <v>45045</v>
+      </c>
+      <c r="I7" s="278">
+        <f>C7/B7</f>
+        <v>4.8117931554435479E-2</v>
+      </c>
+      <c r="L7" s="327"/>
+      <c r="M7" s="326">
+        <v>3.0669633617302388E-2</v>
+      </c>
+      <c r="N7" s="328">
+        <v>1.6280268144578312E-2</v>
+      </c>
+      <c r="O7" s="328">
+        <v>1.2289907989089242E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" ht="15">
+      <c r="A8" s="279" t="s">
+        <v>36</v>
+      </c>
+      <c r="B8" s="280">
+        <v>2.0249999999999999</v>
+      </c>
+      <c r="C8" s="282">
+        <v>0.1171249980495</v>
+      </c>
+      <c r="D8" s="283">
+        <v>5.7839505209629634</v>
+      </c>
+      <c r="E8" s="284">
+        <v>9.4235928253125004E-3</v>
+      </c>
+      <c r="F8" s="283">
+        <v>0.46536260865740742</v>
+      </c>
+      <c r="G8" s="283">
+        <v>12.428911161663647</v>
+      </c>
+      <c r="H8" s="285">
+        <v>45045</v>
+      </c>
+      <c r="I8" s="286">
+        <f>C8/B8</f>
+        <v>5.7839505209629632E-2</v>
+      </c>
+      <c r="N8" s="328">
+        <v>3.4453948702562319E-2</v>
+      </c>
+      <c r="O8" s="328">
+        <v>4.2561740354097384E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" ht="15">
+      <c r="A9" s="279" t="s">
+        <v>37</v>
+      </c>
+      <c r="B9" s="280">
+        <v>1.8480000000000001</v>
+      </c>
+      <c r="C9" s="282">
+        <v>7.1056641671250004E-2</v>
+      </c>
+      <c r="D9" s="283">
+        <v>3.8450563674918827</v>
+      </c>
+      <c r="E9" s="284">
+        <v>9.1419326221874996E-3</v>
+      </c>
+      <c r="F9" s="283">
+        <v>0.49469332371144475</v>
+      </c>
+      <c r="G9" s="283">
+        <v>7.7726061444376988</v>
+      </c>
+      <c r="H9" s="285">
+        <v>45045</v>
+      </c>
+      <c r="I9" s="286">
+        <f>C9/B9</f>
+        <v>3.8450563674918829E-2</v>
+      </c>
+      <c r="N9" s="328">
+        <v>6.3932943295208655E-2</v>
+      </c>
+      <c r="O9" s="328">
+        <v>3.8038774552472371E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" ht="15">
+      <c r="A10" s="279" t="s">
+        <v>38</v>
+      </c>
+      <c r="B10" s="280">
+        <v>2.0110000000000001</v>
+      </c>
+      <c r="C10" s="282">
+        <v>9.6373046376749996E-2</v>
+      </c>
+      <c r="D10" s="283">
+        <v>4.7922946979985079</v>
+      </c>
+      <c r="E10" s="284">
+        <v>8.4232530806250018E-3</v>
+      </c>
+      <c r="F10" s="283">
+        <v>0.4188589299167082</v>
+      </c>
+      <c r="G10" s="283">
+        <v>11.441309605005856</v>
+      </c>
+      <c r="H10" s="285">
+        <v>45045</v>
+      </c>
+      <c r="I10" s="286">
+        <f>C10/B10</f>
+        <v>4.792294697998508E-2</v>
+      </c>
+      <c r="N10" s="328">
+        <v>1.9121543922762271E-2</v>
+      </c>
+      <c r="O10" s="328">
+        <v>4.1529324627726745E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" ht="15">
+      <c r="A11" s="279" t="s">
+        <v>39</v>
+      </c>
+      <c r="B11" s="280">
+        <v>1.9950000000000001</v>
+      </c>
+      <c r="C11" s="282">
+        <v>2.1440001280499998E-2</v>
+      </c>
+      <c r="D11" s="283">
+        <v>1.0746867809774434</v>
+      </c>
+      <c r="E11" s="284">
+        <v>5.5995181921874998E-3</v>
+      </c>
+      <c r="F11" s="283">
+        <v>0.28067760361842103</v>
+      </c>
+      <c r="G11" s="283">
+        <v>3.8289010848135629</v>
+      </c>
+      <c r="H11" s="285">
+        <v>45045</v>
+      </c>
+      <c r="I11" s="286">
+        <f>C11/B11</f>
+        <v>1.0746867809774435E-2</v>
+      </c>
+      <c r="N11" s="328">
+        <v>4.8123480487998367E-2</v>
+      </c>
+      <c r="O11" s="328">
+        <v>3.1173460359890111E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" ht="15.75" thickBot="1">
+      <c r="A12" s="289" t="s">
+        <v>40</v>
+      </c>
+      <c r="B12" s="290">
+        <v>2.1760000000000002</v>
+      </c>
+      <c r="C12" s="292">
+        <v>6.6737122751250003E-2</v>
+      </c>
+      <c r="D12" s="293">
+        <v>3.066963361730239</v>
+      </c>
+      <c r="E12" s="294">
+        <v>1.13404762040625E-2</v>
+      </c>
+      <c r="F12" s="293">
+        <v>0.52116159026022513</v>
+      </c>
+      <c r="G12" s="293">
+        <v>5.8848607016469696</v>
+      </c>
+      <c r="H12" s="295">
+        <v>45045</v>
+      </c>
+      <c r="I12" s="296">
+        <f>C12/B12</f>
+        <v>3.0669633617302388E-2</v>
+      </c>
+      <c r="N12" s="328">
+        <v>5.3229190612098028E-2</v>
+      </c>
+      <c r="O12" s="328">
+        <v>3.0115005225647792E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" ht="15">
+      <c r="A13" s="57" t="s">
+        <v>54</v>
+      </c>
+      <c r="B13" s="58">
+        <v>1.75</v>
+      </c>
+      <c r="C13" s="60">
+        <v>6.5470128460624999E-2</v>
+      </c>
+      <c r="D13" s="61">
+        <v>3.7411501977499997</v>
+      </c>
+      <c r="E13" s="62">
+        <v>3.6854199580781252E-3</v>
+      </c>
+      <c r="F13" s="61">
+        <v>0.21059542617589286</v>
+      </c>
+      <c r="G13" s="61">
+        <v>17.764631766624067</v>
+      </c>
+      <c r="H13" s="63">
+        <v>45100</v>
+      </c>
+      <c r="I13" s="64">
+        <f>C13/B13</f>
+        <v>3.7411501977499997E-2</v>
+      </c>
+      <c r="L13" s="315">
+        <f>AVERAGE(L2:L12)</f>
+        <v>3.880192989966573E-2</v>
+      </c>
+      <c r="M13" s="315">
+        <f t="shared" ref="M13:O13" si="0">AVERAGE(M2:M12)</f>
+        <v>3.2022646854353055E-2</v>
+      </c>
+      <c r="N13" s="315">
+        <f t="shared" si="0"/>
+        <v>3.2271320542479581E-2</v>
+      </c>
+      <c r="O13" s="315">
+        <f t="shared" si="0"/>
+        <v>3.3130888230444688E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" ht="15">
+      <c r="A14" s="21" t="s">
+        <v>55</v>
+      </c>
+      <c r="B14" s="13">
+        <v>2.109</v>
+      </c>
+      <c r="C14" s="16">
+        <v>7.1738917170749997E-2</v>
+      </c>
+      <c r="D14" s="17">
+        <v>3.401560795199146</v>
+      </c>
+      <c r="E14" s="18">
+        <v>4.1068464931406246E-3</v>
+      </c>
+      <c r="F14" s="17">
+        <v>0.19472956344905759</v>
+      </c>
+      <c r="G14" s="17">
+        <v>17.468127257877896</v>
+      </c>
+      <c r="H14" s="35">
+        <v>45100</v>
+      </c>
+      <c r="I14" s="36">
+        <f>C14/B14</f>
+        <v>3.4015607951991461E-2</v>
+      </c>
+      <c r="L14" s="330">
+        <f>AVERAGE(L2:M7)</f>
+        <v>3.5104139147676995E-2</v>
+      </c>
+      <c r="M14" s="329"/>
+      <c r="N14" s="330">
+        <f>AVERAGE(N2:O12)</f>
+        <v>3.2701104386462135E-2</v>
+      </c>
+      <c r="O14" s="329"/>
+    </row>
+    <row r="15" spans="1:15" ht="15">
+      <c r="A15" s="21" t="s">
+        <v>56</v>
+      </c>
+      <c r="B15" s="13">
+        <v>2.359</v>
+      </c>
+      <c r="C15" s="16">
+        <v>4.2194616513437498E-2</v>
+      </c>
+      <c r="D15" s="17">
+        <v>1.7886653884458457</v>
+      </c>
+      <c r="E15" s="18">
+        <v>8.2568382809062486E-3</v>
+      </c>
+      <c r="F15" s="17">
+        <v>0.35001434001298215</v>
+      </c>
+      <c r="G15" s="17">
+        <v>5.1102631634449702</v>
+      </c>
+      <c r="H15" s="35">
+        <v>45100</v>
+      </c>
+      <c r="I15" s="36">
+        <f>C15/B15</f>
+        <v>1.7886653884458457E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" ht="15">
+      <c r="A16" s="21" t="s">
+        <v>57</v>
+      </c>
+      <c r="B16" s="13">
+        <v>1.8660000000000001</v>
+      </c>
+      <c r="C16" s="16">
+        <v>7.7835546901874997E-2</v>
+      </c>
+      <c r="D16" s="17">
+        <v>4.1712511737339222</v>
+      </c>
+      <c r="E16" s="18">
+        <v>6.2214054598124999E-3</v>
+      </c>
+      <c r="F16" s="17">
+        <v>0.33340865272307069</v>
+      </c>
+      <c r="G16" s="17">
+        <v>12.510926575137702</v>
+      </c>
+      <c r="H16" s="35">
+        <v>45100</v>
+      </c>
+      <c r="I16" s="36">
+        <f>C16/B16</f>
+        <v>4.1712511737339225E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" ht="15">
+      <c r="A17" s="21" t="s">
+        <v>58</v>
+      </c>
+      <c r="B17" s="14">
+        <v>2.2109999999999999</v>
+      </c>
+      <c r="C17" s="16">
+        <v>0.10758820218224999</v>
+      </c>
+      <c r="D17" s="17">
+        <v>4.866042613398915</v>
+      </c>
+      <c r="E17" s="18">
+        <v>1.4330423351250001E-2</v>
+      </c>
+      <c r="F17" s="17">
+        <v>0.64814216875848041</v>
+      </c>
+      <c r="G17" s="17">
+        <v>7.5076778644411348</v>
+      </c>
+      <c r="H17" s="35">
+        <v>45100</v>
+      </c>
+      <c r="I17" s="36">
+        <f>C17/B17</f>
+        <v>4.8660426133989146E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" ht="15.75" thickBot="1">
+      <c r="A18" s="297" t="s">
+        <v>59</v>
+      </c>
+      <c r="B18" s="298">
+        <v>1.8680000000000001</v>
+      </c>
+      <c r="C18" s="300">
+        <v>4.1293259153374992E-2</v>
+      </c>
+      <c r="D18" s="301">
+        <v>2.2105599118509094</v>
+      </c>
+      <c r="E18" s="302">
+        <v>3.2440670218124995E-3</v>
+      </c>
+      <c r="F18" s="301">
+        <v>0.17366525812700745</v>
+      </c>
+      <c r="G18" s="301">
+        <v>12.728855130219827</v>
+      </c>
+      <c r="H18" s="303">
+        <v>45100</v>
+      </c>
+      <c r="I18" s="304">
+        <f>C18/B18</f>
+        <v>2.2105599118509095E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" ht="15">
+      <c r="A19" s="57" t="s">
+        <v>63</v>
+      </c>
+      <c r="B19" s="125">
+        <v>2.3479999999999999</v>
+      </c>
+      <c r="C19" s="60">
+        <v>3.3254521879499996E-2</v>
+      </c>
+      <c r="D19" s="61">
+        <v>1.4162913918015332</v>
+      </c>
+      <c r="E19" s="62">
+        <v>1.3559283408750001E-2</v>
+      </c>
+      <c r="F19" s="61">
+        <v>0.57748225761286209</v>
+      </c>
+      <c r="G19" s="61">
+        <v>2.4525279748958102</v>
+      </c>
+      <c r="H19" s="63">
+        <v>45120</v>
+      </c>
+      <c r="I19" s="64">
+        <f>C19/B19</f>
+        <v>1.4162913918015331E-2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" ht="15">
+      <c r="A20" s="21" t="s">
+        <v>64</v>
+      </c>
+      <c r="B20" s="14">
+        <v>2.0059999999999998</v>
+      </c>
+      <c r="C20" s="16">
+        <v>3.2831144978625E-2</v>
+      </c>
+      <c r="D20" s="17">
+        <v>1.6366473070102194</v>
+      </c>
+      <c r="E20" s="18">
+        <v>1.3054441025625E-2</v>
+      </c>
+      <c r="F20" s="17">
+        <v>0.65076974205508487</v>
+      </c>
+      <c r="G20" s="17">
+        <v>2.5149406944487049</v>
+      </c>
+      <c r="H20" s="35">
+        <v>45120</v>
+      </c>
+      <c r="I20" s="36">
+        <f>C20/B20</f>
+        <v>1.6366473070102194E-2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" ht="15">
+      <c r="A21" s="21" t="s">
+        <v>65</v>
+      </c>
+      <c r="B21" s="14">
+        <v>1.992</v>
+      </c>
+      <c r="C21" s="16">
+        <v>3.2430294143999998E-2</v>
+      </c>
+      <c r="D21" s="17">
+        <v>1.6280268144578312</v>
+      </c>
+      <c r="E21" s="18">
+        <v>1.3134819616875E-2</v>
+      </c>
+      <c r="F21" s="17">
+        <v>0.65937849482304212</v>
+      </c>
+      <c r="G21" s="17">
+        <v>2.4690323194339934</v>
+      </c>
+      <c r="H21" s="35">
+        <v>45120</v>
+      </c>
+      <c r="I21" s="36">
+        <f>C21/B21</f>
+        <v>1.6280268144578312E-2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" ht="15">
+      <c r="A22" s="21" t="s">
+        <v>66</v>
+      </c>
+      <c r="B22" s="14">
+        <v>2.1360000000000001</v>
+      </c>
+      <c r="C22" s="16">
+        <v>0.10333480772399999</v>
+      </c>
+      <c r="D22" s="17">
+        <v>4.8377718971910104</v>
+      </c>
+      <c r="E22" s="18">
+        <v>8.0501506481250006E-3</v>
+      </c>
+      <c r="F22" s="17">
+        <v>0.37687971199087078</v>
+      </c>
+      <c r="G22" s="17">
+        <v>12.83638185678776</v>
+      </c>
+      <c r="H22" s="35">
+        <v>45120</v>
+      </c>
+      <c r="I22" s="36">
+        <f>C22/B22</f>
+        <v>4.8377718971910101E-2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" ht="15">
+      <c r="A23" s="21" t="s">
+        <v>67</v>
+      </c>
+      <c r="B23" s="14">
+        <v>2.0489999999999999</v>
+      </c>
+      <c r="C23" s="16">
+        <v>1.6136492700187501E-2</v>
+      </c>
+      <c r="D23" s="17">
+        <v>0.78753014642203523</v>
+      </c>
+      <c r="E23" s="18">
+        <v>5.5636888035937504E-3</v>
+      </c>
+      <c r="F23" s="17">
+        <v>0.27153190842331631</v>
+      </c>
+      <c r="G23" s="17">
+        <v>2.9003226581911745</v>
+      </c>
+      <c r="H23" s="35">
+        <v>45120</v>
+      </c>
+      <c r="I23" s="36">
+        <f>C23/B23</f>
+        <v>7.8753014642203526E-3</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" ht="15.75" thickBot="1">
+      <c r="A24" s="297" t="s">
+        <v>68</v>
+      </c>
+      <c r="B24" s="305">
+        <v>2.0449999999999999</v>
+      </c>
+      <c r="C24" s="300">
+        <v>2.5132861837687499E-2</v>
+      </c>
+      <c r="D24" s="301">
+        <v>1.2289907989089242</v>
+      </c>
+      <c r="E24" s="302">
+        <v>6.0400620675000009E-3</v>
+      </c>
+      <c r="F24" s="301">
+        <v>0.29535755831295851</v>
+      </c>
+      <c r="G24" s="301">
+        <v>4.161027081645547</v>
+      </c>
+      <c r="H24" s="303">
+        <v>45120</v>
+      </c>
+      <c r="I24" s="304">
+        <f>C24/B24</f>
+        <v>1.2289907989089242E-2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" ht="15">
+      <c r="A25" s="57" t="s">
+        <v>60</v>
+      </c>
+      <c r="B25" s="125">
+        <v>2.1659999999999999</v>
+      </c>
+      <c r="C25" s="60">
+        <v>7.4627252889749987E-2</v>
+      </c>
+      <c r="D25" s="61">
+        <v>3.4453948702562318</v>
+      </c>
+      <c r="E25" s="62">
+        <v>7.8202946596874993E-3</v>
+      </c>
+      <c r="F25" s="61">
+        <v>0.36104776822195289</v>
+      </c>
+      <c r="G25" s="61">
+        <v>9.5427673939759341</v>
+      </c>
+      <c r="H25" s="63">
+        <v>45134</v>
+      </c>
+      <c r="I25" s="64">
+        <f>C25/B25</f>
+        <v>3.4453948702562319E-2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" ht="15">
+      <c r="A26" s="21" t="s">
+        <v>61</v>
+      </c>
+      <c r="B26" s="14">
+        <v>1.9410000000000001</v>
+      </c>
+      <c r="C26" s="16">
+        <v>0.124093842936</v>
+      </c>
+      <c r="D26" s="17">
+        <v>6.3932943295208657</v>
+      </c>
+      <c r="E26" s="18">
+        <v>8.646821086875001E-3</v>
+      </c>
+      <c r="F26" s="17">
+        <v>0.44548279685085013</v>
+      </c>
+      <c r="G26" s="17">
+        <v>14.35138320652452</v>
+      </c>
+      <c r="H26" s="35">
+        <v>45134</v>
+      </c>
+      <c r="I26" s="36">
+        <f>C26/B26</f>
+        <v>6.3932943295208655E-2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" ht="15">
+      <c r="A27" s="21" t="s">
+        <v>43</v>
+      </c>
+      <c r="B27" s="14">
+        <v>2.0779999999999998</v>
+      </c>
+      <c r="C27" s="16">
+        <v>3.9734568271499994E-2</v>
+      </c>
+      <c r="D27" s="17">
+        <v>1.912154392276227</v>
+      </c>
+      <c r="E27" s="18">
+        <v>6.7338353981250005E-3</v>
+      </c>
+      <c r="F27" s="17">
+        <v>0.32405367652189609</v>
+      </c>
+      <c r="G27" s="17">
+        <v>5.9007335229138311</v>
+      </c>
+      <c r="H27" s="35">
+        <v>45134</v>
+      </c>
+      <c r="I27" s="36">
+        <f>C27/B27</f>
+        <v>1.9121543922762271E-2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" ht="15">
+      <c r="A28" s="21" t="s">
+        <v>62</v>
+      </c>
+      <c r="B28" s="13">
+        <v>2.105</v>
+      </c>
+      <c r="C28" s="16">
+        <v>8.9592463445374998E-2</v>
+      </c>
+      <c r="D28" s="17">
+        <v>4.2561740354097388</v>
+      </c>
+      <c r="E28" s="18">
+        <v>4.0582605854531254E-3</v>
+      </c>
+      <c r="F28" s="17">
+        <v>0.19279147674361641</v>
+      </c>
+      <c r="G28" s="17">
+        <v>22.076567425591165</v>
+      </c>
+      <c r="H28" s="35">
+        <v>45134</v>
+      </c>
+      <c r="I28" s="36">
+        <f>C28/B28</f>
+        <v>4.2561740354097384E-2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" ht="15">
+      <c r="A29" s="21" t="s">
+        <v>44</v>
+      </c>
+      <c r="B29" s="14">
+        <v>1.901</v>
+      </c>
+      <c r="C29" s="16">
+        <v>7.2311710424249984E-2</v>
+      </c>
+      <c r="D29" s="17">
+        <v>3.8038774552472372</v>
+      </c>
+      <c r="E29" s="18">
+        <v>7.4870013290625004E-3</v>
+      </c>
+      <c r="F29" s="17">
+        <v>0.39384541446935828</v>
+      </c>
+      <c r="G29" s="17">
+        <v>9.6583007329724406</v>
+      </c>
+      <c r="H29" s="35">
+        <v>45134</v>
+      </c>
+      <c r="I29" s="36">
+        <f>C29/B29</f>
+        <v>3.8038774552472371E-2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" ht="15.75" thickBot="1">
+      <c r="A30" s="297" t="s">
+        <v>45</v>
+      </c>
+      <c r="B30" s="305">
+        <v>1.742</v>
+      </c>
+      <c r="C30" s="300">
+        <v>7.2344083501499984E-2</v>
+      </c>
+      <c r="D30" s="301">
+        <v>4.1529324627726742</v>
+      </c>
+      <c r="E30" s="302">
+        <v>1.59767045325E-2</v>
+      </c>
+      <c r="F30" s="301">
+        <v>0.91714721770952934</v>
+      </c>
+      <c r="G30" s="301">
+        <v>4.5280979788001208</v>
+      </c>
+      <c r="H30" s="303">
+        <v>45134</v>
+      </c>
+      <c r="I30" s="304">
+        <f>C30/B30</f>
+        <v>4.1529324627726745E-2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" ht="15">
+      <c r="A31" s="57" t="s">
+        <v>76</v>
+      </c>
+      <c r="B31" s="58">
+        <v>2.4580000000000002</v>
+      </c>
+      <c r="C31" s="60">
+        <v>0.1182875150395</v>
+      </c>
+      <c r="D31" s="61">
+        <v>4.8123480487998371</v>
+      </c>
+      <c r="E31" s="62">
+        <v>5.08671067303125E-3</v>
+      </c>
+      <c r="F31" s="61">
+        <v>0.20694510467987184</v>
+      </c>
+      <c r="G31" s="61">
+        <v>23.254225105948599</v>
+      </c>
+      <c r="H31" s="63">
+        <v>45146</v>
+      </c>
+      <c r="I31" s="64">
+        <f>C31/B31</f>
+        <v>4.8123480487998367E-2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" ht="15">
+      <c r="A32" s="21" t="s">
+        <v>80</v>
+      </c>
+      <c r="B32" s="13">
+        <v>1.9279999999999999</v>
+      </c>
+      <c r="C32" s="16">
+        <v>0.102625879500125</v>
+      </c>
+      <c r="D32" s="17">
+        <v>5.3229190612098032</v>
+      </c>
+      <c r="E32" s="18">
+        <v>4.3786440464062496E-3</v>
+      </c>
+      <c r="F32" s="17">
+        <v>0.2271080936932702</v>
+      </c>
+      <c r="G32" s="17">
+        <v>23.437821940414334</v>
+      </c>
+      <c r="H32" s="35">
+        <v>45146</v>
+      </c>
+      <c r="I32" s="36">
+        <f>C32/B32</f>
+        <v>5.3229190612098028E-2</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" ht="15">
+      <c r="A33" s="21" t="s">
+        <v>77</v>
+      </c>
+      <c r="B33" s="14">
+        <v>2.1779999999999999</v>
+      </c>
+      <c r="C33" s="16">
+        <v>0.32170648487100001</v>
+      </c>
+      <c r="D33" s="17">
+        <v>14.77072933292011</v>
+      </c>
+      <c r="E33" s="18">
+        <v>1.763577148875E-2</v>
+      </c>
+      <c r="F33" s="17">
+        <v>0.80972320884986226</v>
+      </c>
+      <c r="G33" s="17">
+        <v>18.241701820428958</v>
+      </c>
+      <c r="H33" s="35">
+        <v>45146</v>
+      </c>
+      <c r="I33" s="36">
+        <f>C33/B33</f>
+        <v>0.1477072933292011</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" ht="15">
+      <c r="A34" s="21" t="s">
+        <v>78</v>
+      </c>
+      <c r="B34" s="13">
+        <v>2.093</v>
+      </c>
+      <c r="C34" s="16">
+        <v>6.5246052533249999E-2</v>
+      </c>
+      <c r="D34" s="17">
+        <v>3.1173460359890113</v>
+      </c>
+      <c r="E34" s="18">
+        <v>3.5472578961093749E-3</v>
+      </c>
+      <c r="F34" s="17">
+        <v>0.16948198261392142</v>
+      </c>
+      <c r="G34" s="17">
+        <v>18.393377206887532</v>
+      </c>
+      <c r="H34" s="35">
+        <v>45146</v>
+      </c>
+      <c r="I34" s="36">
+        <f>C34/B34</f>
+        <v>3.1173460359890111E-2</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" ht="15.75" thickBot="1">
+      <c r="A35" s="297" t="s">
+        <v>79</v>
+      </c>
+      <c r="B35" s="305">
+        <v>2.0840000000000001</v>
+      </c>
+      <c r="C35" s="300">
+        <v>6.2759670890250002E-2</v>
+      </c>
+      <c r="D35" s="301">
+        <v>3.0115005225647793</v>
+      </c>
+      <c r="E35" s="302">
+        <v>7.5660358650000009E-3</v>
+      </c>
+      <c r="F35" s="301">
+        <v>0.36305354438579657</v>
+      </c>
+      <c r="G35" s="301">
+        <v>8.2949211462996413</v>
+      </c>
+      <c r="H35" s="303">
+        <v>45146</v>
+      </c>
+      <c r="I35" s="304">
+        <f>C35/B35</f>
+        <v>3.0115005225647792E-2</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="L14:M14"/>
+    <mergeCell ref="N14:O14"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
update on carbon data
</commit_message>
<xml_diff>
--- a/Bed_Carbon/Carbon_Sediment_Samples.xlsx
+++ b/Bed_Carbon/Carbon_Sediment_Samples.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nicol\Documents\GitHub\La_Jara\Bed_Carbon\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC08C22C-1500-44BD-A3EF-029F8BB5BE8D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA88580D-8D5B-4CB9-A098-D80B5D8C631C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{797E201D-8F44-4DD9-9B42-7B8F6976B830}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="All Samples" sheetId="1" r:id="rId1"/>
     <sheet name="Composite Samples" sheetId="2" r:id="rId2"/>
     <sheet name="Seasonal" sheetId="3" r:id="rId3"/>
-    <sheet name="Summary" sheetId="4" r:id="rId4"/>
+    <sheet name="Significance" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -975,7 +975,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="341">
+  <cellXfs count="340">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -1951,19 +1951,20 @@
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1972,17 +1973,15 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="centerContinuous"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -32967,7 +32966,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{49720B70-5BE3-4E08-B389-4F33CC21E2D2}">
   <dimension ref="A1:S105"/>
   <sheetViews>
-    <sheetView topLeftCell="P60" zoomScale="83" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView topLeftCell="P1" zoomScale="83" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="AJ37" sqref="AJ37"/>
     </sheetView>
   </sheetViews>
@@ -39869,20 +39868,20 @@
         <f t="shared" si="0"/>
         <v>3.1779787840978201E-2</v>
       </c>
-      <c r="M31" s="328" t="s">
+      <c r="M31" s="334" t="s">
         <v>109</v>
       </c>
-      <c r="N31" s="328"/>
-      <c r="O31" s="328"/>
-      <c r="P31" s="328"/>
-      <c r="Q31" s="328"/>
-      <c r="R31" s="328"/>
-      <c r="S31" s="328"/>
-      <c r="T31" s="328"/>
-      <c r="U31" s="328"/>
-      <c r="V31" s="328"/>
-      <c r="W31" s="328"/>
-      <c r="X31" s="328"/>
+      <c r="N31" s="334"/>
+      <c r="O31" s="334"/>
+      <c r="P31" s="334"/>
+      <c r="Q31" s="334"/>
+      <c r="R31" s="334"/>
+      <c r="S31" s="334"/>
+      <c r="T31" s="334"/>
+      <c r="U31" s="334"/>
+      <c r="V31" s="334"/>
+      <c r="W31" s="334"/>
+      <c r="X31" s="334"/>
     </row>
     <row r="32" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A32" s="251" t="s">
@@ -41063,20 +41062,20 @@
         <f t="shared" si="0"/>
         <v>3.7411501977499997E-2</v>
       </c>
-      <c r="M48" s="328" t="s">
+      <c r="M48" s="334" t="s">
         <v>110</v>
       </c>
-      <c r="N48" s="328"/>
-      <c r="O48" s="328"/>
-      <c r="P48" s="328"/>
-      <c r="Q48" s="328"/>
-      <c r="R48" s="328"/>
-      <c r="S48" s="328"/>
-      <c r="T48" s="328"/>
-      <c r="U48" s="328"/>
-      <c r="V48" s="328"/>
-      <c r="W48" s="328"/>
-      <c r="X48" s="328"/>
+      <c r="N48" s="334"/>
+      <c r="O48" s="334"/>
+      <c r="P48" s="334"/>
+      <c r="Q48" s="334"/>
+      <c r="R48" s="334"/>
+      <c r="S48" s="334"/>
+      <c r="T48" s="334"/>
+      <c r="U48" s="334"/>
+      <c r="V48" s="334"/>
+      <c r="W48" s="334"/>
+      <c r="X48" s="334"/>
     </row>
     <row r="49" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A49" s="21" t="s">
@@ -42594,19 +42593,19 @@
       </c>
     </row>
     <row r="74" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A74" s="327" t="s">
+      <c r="A74" s="333" t="s">
         <v>111</v>
       </c>
-      <c r="B74" s="327"/>
-      <c r="C74" s="327"/>
-      <c r="D74" s="327"/>
-      <c r="E74" s="327"/>
-      <c r="F74" s="327"/>
-      <c r="G74" s="327"/>
-      <c r="H74" s="327"/>
-      <c r="I74" s="327"/>
-      <c r="J74" s="327"/>
-      <c r="K74" s="327"/>
+      <c r="B74" s="333"/>
+      <c r="C74" s="333"/>
+      <c r="D74" s="333"/>
+      <c r="E74" s="333"/>
+      <c r="F74" s="333"/>
+      <c r="G74" s="333"/>
+      <c r="H74" s="333"/>
+      <c r="I74" s="333"/>
+      <c r="J74" s="333"/>
+      <c r="K74" s="333"/>
     </row>
     <row r="75" spans="1:18" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A75" s="1" t="s">
@@ -42959,19 +42958,19 @@
       </c>
     </row>
     <row r="85" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A85" s="327" t="s">
+      <c r="A85" s="333" t="s">
         <v>112</v>
       </c>
-      <c r="B85" s="327"/>
-      <c r="C85" s="327"/>
-      <c r="D85" s="327"/>
-      <c r="E85" s="327"/>
-      <c r="F85" s="327"/>
-      <c r="G85" s="327"/>
-      <c r="H85" s="327"/>
-      <c r="I85" s="327"/>
-      <c r="J85" s="327"/>
-      <c r="K85" s="327"/>
+      <c r="B85" s="333"/>
+      <c r="C85" s="333"/>
+      <c r="D85" s="333"/>
+      <c r="E85" s="333"/>
+      <c r="F85" s="333"/>
+      <c r="G85" s="333"/>
+      <c r="H85" s="333"/>
+      <c r="I85" s="333"/>
+      <c r="J85" s="333"/>
+      <c r="K85" s="333"/>
     </row>
     <row r="86" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A86" s="1" t="s">
@@ -43429,19 +43428,19 @@
       </c>
     </row>
     <row r="99" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A99" s="327" t="s">
+      <c r="A99" s="333" t="s">
         <v>113</v>
       </c>
-      <c r="B99" s="327"/>
-      <c r="C99" s="327"/>
-      <c r="D99" s="327"/>
-      <c r="E99" s="327"/>
-      <c r="F99" s="327"/>
-      <c r="G99" s="327"/>
-      <c r="H99" s="327"/>
-      <c r="I99" s="327"/>
-      <c r="J99" s="327"/>
-      <c r="K99" s="327"/>
+      <c r="B99" s="333"/>
+      <c r="C99" s="333"/>
+      <c r="D99" s="333"/>
+      <c r="E99" s="333"/>
+      <c r="F99" s="333"/>
+      <c r="G99" s="333"/>
+      <c r="H99" s="333"/>
+      <c r="I99" s="333"/>
+      <c r="J99" s="333"/>
+      <c r="K99" s="333"/>
     </row>
     <row r="100" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A100" s="1" t="s">
@@ -43830,19 +43829,19 @@
       </c>
     </row>
     <row r="111" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A111" s="327" t="s">
+      <c r="A111" s="333" t="s">
         <v>114</v>
       </c>
-      <c r="B111" s="327"/>
-      <c r="C111" s="327"/>
-      <c r="D111" s="327"/>
-      <c r="E111" s="327"/>
-      <c r="F111" s="327"/>
-      <c r="G111" s="327"/>
-      <c r="H111" s="327"/>
-      <c r="I111" s="327"/>
-      <c r="J111" s="327"/>
-      <c r="K111" s="327"/>
+      <c r="B111" s="333"/>
+      <c r="C111" s="333"/>
+      <c r="D111" s="333"/>
+      <c r="E111" s="333"/>
+      <c r="F111" s="333"/>
+      <c r="G111" s="333"/>
+      <c r="H111" s="333"/>
+      <c r="I111" s="333"/>
+      <c r="J111" s="333"/>
+      <c r="K111" s="333"/>
     </row>
     <row r="112" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A112" s="1" t="s">
@@ -44195,19 +44194,19 @@
       </c>
     </row>
     <row r="122" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A122" s="327" t="s">
+      <c r="A122" s="333" t="s">
         <v>115</v>
       </c>
-      <c r="B122" s="327"/>
-      <c r="C122" s="327"/>
-      <c r="D122" s="327"/>
-      <c r="E122" s="327"/>
-      <c r="F122" s="327"/>
-      <c r="G122" s="327"/>
-      <c r="H122" s="327"/>
-      <c r="I122" s="327"/>
-      <c r="J122" s="327"/>
-      <c r="K122" s="327"/>
+      <c r="B122" s="333"/>
+      <c r="C122" s="333"/>
+      <c r="D122" s="333"/>
+      <c r="E122" s="333"/>
+      <c r="F122" s="333"/>
+      <c r="G122" s="333"/>
+      <c r="H122" s="333"/>
+      <c r="I122" s="333"/>
+      <c r="J122" s="333"/>
+      <c r="K122" s="333"/>
     </row>
     <row r="123" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A123" s="1" t="s">
@@ -44700,19 +44699,19 @@
       </c>
     </row>
     <row r="137" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A137" s="327" t="s">
+      <c r="A137" s="333" t="s">
         <v>116</v>
       </c>
-      <c r="B137" s="327"/>
-      <c r="C137" s="327"/>
-      <c r="D137" s="327"/>
-      <c r="E137" s="327"/>
-      <c r="F137" s="327"/>
-      <c r="G137" s="327"/>
-      <c r="H137" s="327"/>
-      <c r="I137" s="327"/>
-      <c r="J137" s="327"/>
-      <c r="K137" s="327"/>
+      <c r="B137" s="333"/>
+      <c r="C137" s="333"/>
+      <c r="D137" s="333"/>
+      <c r="E137" s="333"/>
+      <c r="F137" s="333"/>
+      <c r="G137" s="333"/>
+      <c r="H137" s="333"/>
+      <c r="I137" s="333"/>
+      <c r="J137" s="333"/>
+      <c r="K137" s="333"/>
     </row>
     <row r="138" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A138" s="1" t="s">
@@ -45158,7 +45157,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B9518CF0-901B-4257-8749-E67B3F2BB51B}">
   <dimension ref="B1:AP76"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView topLeftCell="S1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="AS22" sqref="AS22"/>
     </sheetView>
   </sheetViews>
@@ -48034,8 +48033,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C9262DC-E5B7-49F4-A43F-DEF8C5BFDEDE}">
   <dimension ref="A1:V48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="P21" sqref="P21"/>
+    <sheetView tabSelected="1" topLeftCell="C27" workbookViewId="0">
+      <selection activeCell="Q37" sqref="Q37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -48077,12 +48076,12 @@
       <c r="I1" s="31" t="s">
         <v>74</v>
       </c>
-      <c r="L1" s="332" t="s">
+      <c r="L1" s="335" t="s">
         <v>144</v>
       </c>
-      <c r="M1" s="333"/>
-      <c r="N1" s="333"/>
-      <c r="O1" s="333"/>
+      <c r="M1" s="336"/>
+      <c r="N1" s="336"/>
+      <c r="O1" s="336"/>
     </row>
     <row r="2" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A2" s="271" t="s">
@@ -48320,11 +48319,11 @@
       <c r="R6" s="325">
         <v>1.4162913918015331E-2</v>
       </c>
-      <c r="T6" s="336"/>
-      <c r="U6" s="336" t="s">
+      <c r="T6" s="328"/>
+      <c r="U6" s="328" t="s">
         <v>146</v>
       </c>
-      <c r="V6" s="336" t="s">
+      <c r="V6" s="328" t="s">
         <v>147</v>
       </c>
     </row>
@@ -48375,13 +48374,13 @@
       <c r="R7" s="325">
         <v>1.6366473070102194E-2</v>
       </c>
-      <c r="T7" s="334" t="s">
+      <c r="T7" t="s">
         <v>148</v>
       </c>
-      <c r="U7" s="334">
+      <c r="U7">
         <v>3.5104139147676995E-2</v>
       </c>
-      <c r="V7" s="334">
+      <c r="V7">
         <v>3.2701104386462135E-2</v>
       </c>
     </row>
@@ -48429,13 +48428,13 @@
       <c r="R8" s="325">
         <v>1.6280268144578312E-2</v>
       </c>
-      <c r="T8" s="334" t="s">
+      <c r="T8" t="s">
         <v>149</v>
       </c>
-      <c r="U8" s="334">
+      <c r="U8">
         <v>1.9421210788284106E-4</v>
       </c>
-      <c r="V8" s="334">
+      <c r="V8">
         <v>2.3262927213504837E-4</v>
       </c>
     </row>
@@ -48480,13 +48479,13 @@
       <c r="R9" s="325">
         <v>3.4453948702562319E-2</v>
       </c>
-      <c r="T9" s="334" t="s">
+      <c r="T9" t="s">
         <v>150</v>
       </c>
-      <c r="U9" s="334">
+      <c r="U9">
         <v>11</v>
       </c>
-      <c r="V9" s="334">
+      <c r="V9">
         <v>22</v>
       </c>
     </row>
@@ -48531,13 +48530,12 @@
       <c r="R10" s="325">
         <v>6.3932943295208655E-2</v>
       </c>
-      <c r="T10" s="334" t="s">
+      <c r="T10" t="s">
         <v>151</v>
       </c>
-      <c r="U10" s="334">
+      <c r="U10">
         <v>0</v>
       </c>
-      <c r="V10" s="334"/>
     </row>
     <row r="11" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A11" s="279" t="s">
@@ -48580,13 +48578,12 @@
       <c r="R11" s="325">
         <v>1.9121543922762271E-2</v>
       </c>
-      <c r="T11" s="334" t="s">
+      <c r="T11" t="s">
         <v>152</v>
       </c>
-      <c r="U11" s="334">
+      <c r="U11">
         <v>22</v>
       </c>
-      <c r="V11" s="334"/>
     </row>
     <row r="12" spans="1:22" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="289" t="s">
@@ -48629,13 +48626,12 @@
       <c r="R12" s="325">
         <v>4.8123480487998367E-2</v>
       </c>
-      <c r="T12" s="338" t="s">
+      <c r="T12" s="330" t="s">
         <v>153</v>
       </c>
-      <c r="U12" s="338">
+      <c r="U12" s="330">
         <v>0.45227948709057175</v>
       </c>
-      <c r="V12" s="334"/>
     </row>
     <row r="13" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A13" s="57" t="s">
@@ -48678,13 +48674,12 @@
       <c r="R13" s="325">
         <v>5.3229190612098028E-2</v>
       </c>
-      <c r="T13" s="334" t="s">
+      <c r="T13" t="s">
         <v>154</v>
       </c>
-      <c r="U13" s="334">
+      <c r="U13">
         <v>0.32774786846405812</v>
       </c>
-      <c r="V13" s="334"/>
     </row>
     <row r="14" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A14" s="21" t="s">
@@ -48737,13 +48732,12 @@
       <c r="R14" s="325">
         <v>4.1712511737339225E-2</v>
       </c>
-      <c r="T14" s="338" t="s">
+      <c r="T14" s="330" t="s">
         <v>155</v>
       </c>
-      <c r="U14" s="338">
+      <c r="U14" s="330">
         <v>1.7171443743802424</v>
       </c>
-      <c r="V14" s="334"/>
     </row>
     <row r="15" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A15" s="21" t="s">
@@ -48774,29 +48768,28 @@
         <f t="shared" si="0"/>
         <v>1.7886653884458457E-2</v>
       </c>
-      <c r="K15" s="329" t="s">
+      <c r="K15" s="339" t="s">
         <v>145</v>
       </c>
-      <c r="L15" s="330">
+      <c r="L15" s="337">
         <f>AVERAGE(L3:M8)</f>
         <v>3.5104139147676995E-2</v>
       </c>
-      <c r="M15" s="331"/>
-      <c r="N15" s="330">
+      <c r="M15" s="338"/>
+      <c r="N15" s="337">
         <f>AVERAGE(N14:O14)</f>
         <v>3.2701104386462135E-2</v>
       </c>
-      <c r="O15" s="331"/>
+      <c r="O15" s="338"/>
       <c r="R15" s="325">
         <v>4.8660426133989146E-2</v>
       </c>
-      <c r="T15" s="334" t="s">
+      <c r="T15" t="s">
         <v>156</v>
       </c>
-      <c r="U15" s="334">
+      <c r="U15">
         <v>0.65549573692811625</v>
       </c>
-      <c r="V15" s="334"/>
     </row>
     <row r="16" spans="1:22" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A16" s="21" t="s">
@@ -48827,27 +48820,27 @@
         <f t="shared" si="0"/>
         <v>4.1712511737339225E-2</v>
       </c>
-      <c r="K16" s="329"/>
-      <c r="L16" s="330">
+      <c r="K16" s="339"/>
+      <c r="L16" s="337">
         <f>AVERAGE(L14:M14)</f>
         <v>3.5412288377009396E-2</v>
       </c>
-      <c r="M16" s="331"/>
-      <c r="N16" s="330">
+      <c r="M16" s="338"/>
+      <c r="N16" s="337">
         <f>AVERAGE(N14:O14)</f>
         <v>3.2701104386462135E-2</v>
       </c>
-      <c r="O16" s="331"/>
+      <c r="O16" s="338"/>
       <c r="R16" s="325">
         <v>2.2105599118509095E-2</v>
       </c>
-      <c r="T16" s="340" t="s">
+      <c r="T16" s="332" t="s">
         <v>157</v>
       </c>
-      <c r="U16" s="340">
+      <c r="U16" s="332">
         <v>2.0738730679040258</v>
       </c>
-      <c r="V16" s="335"/>
+      <c r="V16" s="327"/>
     </row>
     <row r="17" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A17" s="21" t="s">
@@ -48914,16 +48907,16 @@
       <c r="K18" s="32" t="s">
         <v>142</v>
       </c>
-      <c r="L18" s="330">
+      <c r="L18" s="337">
         <f xml:space="preserve"> MEDIAN(L3:M8)</f>
         <v>3.2583484975625902E-2</v>
       </c>
-      <c r="M18" s="330"/>
-      <c r="N18" s="330">
+      <c r="M18" s="337"/>
+      <c r="N18" s="337">
         <f>MEDIAN(N3:O13)</f>
         <v>3.4234778327276894E-2</v>
       </c>
-      <c r="O18" s="330"/>
+      <c r="O18" s="337"/>
       <c r="R18" s="325">
         <v>7.8753014642203526E-3</v>
       </c>
@@ -49013,11 +49006,11 @@
       <c r="R20" s="325">
         <v>4.2561740354097384E-2</v>
       </c>
-      <c r="T20" s="336"/>
-      <c r="U20" s="336" t="s">
+      <c r="T20" s="328"/>
+      <c r="U20" s="328" t="s">
         <v>180</v>
       </c>
-      <c r="V20" s="336" t="s">
+      <c r="V20" s="328" t="s">
         <v>181</v>
       </c>
     </row>
@@ -49053,13 +49046,13 @@
       <c r="R21" s="325">
         <v>3.8038774552472371E-2</v>
       </c>
-      <c r="T21" s="334" t="s">
+      <c r="T21" t="s">
         <v>148</v>
       </c>
-      <c r="U21" s="334">
+      <c r="U21">
         <v>3.5104139147676995E-2</v>
       </c>
-      <c r="V21" s="334">
+      <c r="V21">
         <v>3.2701104386462135E-2</v>
       </c>
     </row>
@@ -49095,13 +49088,13 @@
       <c r="R22" s="325">
         <v>4.1529324627726745E-2</v>
       </c>
-      <c r="T22" s="334" t="s">
+      <c r="T22" t="s">
         <v>149</v>
       </c>
-      <c r="U22" s="334">
+      <c r="U22">
         <v>1.9421210788284106E-4</v>
       </c>
-      <c r="V22" s="334">
+      <c r="V22">
         <v>2.3262927213504837E-4</v>
       </c>
     </row>
@@ -49137,13 +49130,13 @@
       <c r="R23" s="325">
         <v>3.1173460359890111E-2</v>
       </c>
-      <c r="T23" s="334" t="s">
+      <c r="T23" t="s">
         <v>150</v>
       </c>
-      <c r="U23" s="334">
+      <c r="U23">
         <v>11</v>
       </c>
-      <c r="V23" s="334">
+      <c r="V23">
         <v>22</v>
       </c>
     </row>
@@ -49179,13 +49172,13 @@
       <c r="R24" s="325">
         <v>3.0115005225647792E-2</v>
       </c>
-      <c r="T24" s="334" t="s">
+      <c r="T24" t="s">
         <v>152</v>
       </c>
-      <c r="U24" s="334">
+      <c r="U24">
         <v>10</v>
       </c>
-      <c r="V24" s="334">
+      <c r="V24">
         <v>21</v>
       </c>
     </row>
@@ -49218,13 +49211,12 @@
         <f t="shared" si="0"/>
         <v>3.4453948702562319E-2</v>
       </c>
-      <c r="T25" s="338" t="s">
+      <c r="T25" s="330" t="s">
         <v>160</v>
       </c>
-      <c r="U25" s="338">
+      <c r="U25" s="330">
         <v>0.83485670612464902</v>
       </c>
-      <c r="V25" s="334"/>
     </row>
     <row r="26" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A26" s="21" t="s">
@@ -49257,13 +49249,12 @@
       </c>
       <c r="Q26" s="315"/>
       <c r="R26" s="315"/>
-      <c r="T26" s="334" t="s">
+      <c r="T26" t="s">
         <v>161</v>
       </c>
-      <c r="U26" s="334">
+      <c r="U26">
         <v>0.39817739333655444</v>
       </c>
-      <c r="V26" s="334"/>
     </row>
     <row r="27" spans="1:22" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A27" s="21" t="s">
@@ -49294,13 +49285,13 @@
         <f t="shared" si="0"/>
         <v>1.9121543922762271E-2</v>
       </c>
-      <c r="T27" s="340" t="s">
+      <c r="T27" s="332" t="s">
         <v>162</v>
       </c>
-      <c r="U27" s="340">
+      <c r="U27" s="332">
         <v>0.36184662174130539</v>
       </c>
-      <c r="V27" s="335"/>
+      <c r="V27" s="327"/>
     </row>
     <row r="28" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A28" s="21" t="s">
@@ -49391,14 +49382,14 @@
         <f t="shared" si="0"/>
         <v>4.1529324627726745E-2</v>
       </c>
-      <c r="K30" s="337" t="s">
+      <c r="K30" s="329" t="s">
         <v>176</v>
       </c>
-      <c r="L30" s="337"/>
-      <c r="N30" s="337" t="s">
+      <c r="L30" s="329"/>
+      <c r="N30" s="329" t="s">
         <v>177</v>
       </c>
-      <c r="O30" s="337"/>
+      <c r="O30" s="329"/>
     </row>
     <row r="31" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A31" s="57" t="s">
@@ -49429,10 +49420,6 @@
         <f t="shared" si="0"/>
         <v>4.8123480487998367E-2</v>
       </c>
-      <c r="K31" s="334"/>
-      <c r="L31" s="334"/>
-      <c r="N31" s="334"/>
-      <c r="O31" s="334"/>
     </row>
     <row r="32" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A32" s="21" t="s">
@@ -49463,16 +49450,16 @@
         <f t="shared" si="0"/>
         <v>5.3229190612098028E-2</v>
       </c>
-      <c r="K32" s="334" t="s">
+      <c r="K32" t="s">
         <v>148</v>
       </c>
-      <c r="L32" s="334">
+      <c r="L32">
         <v>3.5104139147676995E-2</v>
       </c>
-      <c r="N32" s="334" t="s">
+      <c r="N32" t="s">
         <v>148</v>
       </c>
-      <c r="O32" s="334">
+      <c r="O32">
         <v>3.2701104386462135E-2</v>
       </c>
     </row>
@@ -49505,16 +49492,16 @@
         <f>C33/B33</f>
         <v>0.1477072933292011</v>
       </c>
-      <c r="K33" s="334" t="s">
+      <c r="K33" t="s">
         <v>163</v>
       </c>
-      <c r="L33" s="334">
+      <c r="L33">
         <v>4.2018622265808962E-3</v>
       </c>
-      <c r="N33" s="334" t="s">
+      <c r="N33" t="s">
         <v>163</v>
       </c>
-      <c r="O33" s="334">
+      <c r="O33">
         <v>3.2517776406637E-3</v>
       </c>
     </row>
@@ -49547,16 +49534,16 @@
         <f t="shared" si="0"/>
         <v>3.1173460359890111E-2</v>
       </c>
-      <c r="K34" s="334" t="s">
+      <c r="K34" t="s">
         <v>164</v>
       </c>
-      <c r="L34" s="334">
+      <c r="L34">
         <v>3.2583484975625902E-2</v>
       </c>
-      <c r="N34" s="334" t="s">
+      <c r="N34" t="s">
         <v>164</v>
       </c>
-      <c r="O34" s="334">
+      <c r="O34">
         <v>3.4234778327276894E-2</v>
       </c>
     </row>
@@ -49589,157 +49576,157 @@
         <f t="shared" si="0"/>
         <v>3.0115005225647792E-2</v>
       </c>
-      <c r="K35" s="334" t="s">
+      <c r="K35" t="s">
         <v>165</v>
       </c>
-      <c r="L35" s="334" t="e">
+      <c r="L35" t="e">
         <v>#N/A</v>
       </c>
-      <c r="N35" s="334" t="s">
+      <c r="N35" t="s">
         <v>165</v>
       </c>
-      <c r="O35" s="334" t="e">
+      <c r="O35" t="e">
         <v>#N/A</v>
       </c>
     </row>
     <row r="36" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="K36" s="334" t="s">
+      <c r="K36" t="s">
         <v>166</v>
       </c>
-      <c r="L36" s="334">
+      <c r="L36">
         <v>1.3936000426336139E-2</v>
       </c>
-      <c r="N36" s="334" t="s">
+      <c r="N36" t="s">
         <v>166</v>
       </c>
-      <c r="O36" s="334">
+      <c r="O36">
         <v>1.5252189093210468E-2</v>
       </c>
     </row>
     <row r="37" spans="1:15" x14ac:dyDescent="0.3">
       <c r="I37" s="315"/>
-      <c r="K37" s="334" t="s">
+      <c r="K37" t="s">
         <v>167</v>
       </c>
-      <c r="L37" s="334">
+      <c r="L37">
         <v>1.9421210788284106E-4</v>
       </c>
-      <c r="N37" s="334" t="s">
+      <c r="N37" t="s">
         <v>167</v>
       </c>
-      <c r="O37" s="334">
+      <c r="O37">
         <v>2.3262927213504837E-4</v>
       </c>
     </row>
     <row r="38" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="K38" s="338" t="s">
+      <c r="K38" s="330" t="s">
         <v>168</v>
       </c>
-      <c r="L38" s="338">
+      <c r="L38" s="330">
         <v>-0.58388498219898066</v>
       </c>
-      <c r="N38" s="338" t="s">
+      <c r="N38" s="330" t="s">
         <v>168</v>
       </c>
-      <c r="O38" s="338">
+      <c r="O38" s="330">
         <v>-0.85160074372777483</v>
       </c>
     </row>
     <row r="39" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="K39" s="338" t="s">
+      <c r="K39" s="330" t="s">
         <v>169</v>
       </c>
-      <c r="L39" s="338">
+      <c r="L39" s="330">
         <v>-5.7064657840578417E-2</v>
       </c>
-      <c r="N39" s="338" t="s">
+      <c r="N39" s="330" t="s">
         <v>169</v>
       </c>
-      <c r="O39" s="338">
+      <c r="O39" s="330">
         <v>0.10948740809552054</v>
       </c>
     </row>
     <row r="40" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="K40" s="334" t="s">
+      <c r="K40" t="s">
         <v>170</v>
       </c>
-      <c r="L40" s="334">
+      <c r="L40">
         <v>4.7092637399855197E-2</v>
       </c>
-      <c r="N40" s="334" t="s">
+      <c r="N40" t="s">
         <v>170</v>
       </c>
-      <c r="O40" s="334">
+      <c r="O40">
         <v>5.6057641830988304E-2</v>
       </c>
     </row>
     <row r="41" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="K41" s="334" t="s">
+      <c r="K41" t="s">
         <v>171</v>
       </c>
-      <c r="L41" s="334">
+      <c r="L41">
         <v>1.0746867809774435E-2</v>
       </c>
-      <c r="N41" s="334" t="s">
+      <c r="N41" t="s">
         <v>171</v>
       </c>
-      <c r="O41" s="334">
+      <c r="O41">
         <v>7.8753014642203526E-3</v>
       </c>
     </row>
     <row r="42" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="K42" s="334" t="s">
+      <c r="K42" t="s">
         <v>172</v>
       </c>
-      <c r="L42" s="334">
+      <c r="L42">
         <v>5.7839505209629632E-2</v>
       </c>
-      <c r="N42" s="334" t="s">
+      <c r="N42" t="s">
         <v>172</v>
       </c>
-      <c r="O42" s="334">
+      <c r="O42">
         <v>6.3932943295208655E-2</v>
       </c>
     </row>
     <row r="43" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="K43" s="334" t="s">
+      <c r="K43" t="s">
         <v>173</v>
       </c>
-      <c r="L43" s="334">
+      <c r="L43">
         <v>0.38614553062444695</v>
       </c>
-      <c r="N43" s="334" t="s">
+      <c r="N43" t="s">
         <v>173</v>
       </c>
-      <c r="O43" s="334">
+      <c r="O43">
         <v>0.71942429650216699</v>
       </c>
     </row>
     <row r="44" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="K44" s="338" t="s">
+      <c r="K44" s="330" t="s">
         <v>174</v>
       </c>
-      <c r="L44" s="338">
+      <c r="L44" s="330">
         <v>11</v>
       </c>
-      <c r="N44" s="338" t="s">
+      <c r="N44" s="330" t="s">
         <v>174</v>
       </c>
-      <c r="O44" s="338">
+      <c r="O44" s="330">
         <v>22</v>
       </c>
     </row>
     <row r="45" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="K45" s="335" t="s">
+      <c r="K45" s="327" t="s">
         <v>175</v>
       </c>
-      <c r="L45" s="335">
+      <c r="L45" s="327">
         <v>9.3623324777384487E-3</v>
       </c>
-      <c r="N45" s="335" t="s">
+      <c r="N45" s="327" t="s">
         <v>175</v>
       </c>
-      <c r="O45" s="335">
+      <c r="O45" s="327">
         <v>6.7624418015001415E-3</v>
       </c>
     </row>
@@ -49760,17 +49747,17 @@
       </c>
     </row>
     <row r="48" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="K48" s="339" t="s">
+      <c r="K48" s="331" t="s">
         <v>179</v>
       </c>
-      <c r="L48" s="339">
+      <c r="L48" s="331">
         <f>_xlfn.CHISQ.DIST.RT(L47, 2)</f>
         <v>0.92208958733077973</v>
       </c>
-      <c r="N48" s="339" t="s">
+      <c r="N48" s="331" t="s">
         <v>179</v>
       </c>
-      <c r="O48" s="339">
+      <c r="O48" s="331">
         <f>_xlfn.CHISQ.DIST.RT(O47, 2)</f>
         <v>0.701614393030218</v>
       </c>

</xml_diff>

<commit_message>
viendo carbon concentrations for jesus
</commit_message>
<xml_diff>
--- a/Bed_Carbon/Carbon_Sediment_Samples.xlsx
+++ b/Bed_Carbon/Carbon_Sediment_Samples.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nicol\Documents\GitHub\La_Jara\Bed_Carbon\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA88580D-8D5B-4CB9-A098-D80B5D8C631C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A72E3245-279F-4DDC-B1CC-FBEC456B564A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{797E201D-8F44-4DD9-9B42-7B8F6976B830}"/>
+    <workbookView xWindow="11424" yWindow="0" windowWidth="11712" windowHeight="12336" xr2:uid="{797E201D-8F44-4DD9-9B42-7B8F6976B830}"/>
   </bookViews>
   <sheets>
     <sheet name="All Samples" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="823" uniqueCount="182">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="829" uniqueCount="188">
   <si>
     <t>Name</t>
   </si>
@@ -585,6 +585,24 @@
   </si>
   <si>
     <t>SM</t>
+  </si>
+  <si>
+    <t>avg mgC</t>
+  </si>
+  <si>
+    <t>avg mgC/mg</t>
+  </si>
+  <si>
+    <t>min mgC</t>
+  </si>
+  <si>
+    <t>min mgC/mg</t>
+  </si>
+  <si>
+    <t>max mgC</t>
+  </si>
+  <si>
+    <t>max mgC/mg</t>
   </si>
 </sst>
 </file>
@@ -2107,7 +2125,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>'All Samples'!$N$36:$N$44</c:f>
+              <c:f>'All Samples'!$O$36:$O$44</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
                 <c:ptCount val="9"/>
@@ -2143,7 +2161,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'All Samples'!$O$36:$O$44</c:f>
+              <c:f>'All Samples'!$P$36:$P$44</c:f>
               <c:numCache>
                 <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="9"/>
@@ -2216,7 +2234,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>'All Samples'!$N$46:$N$57</c:f>
+              <c:f>'All Samples'!$O$46:$O$57</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
                 <c:ptCount val="12"/>
@@ -2261,7 +2279,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'All Samples'!$O$46:$O$57</c:f>
+              <c:f>'All Samples'!$P$46:$P$57</c:f>
               <c:numCache>
                 <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="12"/>
@@ -2343,7 +2361,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>'All Samples'!$N$59:$N$68</c:f>
+              <c:f>'All Samples'!$O$59:$O$68</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
                 <c:ptCount val="10"/>
@@ -2382,7 +2400,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'All Samples'!$O$59:$O$68</c:f>
+              <c:f>'All Samples'!$P$59:$P$68</c:f>
               <c:numCache>
                 <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="10"/>
@@ -2751,7 +2769,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>'All Samples'!$N$71:$N$78</c:f>
+              <c:f>'All Samples'!$O$71:$O$78</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
                 <c:ptCount val="8"/>
@@ -2784,7 +2802,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'All Samples'!$S$71:$S$78</c:f>
+              <c:f>'All Samples'!$T$71:$T$78</c:f>
               <c:numCache>
                 <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="8"/>
@@ -2854,7 +2872,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>'All Samples'!$N$80:$N$92</c:f>
+              <c:f>'All Samples'!$O$80:$O$92</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
                 <c:ptCount val="13"/>
@@ -2902,7 +2920,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'All Samples'!$S$80:$S$92</c:f>
+              <c:f>'All Samples'!$T$80:$T$92</c:f>
               <c:numCache>
                 <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="13"/>
@@ -2987,7 +3005,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>'All Samples'!$N$94:$N$105</c:f>
+              <c:f>'All Samples'!$O$94:$O$105</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
                 <c:ptCount val="12"/>
@@ -3032,7 +3050,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'All Samples'!$S$94:$S$105</c:f>
+              <c:f>'All Samples'!$T$94:$T$105</c:f>
               <c:numCache>
                 <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="12"/>
@@ -5939,7 +5957,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="es-AR"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -6817,7 +6835,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="es-AR"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -7677,7 +7695,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="es-AR"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -8489,7 +8507,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="es-AR"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -9283,7 +9301,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="es-AR"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -9910,7 +9928,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>'All Samples'!$N$36:$N$44</c:f>
+              <c:f>'All Samples'!$O$36:$O$44</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
                 <c:ptCount val="9"/>
@@ -9946,7 +9964,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'All Samples'!$P$36:$P$44</c:f>
+              <c:f>'All Samples'!$Q$36:$Q$44</c:f>
               <c:numCache>
                 <c:formatCode>0.0000</c:formatCode>
                 <c:ptCount val="9"/>
@@ -10019,7 +10037,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>'All Samples'!$N$46:$N$57</c:f>
+              <c:f>'All Samples'!$O$46:$O$57</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
                 <c:ptCount val="12"/>
@@ -10064,7 +10082,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'All Samples'!$P$46:$P$57</c:f>
+              <c:f>'All Samples'!$Q$46:$Q$57</c:f>
               <c:numCache>
                 <c:formatCode>0.0000</c:formatCode>
                 <c:ptCount val="12"/>
@@ -10146,7 +10164,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>'All Samples'!$N$59:$N$68</c:f>
+              <c:f>'All Samples'!$O$59:$O$68</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
                 <c:ptCount val="10"/>
@@ -10185,7 +10203,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'All Samples'!$P$59:$P$68</c:f>
+              <c:f>'All Samples'!$Q$59:$Q$68</c:f>
               <c:numCache>
                 <c:formatCode>0.0000</c:formatCode>
                 <c:ptCount val="10"/>
@@ -10517,7 +10535,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="es-AR"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -11107,7 +11125,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="es-AR"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -11673,7 +11691,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="es-AR"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -12239,7 +12257,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="es-AR"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -12817,7 +12835,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="es-AR"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -13432,7 +13450,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>'All Samples'!$N$71:$N$78</c:f>
+              <c:f>'All Samples'!$O$71:$O$78</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
                 <c:ptCount val="8"/>
@@ -13465,7 +13483,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'All Samples'!$P$71:$P$78</c:f>
+              <c:f>'All Samples'!$Q$71:$Q$78</c:f>
               <c:numCache>
                 <c:formatCode>0.0000</c:formatCode>
                 <c:ptCount val="8"/>
@@ -13535,7 +13553,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>'All Samples'!$N$80:$N$92</c:f>
+              <c:f>'All Samples'!$O$80:$O$92</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
                 <c:ptCount val="13"/>
@@ -13583,7 +13601,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'All Samples'!$P$80:$P$92</c:f>
+              <c:f>'All Samples'!$Q$80:$Q$92</c:f>
               <c:numCache>
                 <c:formatCode>0.0000</c:formatCode>
                 <c:ptCount val="13"/>
@@ -13668,7 +13686,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>'All Samples'!$N$94:$N$105</c:f>
+              <c:f>'All Samples'!$O$94:$O$105</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
                 <c:ptCount val="12"/>
@@ -13713,7 +13731,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'All Samples'!$P$94:$P$105</c:f>
+              <c:f>'All Samples'!$Q$94:$Q$105</c:f>
               <c:numCache>
                 <c:formatCode>0.0000</c:formatCode>
                 <c:ptCount val="12"/>
@@ -14088,7 +14106,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>'All Samples'!$N$71:$N$78</c:f>
+              <c:f>'All Samples'!$O$71:$O$78</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
                 <c:ptCount val="8"/>
@@ -14121,7 +14139,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'All Samples'!$O$71:$O$78</c:f>
+              <c:f>'All Samples'!$P$71:$P$78</c:f>
               <c:numCache>
                 <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="8"/>
@@ -14191,7 +14209,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>'All Samples'!$N$80:$N$92</c:f>
+              <c:f>'All Samples'!$O$80:$O$92</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
                 <c:ptCount val="13"/>
@@ -14239,7 +14257,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'All Samples'!$O$80:$O$92</c:f>
+              <c:f>'All Samples'!$P$80:$P$92</c:f>
               <c:numCache>
                 <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="13"/>
@@ -14324,7 +14342,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>'All Samples'!$N$94:$N$105</c:f>
+              <c:f>'All Samples'!$O$94:$O$105</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
                 <c:ptCount val="12"/>
@@ -14369,7 +14387,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'All Samples'!$O$94:$O$105</c:f>
+              <c:f>'All Samples'!$P$94:$P$105</c:f>
               <c:numCache>
                 <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="12"/>
@@ -14744,7 +14762,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>'All Samples'!$N$36:$N$44</c:f>
+              <c:f>'All Samples'!$O$36:$O$44</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
                 <c:ptCount val="9"/>
@@ -14780,7 +14798,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'All Samples'!$Q$36:$Q$44</c:f>
+              <c:f>'All Samples'!$R$36:$R$44</c:f>
               <c:numCache>
                 <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="9"/>
@@ -14853,7 +14871,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>'All Samples'!$N$46:$N$57</c:f>
+              <c:f>'All Samples'!$O$46:$O$57</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
                 <c:ptCount val="12"/>
@@ -14898,7 +14916,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'All Samples'!$Q$46:$Q$57</c:f>
+              <c:f>'All Samples'!$R$46:$R$57</c:f>
               <c:numCache>
                 <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="12"/>
@@ -14980,7 +14998,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>'All Samples'!$N$59:$N$68</c:f>
+              <c:f>'All Samples'!$O$59:$O$68</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
                 <c:ptCount val="10"/>
@@ -15019,7 +15037,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'All Samples'!$Q$59:$Q$68</c:f>
+              <c:f>'All Samples'!$R$59:$R$68</c:f>
               <c:numCache>
                 <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="10"/>
@@ -15385,7 +15403,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>'All Samples'!$N$71:$N$78</c:f>
+              <c:f>'All Samples'!$O$71:$O$78</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
                 <c:ptCount val="8"/>
@@ -15418,7 +15436,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'All Samples'!$Q$71:$Q$78</c:f>
+              <c:f>'All Samples'!$R$71:$R$78</c:f>
               <c:numCache>
                 <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="8"/>
@@ -15488,7 +15506,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>'All Samples'!$N$80:$N$92</c:f>
+              <c:f>'All Samples'!$O$80:$O$92</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
                 <c:ptCount val="13"/>
@@ -15536,7 +15554,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'All Samples'!$Q$80:$Q$92</c:f>
+              <c:f>'All Samples'!$R$80:$R$92</c:f>
               <c:numCache>
                 <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="13"/>
@@ -15621,7 +15639,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>'All Samples'!$N$94:$N$105</c:f>
+              <c:f>'All Samples'!$O$94:$O$105</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
                 <c:ptCount val="12"/>
@@ -15666,7 +15684,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'All Samples'!$Q$94:$Q$105</c:f>
+              <c:f>'All Samples'!$R$94:$R$105</c:f>
               <c:numCache>
                 <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="12"/>
@@ -16049,7 +16067,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>'All Samples'!$N$36:$N$44</c:f>
+              <c:f>'All Samples'!$O$36:$O$44</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
                 <c:ptCount val="9"/>
@@ -16085,7 +16103,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'All Samples'!$R$36:$R$44</c:f>
+              <c:f>'All Samples'!$S$36:$S$44</c:f>
               <c:numCache>
                 <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="9"/>
@@ -16158,7 +16176,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>'All Samples'!$N$46:$N$57</c:f>
+              <c:f>'All Samples'!$O$46:$O$57</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
                 <c:ptCount val="12"/>
@@ -16203,7 +16221,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'All Samples'!$R$46:$R$57</c:f>
+              <c:f>'All Samples'!$S$46:$S$57</c:f>
               <c:numCache>
                 <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="12"/>
@@ -16285,7 +16303,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>'All Samples'!$N$59:$N$68</c:f>
+              <c:f>'All Samples'!$O$59:$O$68</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
                 <c:ptCount val="10"/>
@@ -16324,7 +16342,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'All Samples'!$R$59:$R$68</c:f>
+              <c:f>'All Samples'!$S$59:$S$68</c:f>
               <c:numCache>
                 <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="10"/>
@@ -16693,7 +16711,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>'All Samples'!$N$71:$N$78</c:f>
+              <c:f>'All Samples'!$O$71:$O$78</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
                 <c:ptCount val="8"/>
@@ -16726,7 +16744,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'All Samples'!$R$71:$R$78</c:f>
+              <c:f>'All Samples'!$S$71:$S$78</c:f>
               <c:numCache>
                 <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="8"/>
@@ -16796,7 +16814,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>'All Samples'!$N$80:$N$92</c:f>
+              <c:f>'All Samples'!$O$80:$O$92</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
                 <c:ptCount val="13"/>
@@ -16844,7 +16862,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'All Samples'!$R$80:$R$92</c:f>
+              <c:f>'All Samples'!$S$80:$S$92</c:f>
               <c:numCache>
                 <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="13"/>
@@ -16929,7 +16947,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>'All Samples'!$N$94:$N$105</c:f>
+              <c:f>'All Samples'!$O$94:$O$105</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
                 <c:ptCount val="12"/>
@@ -16974,7 +16992,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'All Samples'!$R$94:$R$105</c:f>
+              <c:f>'All Samples'!$S$94:$S$105</c:f>
               <c:numCache>
                 <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="12"/>
@@ -17357,7 +17375,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>'All Samples'!$N$36:$N$44</c:f>
+              <c:f>'All Samples'!$O$36:$O$44</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
                 <c:ptCount val="9"/>
@@ -17393,7 +17411,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'All Samples'!$S$36:$S$44</c:f>
+              <c:f>'All Samples'!$T$36:$T$44</c:f>
               <c:numCache>
                 <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="9"/>
@@ -17466,7 +17484,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>'All Samples'!$N$46:$N$57</c:f>
+              <c:f>'All Samples'!$O$46:$O$57</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
                 <c:ptCount val="12"/>
@@ -17511,7 +17529,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'All Samples'!$S$46:$S$57</c:f>
+              <c:f>'All Samples'!$T$46:$T$57</c:f>
               <c:numCache>
                 <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="12"/>
@@ -17593,7 +17611,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>'All Samples'!$N$59:$N$68</c:f>
+              <c:f>'All Samples'!$O$59:$O$68</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
                 <c:ptCount val="10"/>
@@ -17632,7 +17650,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'All Samples'!$S$59:$S$68</c:f>
+              <c:f>'All Samples'!$T$59:$T$68</c:f>
               <c:numCache>
                 <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="10"/>
@@ -31227,13 +31245,13 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>13</xdr:col>
+      <xdr:col>14</xdr:col>
       <xdr:colOff>109370</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>92504</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>26</xdr:col>
+      <xdr:col>27</xdr:col>
       <xdr:colOff>544941</xdr:colOff>
       <xdr:row>15</xdr:row>
       <xdr:rowOff>126795</xdr:rowOff>
@@ -31263,13 +31281,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>27</xdr:col>
+      <xdr:col>28</xdr:col>
       <xdr:colOff>44823</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>108248</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>42</xdr:col>
+      <xdr:col>43</xdr:col>
       <xdr:colOff>446</xdr:colOff>
       <xdr:row>15</xdr:row>
       <xdr:rowOff>146349</xdr:rowOff>
@@ -31301,13 +31319,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>27</xdr:col>
+      <xdr:col>28</xdr:col>
       <xdr:colOff>78442</xdr:colOff>
       <xdr:row>16</xdr:row>
       <xdr:rowOff>112058</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>42</xdr:col>
+      <xdr:col>43</xdr:col>
       <xdr:colOff>24540</xdr:colOff>
       <xdr:row>31</xdr:row>
       <xdr:rowOff>149934</xdr:rowOff>
@@ -31339,13 +31357,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>13</xdr:col>
+      <xdr:col>14</xdr:col>
       <xdr:colOff>89647</xdr:colOff>
       <xdr:row>16</xdr:row>
       <xdr:rowOff>123264</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>26</xdr:col>
+      <xdr:col>27</xdr:col>
       <xdr:colOff>517598</xdr:colOff>
       <xdr:row>31</xdr:row>
       <xdr:rowOff>159235</xdr:rowOff>
@@ -31377,13 +31395,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>20</xdr:col>
+      <xdr:col>21</xdr:col>
       <xdr:colOff>22412</xdr:colOff>
       <xdr:row>32</xdr:row>
       <xdr:rowOff>171899</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>35</xdr:col>
+      <xdr:col>36</xdr:col>
       <xdr:colOff>44824</xdr:colOff>
       <xdr:row>48</xdr:row>
       <xdr:rowOff>152066</xdr:rowOff>
@@ -31415,13 +31433,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>20</xdr:col>
+      <xdr:col>21</xdr:col>
       <xdr:colOff>33619</xdr:colOff>
       <xdr:row>49</xdr:row>
       <xdr:rowOff>89871</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>34</xdr:col>
+      <xdr:col>35</xdr:col>
       <xdr:colOff>579120</xdr:colOff>
       <xdr:row>64</xdr:row>
       <xdr:rowOff>140858</xdr:rowOff>
@@ -31453,13 +31471,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>20</xdr:col>
+      <xdr:col>21</xdr:col>
       <xdr:colOff>22412</xdr:colOff>
       <xdr:row>68</xdr:row>
       <xdr:rowOff>44824</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>35</xdr:col>
+      <xdr:col>36</xdr:col>
       <xdr:colOff>48634</xdr:colOff>
       <xdr:row>84</xdr:row>
       <xdr:rowOff>55022</xdr:rowOff>
@@ -31491,13 +31509,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>20</xdr:col>
+      <xdr:col>21</xdr:col>
       <xdr:colOff>39334</xdr:colOff>
       <xdr:row>84</xdr:row>
       <xdr:rowOff>168312</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>34</xdr:col>
+      <xdr:col>35</xdr:col>
       <xdr:colOff>582930</xdr:colOff>
       <xdr:row>100</xdr:row>
       <xdr:rowOff>54796</xdr:rowOff>
@@ -31529,13 +31547,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>35</xdr:col>
+      <xdr:col>36</xdr:col>
       <xdr:colOff>224118</xdr:colOff>
       <xdr:row>68</xdr:row>
       <xdr:rowOff>33618</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>50</xdr:col>
+      <xdr:col>51</xdr:col>
       <xdr:colOff>254149</xdr:colOff>
       <xdr:row>84</xdr:row>
       <xdr:rowOff>41911</xdr:rowOff>
@@ -31567,13 +31585,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>35</xdr:col>
+      <xdr:col>36</xdr:col>
       <xdr:colOff>241040</xdr:colOff>
       <xdr:row>84</xdr:row>
       <xdr:rowOff>155201</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>50</xdr:col>
+      <xdr:col>51</xdr:col>
       <xdr:colOff>187138</xdr:colOff>
       <xdr:row>100</xdr:row>
       <xdr:rowOff>41685</xdr:rowOff>
@@ -32964,10 +32982,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{49720B70-5BE3-4E08-B389-4F33CC21E2D2}">
-  <dimension ref="A1:S105"/>
+  <dimension ref="A1:T105"/>
   <sheetViews>
-    <sheetView topLeftCell="P1" zoomScale="83" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="AJ37" sqref="AJ37"/>
+    <sheetView tabSelected="1" topLeftCell="A44" zoomScale="72" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="K55" sqref="K55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -32978,12 +32996,12 @@
     <col min="10" max="10" width="16.33203125" style="32" customWidth="1"/>
     <col min="11" max="11" width="15.88671875" customWidth="1"/>
     <col min="12" max="12" width="10.21875" customWidth="1"/>
-    <col min="13" max="13" width="17.77734375" customWidth="1"/>
-    <col min="14" max="14" width="16.77734375" customWidth="1"/>
-    <col min="15" max="15" width="11.6640625" customWidth="1"/>
+    <col min="13" max="14" width="17.77734375" customWidth="1"/>
+    <col min="15" max="15" width="16.77734375" customWidth="1"/>
+    <col min="16" max="16" width="11.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A1" s="20" t="s">
         <v>0</v>
       </c>
@@ -33021,7 +33039,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>15</v>
       </c>
@@ -33060,8 +33078,14 @@
         <f>G2/B2</f>
         <v>-7.7465857446808476E-4</v>
       </c>
+      <c r="M2" s="32" t="s">
+        <v>182</v>
+      </c>
+      <c r="N2" s="32" t="s">
+        <v>183</v>
+      </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>16</v>
       </c>
@@ -33100,8 +33124,16 @@
         <f t="shared" ref="L3:L66" si="1">G3/B3</f>
         <v>1.0369328240675921E-3</v>
       </c>
+      <c r="M3" s="164">
+        <f>AVERAGE(E2:E70)</f>
+        <v>6.2651828826255862E-2</v>
+      </c>
+      <c r="N3" s="164">
+        <f>AVERAGE(K2:K70)</f>
+        <v>3.0977258692568937E-2</v>
+      </c>
     </row>
-    <row r="4" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="104" t="s">
         <v>17</v>
       </c>
@@ -33141,7 +33173,7 @@
         <v>-1.8794106280126401E-3</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A5" s="113" t="s">
         <v>11</v>
       </c>
@@ -33180,8 +33212,14 @@
         <f t="shared" si="1"/>
         <v>1.2061318035695877E-2</v>
       </c>
+      <c r="M5" s="32" t="s">
+        <v>184</v>
+      </c>
+      <c r="N5" s="32" t="s">
+        <v>185</v>
+      </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A6" s="51" t="s">
         <v>13</v>
       </c>
@@ -33220,8 +33258,16 @@
         <f t="shared" si="1"/>
         <v>9.6894732532614507E-5</v>
       </c>
+      <c r="M6" s="164">
+        <f>MIN(E2:E70)</f>
+        <v>1.230196078646875E-2</v>
+      </c>
+      <c r="N6" s="164">
+        <f>MIN(K2:K70)</f>
+        <v>6.4307165637578411E-3</v>
+      </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A7" s="65" t="s">
         <v>10</v>
       </c>
@@ -33261,7 +33307,7 @@
         <v>1.1595263660704859E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A8" s="120" t="s">
         <v>12</v>
       </c>
@@ -33300,8 +33346,14 @@
         <f t="shared" si="1"/>
         <v>1.7454287453069798E-3</v>
       </c>
+      <c r="M8" s="32" t="s">
+        <v>186</v>
+      </c>
+      <c r="N8" s="32" t="s">
+        <v>187</v>
+      </c>
     </row>
-    <row r="9" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="139" t="s">
         <v>14</v>
       </c>
@@ -33340,8 +33392,16 @@
         <f t="shared" si="1"/>
         <v>1.5683176995033121E-3</v>
       </c>
+      <c r="M9" s="164">
+        <f>MAX(E2:E70)</f>
+        <v>0.32170648487100001</v>
+      </c>
+      <c r="N9" s="164">
+        <f>MAX(K2:K70)</f>
+        <v>0.1477072933292011</v>
+      </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A10" s="113" t="s">
         <v>20</v>
       </c>
@@ -33381,7 +33441,7 @@
         <v>1.3292377521363417E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A11" s="51" t="s">
         <v>18</v>
       </c>
@@ -33421,7 +33481,7 @@
         <v>1.0369517155732347E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A12" s="65" t="s">
         <v>21</v>
       </c>
@@ -33461,7 +33521,7 @@
         <v>6.8922560718681701E-4</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A13" s="122" t="s">
         <v>19</v>
       </c>
@@ -33501,7 +33561,7 @@
         <v>1.0901794040645514E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A14" s="120" t="s">
         <v>23</v>
       </c>
@@ -33541,7 +33601,7 @@
         <v>9.3291047016118983E-4</v>
       </c>
     </row>
-    <row r="15" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A15" s="139" t="s">
         <v>22</v>
       </c>
@@ -33581,7 +33641,7 @@
         <v>1.9023096757851137E-3</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A16" s="113" t="s">
         <v>25</v>
       </c>
@@ -33621,7 +33681,7 @@
         <v>2.5853732185710876E-3</v>
       </c>
     </row>
-    <row r="17" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A17" s="51" t="s">
         <v>26</v>
       </c>
@@ -33660,11 +33720,11 @@
         <f t="shared" si="1"/>
         <v>1.7001195690658248E-3</v>
       </c>
-      <c r="R17" t="s">
+      <c r="S17" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="18" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A18" s="65" t="s">
         <v>27</v>
       </c>
@@ -33704,7 +33764,7 @@
         <v>1.6796037884212729E-3</v>
       </c>
     </row>
-    <row r="19" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A19" s="122" t="s">
         <v>24</v>
       </c>
@@ -33744,7 +33804,7 @@
         <v>7.1540883650046531E-4</v>
       </c>
     </row>
-    <row r="20" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A20" s="120" t="s">
         <v>29</v>
       </c>
@@ -33784,7 +33844,7 @@
         <v>-1.8964228261324385E-3</v>
       </c>
     </row>
-    <row r="21" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A21" s="139" t="s">
         <v>28</v>
       </c>
@@ -33824,7 +33884,7 @@
         <v>-1.6027230326546356E-6</v>
       </c>
     </row>
-    <row r="22" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A22" s="57" t="s">
         <v>71</v>
       </c>
@@ -33864,7 +33924,7 @@
         <v>7.9439062617902049E-4</v>
       </c>
     </row>
-    <row r="23" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A23" s="22" t="s">
         <v>72</v>
       </c>
@@ -33904,7 +33964,7 @@
         <v>3.1474946120986233E-3</v>
       </c>
     </row>
-    <row r="24" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A24" s="124" t="s">
         <v>41</v>
       </c>
@@ -33944,7 +34004,7 @@
         <v>3.5392455522788207E-3</v>
       </c>
     </row>
-    <row r="25" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A25" s="148" t="s">
         <v>42</v>
       </c>
@@ -33984,7 +34044,7 @@
         <v>2.1982702913497338E-3</v>
       </c>
     </row>
-    <row r="26" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A26" s="57" t="s">
         <v>48</v>
       </c>
@@ -34024,7 +34084,7 @@
         <v>3.9499744289269913E-3</v>
       </c>
     </row>
-    <row r="27" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A27" s="127" t="s">
         <v>53</v>
       </c>
@@ -34064,7 +34124,7 @@
         <v>1.2083477356246732E-3</v>
       </c>
     </row>
-    <row r="28" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A28" s="124" t="s">
         <v>46</v>
       </c>
@@ -34104,7 +34164,7 @@
         <v>2.3639572792721517E-3</v>
       </c>
     </row>
-    <row r="29" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A29" s="148" t="s">
         <v>47</v>
       </c>
@@ -34144,7 +34204,7 @@
         <v>6.526587407184186E-3</v>
       </c>
     </row>
-    <row r="30" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A30" s="57" t="s">
         <v>49</v>
       </c>
@@ -34184,7 +34244,7 @@
         <v>2.6479190306808779E-3</v>
       </c>
     </row>
-    <row r="31" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A31" s="124" t="s">
         <v>50</v>
       </c>
@@ -34224,7 +34284,7 @@
         <v>3.6101488052774963E-3</v>
       </c>
     </row>
-    <row r="32" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A32" s="148" t="s">
         <v>81</v>
       </c>
@@ -34264,7 +34324,7 @@
         <v>1.4840236413115042E-3</v>
       </c>
     </row>
-    <row r="33" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A33" s="57" t="s">
         <v>51</v>
       </c>
@@ -34304,7 +34364,7 @@
         <v>2.5049740815024095E-3</v>
       </c>
     </row>
-    <row r="34" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A34" s="124" t="s">
         <v>52</v>
       </c>
@@ -34344,7 +34404,7 @@
         <v>2.2584131632020919E-3</v>
       </c>
     </row>
-    <row r="35" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A35" s="156" t="s">
         <v>69</v>
       </c>
@@ -34386,26 +34446,27 @@
       <c r="M35" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="N35" s="31" t="s">
+      <c r="N35" s="31"/>
+      <c r="O35" s="31" t="s">
         <v>73</v>
       </c>
-      <c r="O35" s="31" t="s">
+      <c r="P35" s="31" t="s">
         <v>74</v>
       </c>
-      <c r="P35" s="20" t="s">
+      <c r="Q35" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="Q35" s="1" t="s">
+      <c r="R35" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="R35" s="1" t="s">
+      <c r="S35" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="S35" s="1" t="s">
+      <c r="T35" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="36" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A36" s="148" t="s">
         <v>70</v>
       </c>
@@ -34447,26 +34508,27 @@
       <c r="M36" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="N36" s="34">
+      <c r="N36" s="9"/>
+      <c r="O36" s="34">
         <v>44406</v>
       </c>
-      <c r="O36" s="49">
+      <c r="P36" s="49">
         <v>1.4275283509600518E-2</v>
       </c>
-      <c r="P36" s="10">
+      <c r="Q36" s="10">
         <v>2.7694050008625005E-2</v>
       </c>
-      <c r="Q36" s="11">
+      <c r="R36" s="11">
         <v>1.4275283509600518</v>
       </c>
-      <c r="R36" s="12">
+      <c r="S36" s="12">
         <v>2.339895698925E-2</v>
       </c>
-      <c r="S36" s="11">
+      <c r="T36" s="11">
         <v>1.2061318035695876</v>
       </c>
     </row>
-    <row r="37" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A37" s="39" t="s">
         <v>30</v>
       </c>
@@ -34508,26 +34570,27 @@
       <c r="M37" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="N37" s="34">
+      <c r="N37" s="9"/>
+      <c r="O37" s="34">
         <v>44413</v>
       </c>
-      <c r="O37" s="49">
+      <c r="P37" s="49">
         <v>4.1672818488478154E-2</v>
       </c>
-      <c r="P37" s="10">
+      <c r="Q37" s="10">
         <v>8.6804480911500004E-2</v>
       </c>
-      <c r="Q37" s="11">
+      <c r="R37" s="11">
         <v>4.1672818488478152</v>
       </c>
-      <c r="R37" s="12">
+      <c r="S37" s="12">
         <v>2.7688022377E-2</v>
       </c>
-      <c r="S37" s="11">
+      <c r="T37" s="11">
         <v>1.3292377521363417</v>
       </c>
     </row>
-    <row r="38" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A38" s="22" t="s">
         <v>33</v>
       </c>
@@ -34569,26 +34632,27 @@
       <c r="M38" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="N38" s="34">
+      <c r="N38" s="9"/>
+      <c r="O38" s="34">
         <v>44421</v>
       </c>
-      <c r="O38" s="49">
+      <c r="P38" s="49">
         <v>3.8214387509899805E-2</v>
       </c>
-      <c r="P38" s="10">
+      <c r="Q38" s="10">
         <v>8.0097356220749996E-2</v>
       </c>
-      <c r="Q38" s="11">
+      <c r="R38" s="11">
         <v>3.8214387509899805</v>
       </c>
-      <c r="R38" s="12">
+      <c r="S38" s="12">
         <v>5.418942266125E-3</v>
       </c>
-      <c r="S38" s="11">
+      <c r="T38" s="11">
         <v>0.25853732185710876</v>
       </c>
     </row>
-    <row r="39" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A39" s="127" t="s">
         <v>31</v>
       </c>
@@ -34630,26 +34694,27 @@
       <c r="M39" s="50" t="s">
         <v>30</v>
       </c>
-      <c r="N39" s="34">
+      <c r="N39" s="50"/>
+      <c r="O39" s="34">
         <v>45004</v>
       </c>
-      <c r="O39" s="49">
+      <c r="P39" s="49">
         <v>2.1624750611575927E-2</v>
       </c>
-      <c r="P39" s="47">
+      <c r="Q39" s="47">
         <v>4.3292750724375002E-2</v>
       </c>
-      <c r="Q39" s="48">
+      <c r="R39" s="48">
         <v>2.1624750611575925</v>
       </c>
-      <c r="R39" s="49">
+      <c r="S39" s="49">
         <v>6.2592099693750004E-3</v>
       </c>
-      <c r="S39" s="48">
+      <c r="T39" s="48">
         <v>0.31264785061813194</v>
       </c>
     </row>
-    <row r="40" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A40" s="124" t="s">
         <v>32</v>
       </c>
@@ -34691,26 +34756,27 @@
       <c r="M40" s="50" t="s">
         <v>35</v>
       </c>
-      <c r="N40" s="34">
+      <c r="N40" s="50"/>
+      <c r="O40" s="34">
         <v>45045</v>
       </c>
-      <c r="O40" s="49">
+      <c r="P40" s="49">
         <v>4.8117931554435479E-2</v>
       </c>
-      <c r="P40" s="47">
+      <c r="Q40" s="47">
         <v>9.5465976203999992E-2</v>
       </c>
-      <c r="Q40" s="48">
+      <c r="R40" s="48">
         <v>4.8117931554435476</v>
       </c>
-      <c r="R40" s="49">
+      <c r="S40" s="49">
         <v>8.6655646387499997E-3</v>
       </c>
-      <c r="S40" s="48">
+      <c r="T40" s="48">
         <v>0.43677241122731852</v>
       </c>
     </row>
-    <row r="41" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A41" s="148" t="s">
         <v>34</v>
       </c>
@@ -34752,26 +34818,27 @@
       <c r="M41" s="50" t="s">
         <v>54</v>
       </c>
-      <c r="N41" s="34">
+      <c r="N41" s="50"/>
+      <c r="O41" s="34">
         <v>45100</v>
       </c>
-      <c r="O41" s="49">
+      <c r="P41" s="49">
         <v>3.7411501977499997E-2</v>
       </c>
-      <c r="P41" s="47">
+      <c r="Q41" s="47">
         <v>6.5470128460624999E-2</v>
       </c>
-      <c r="Q41" s="48">
+      <c r="R41" s="48">
         <v>3.7411501977499997</v>
       </c>
-      <c r="R41" s="49">
+      <c r="S41" s="49">
         <v>3.6854199580781252E-3</v>
       </c>
-      <c r="S41" s="48">
+      <c r="T41" s="48">
         <v>0.21059542617589286</v>
       </c>
     </row>
-    <row r="42" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A42" s="39" t="s">
         <v>35</v>
       </c>
@@ -34813,26 +34880,27 @@
       <c r="M42" s="50" t="s">
         <v>63</v>
       </c>
-      <c r="N42" s="34">
+      <c r="N42" s="50"/>
+      <c r="O42" s="34">
         <v>45120</v>
       </c>
-      <c r="O42" s="49">
+      <c r="P42" s="49">
         <v>1.4162913918015331E-2</v>
       </c>
-      <c r="P42" s="47">
+      <c r="Q42" s="47">
         <v>3.3254521879499996E-2</v>
       </c>
-      <c r="Q42" s="48">
+      <c r="R42" s="48">
         <v>1.4162913918015332</v>
       </c>
-      <c r="R42" s="49">
+      <c r="S42" s="49">
         <v>1.3559283408750001E-2</v>
       </c>
-      <c r="S42" s="48">
+      <c r="T42" s="48">
         <v>0.57748225761286209</v>
       </c>
     </row>
-    <row r="43" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A43" s="21" t="s">
         <v>36</v>
       </c>
@@ -34874,26 +34942,27 @@
       <c r="M43" s="50" t="s">
         <v>60</v>
       </c>
-      <c r="N43" s="34">
+      <c r="N43" s="50"/>
+      <c r="O43" s="34">
         <v>45134</v>
       </c>
-      <c r="O43" s="49">
+      <c r="P43" s="49">
         <v>3.4453948702562319E-2</v>
       </c>
-      <c r="P43" s="47">
+      <c r="Q43" s="47">
         <v>7.4627252889749987E-2</v>
       </c>
-      <c r="Q43" s="48">
+      <c r="R43" s="48">
         <v>3.4453948702562318</v>
       </c>
-      <c r="R43" s="49">
+      <c r="S43" s="49">
         <v>7.8202946596874993E-3</v>
       </c>
-      <c r="S43" s="48">
+      <c r="T43" s="48">
         <v>0.36104776822195289</v>
       </c>
     </row>
-    <row r="44" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A44" s="22" t="s">
         <v>37</v>
       </c>
@@ -34935,26 +35004,27 @@
       <c r="M44" s="50" t="s">
         <v>76</v>
       </c>
-      <c r="N44" s="34">
+      <c r="N44" s="50"/>
+      <c r="O44" s="34">
         <v>45146</v>
       </c>
-      <c r="O44" s="49">
+      <c r="P44" s="49">
         <v>4.8123480487998367E-2</v>
       </c>
-      <c r="P44" s="47">
+      <c r="Q44" s="47">
         <v>0.1182875150395</v>
       </c>
-      <c r="Q44" s="48">
+      <c r="R44" s="48">
         <v>4.8123480487998371</v>
       </c>
-      <c r="R44" s="49">
+      <c r="S44" s="49">
         <v>5.08671067303125E-3</v>
       </c>
-      <c r="S44" s="48">
+      <c r="T44" s="48">
         <v>0.20694510467987184</v>
       </c>
     </row>
-    <row r="45" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A45" s="127" t="s">
         <v>38</v>
       </c>
@@ -34996,26 +35066,27 @@
       <c r="M45" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="N45" s="31" t="s">
+      <c r="N45" s="31"/>
+      <c r="O45" s="31" t="s">
         <v>73</v>
       </c>
-      <c r="O45" s="31" t="s">
+      <c r="P45" s="31" t="s">
         <v>74</v>
       </c>
-      <c r="P45" s="20" t="s">
+      <c r="Q45" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="Q45" s="1" t="s">
+      <c r="R45" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="R45" s="1" t="s">
+      <c r="S45" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="S45" s="1" t="s">
+      <c r="T45" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="46" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A46" s="124" t="s">
         <v>39</v>
       </c>
@@ -35057,26 +35128,27 @@
       <c r="M46" s="71" t="s">
         <v>13</v>
       </c>
-      <c r="N46" s="35">
+      <c r="N46" s="71"/>
+      <c r="O46" s="35">
         <v>44406</v>
       </c>
-      <c r="O46" s="18">
+      <c r="P46" s="18">
         <v>3.9289218981435024E-2</v>
       </c>
-      <c r="P46" s="54">
+      <c r="Q46" s="54">
         <v>7.830341343000001E-2</v>
       </c>
-      <c r="Q46" s="55">
+      <c r="R46" s="55">
         <v>3.9289218981435026</v>
       </c>
-      <c r="R46" s="56">
+      <c r="S46" s="56">
         <v>1.9311120193750073E-4</v>
       </c>
-      <c r="S46" s="55">
+      <c r="T46" s="55">
         <v>9.6894732532614505E-3</v>
       </c>
     </row>
-    <row r="47" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A47" s="148" t="s">
         <v>40</v>
       </c>
@@ -35118,26 +35190,27 @@
       <c r="M47" s="71" t="s">
         <v>18</v>
       </c>
-      <c r="N47" s="35">
+      <c r="N47" s="71"/>
+      <c r="O47" s="35">
         <v>44413</v>
       </c>
-      <c r="O47" s="18">
+      <c r="P47" s="18">
         <v>3.0706717222428074E-2</v>
       </c>
-      <c r="P47" s="54">
+      <c r="Q47" s="54">
         <v>7.044120930825E-2</v>
       </c>
-      <c r="Q47" s="55">
+      <c r="R47" s="55">
         <v>3.0706717222428073</v>
       </c>
-      <c r="R47" s="56">
+      <c r="S47" s="56">
         <v>2.3787672355250006E-2</v>
       </c>
-      <c r="S47" s="55">
+      <c r="T47" s="55">
         <v>1.0369517155732346</v>
       </c>
     </row>
-    <row r="48" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A48" s="39" t="s">
         <v>54</v>
       </c>
@@ -35179,26 +35252,27 @@
       <c r="M48" s="71" t="s">
         <v>26</v>
       </c>
-      <c r="N48" s="35">
+      <c r="N48" s="71"/>
+      <c r="O48" s="35">
         <v>44421</v>
       </c>
-      <c r="O48" s="18">
+      <c r="P48" s="18">
         <v>2.4355743821808513E-2</v>
       </c>
-      <c r="P48" s="54">
+      <c r="Q48" s="54">
         <v>4.5788798385000003E-2</v>
       </c>
-      <c r="Q48" s="55">
+      <c r="R48" s="55">
         <v>2.4355743821808513</v>
       </c>
-      <c r="R48" s="56">
+      <c r="S48" s="56">
         <v>3.1962247898437504E-3</v>
       </c>
-      <c r="S48" s="55">
+      <c r="T48" s="55">
         <v>0.17001195690658247</v>
       </c>
     </row>
-    <row r="49" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A49" s="21" t="s">
         <v>55</v>
       </c>
@@ -35240,26 +35314,27 @@
       <c r="M49" s="13" t="s">
         <v>71</v>
       </c>
-      <c r="N49" s="35">
+      <c r="N49" s="13"/>
+      <c r="O49" s="35">
         <v>44754</v>
       </c>
-      <c r="O49" s="18">
+      <c r="P49" s="18">
         <v>1.2947988089113313E-2</v>
       </c>
-      <c r="P49" s="16">
+      <c r="Q49" s="16">
         <v>2.5481640559374998E-2</v>
       </c>
-      <c r="Q49" s="17">
+      <c r="R49" s="17">
         <v>1.2947988089113314</v>
       </c>
-      <c r="R49" s="18">
+      <c r="S49" s="18">
         <v>1.5633607523203124E-3</v>
       </c>
-      <c r="S49" s="17">
+      <c r="T49" s="17">
         <v>7.9439062617902054E-2</v>
       </c>
     </row>
-    <row r="50" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A50" s="22" t="s">
         <v>56</v>
       </c>
@@ -35301,26 +35376,27 @@
       <c r="M50" s="13" t="s">
         <v>48</v>
       </c>
-      <c r="N50" s="35">
+      <c r="N50" s="13"/>
+      <c r="O50" s="35">
         <v>44777</v>
       </c>
-      <c r="O50" s="18">
+      <c r="P50" s="18">
         <v>3.9185770295907078E-2</v>
       </c>
-      <c r="P50" s="16">
+      <c r="Q50" s="16">
         <v>7.0847872694999994E-2</v>
       </c>
-      <c r="Q50" s="17">
+      <c r="R50" s="17">
         <v>3.9185770295907076</v>
       </c>
-      <c r="R50" s="18">
+      <c r="S50" s="18">
         <v>7.1415537675000003E-3</v>
       </c>
-      <c r="S50" s="17">
+      <c r="T50" s="17">
         <v>0.39499744289269911</v>
       </c>
     </row>
-    <row r="51" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A51" s="127" t="s">
         <v>57</v>
       </c>
@@ -35362,26 +35438,27 @@
       <c r="M51" s="13" t="s">
         <v>49</v>
       </c>
-      <c r="N51" s="35">
+      <c r="N51" s="13"/>
+      <c r="O51" s="35">
         <v>44783</v>
       </c>
-      <c r="O51" s="18">
+      <c r="P51" s="18">
         <v>1.0290745463990066E-2</v>
       </c>
-      <c r="P51" s="16">
+      <c r="Q51" s="16">
         <v>1.8646830780749999E-2</v>
       </c>
-      <c r="Q51" s="17">
+      <c r="R51" s="17">
         <v>1.0290745463990065</v>
       </c>
-      <c r="R51" s="18">
+      <c r="S51" s="18">
         <v>4.7980292835937506E-3</v>
       </c>
-      <c r="S51" s="17">
+      <c r="T51" s="17">
         <v>0.26479190306808781</v>
       </c>
     </row>
-    <row r="52" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A52" s="124" t="s">
         <v>58</v>
       </c>
@@ -35423,26 +35500,27 @@
       <c r="M52" s="13" t="s">
         <v>51</v>
       </c>
-      <c r="N52" s="35">
+      <c r="N52" s="13"/>
+      <c r="O52" s="35">
         <v>44796</v>
       </c>
-      <c r="O52" s="18">
+      <c r="P52" s="18">
         <v>1.8901883746156495E-2</v>
       </c>
-      <c r="P52" s="16">
+      <c r="Q52" s="16">
         <v>4.1187204682874998E-2</v>
       </c>
-      <c r="Q52" s="17">
+      <c r="R52" s="17">
         <v>1.8901883746156496</v>
       </c>
-      <c r="R52" s="18">
+      <c r="S52" s="18">
         <v>5.45833852359375E-3</v>
       </c>
-      <c r="S52" s="17">
+      <c r="T52" s="17">
         <v>0.25049740815024096</v>
       </c>
     </row>
-    <row r="53" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A53" s="148" t="s">
         <v>59</v>
       </c>
@@ -35484,26 +35562,27 @@
       <c r="M53" s="13" t="s">
         <v>36</v>
       </c>
-      <c r="N53" s="35">
+      <c r="N53" s="13"/>
+      <c r="O53" s="35">
         <v>45045</v>
       </c>
-      <c r="O53" s="18">
+      <c r="P53" s="18">
         <v>5.7839505209629632E-2</v>
       </c>
-      <c r="P53" s="16">
+      <c r="Q53" s="16">
         <v>0.1171249980495</v>
       </c>
-      <c r="Q53" s="17">
+      <c r="R53" s="17">
         <v>5.7839505209629634</v>
       </c>
-      <c r="R53" s="18">
+      <c r="S53" s="18">
         <v>9.4235928253125004E-3</v>
       </c>
-      <c r="S53" s="17">
+      <c r="T53" s="17">
         <v>0.46536260865740742</v>
       </c>
     </row>
-    <row r="54" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A54" s="39" t="s">
         <v>63</v>
       </c>
@@ -35545,26 +35624,27 @@
       <c r="M54" s="13" t="s">
         <v>55</v>
       </c>
-      <c r="N54" s="35">
+      <c r="N54" s="13"/>
+      <c r="O54" s="35">
         <v>45100</v>
       </c>
-      <c r="O54" s="18">
+      <c r="P54" s="18">
         <v>3.4015607951991461E-2</v>
       </c>
-      <c r="P54" s="16">
+      <c r="Q54" s="16">
         <v>7.1738917170749997E-2</v>
       </c>
-      <c r="Q54" s="17">
+      <c r="R54" s="17">
         <v>3.401560795199146</v>
       </c>
-      <c r="R54" s="18">
+      <c r="S54" s="18">
         <v>4.1068464931406246E-3</v>
       </c>
-      <c r="S54" s="17">
+      <c r="T54" s="17">
         <v>0.19472956344905759</v>
       </c>
     </row>
-    <row r="55" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A55" s="21" t="s">
         <v>64</v>
       </c>
@@ -35606,26 +35686,27 @@
       <c r="M55" s="13" t="s">
         <v>64</v>
       </c>
-      <c r="N55" s="35">
+      <c r="N55" s="13"/>
+      <c r="O55" s="35">
         <v>45120</v>
       </c>
-      <c r="O55" s="18">
+      <c r="P55" s="18">
         <v>1.6366473070102194E-2</v>
       </c>
-      <c r="P55" s="16">
+      <c r="Q55" s="16">
         <v>3.2831144978625E-2</v>
       </c>
-      <c r="Q55" s="17">
+      <c r="R55" s="17">
         <v>1.6366473070102194</v>
       </c>
-      <c r="R55" s="18">
+      <c r="S55" s="18">
         <v>1.3054441025625E-2</v>
       </c>
-      <c r="S55" s="17">
+      <c r="T55" s="17">
         <v>0.65076974205508487</v>
       </c>
     </row>
-    <row r="56" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A56" s="22" t="s">
         <v>65</v>
       </c>
@@ -35667,26 +35748,27 @@
       <c r="M56" s="13" t="s">
         <v>61</v>
       </c>
-      <c r="N56" s="35">
+      <c r="N56" s="13"/>
+      <c r="O56" s="35">
         <v>45134</v>
       </c>
-      <c r="O56" s="18">
+      <c r="P56" s="18">
         <v>6.3932943295208655E-2</v>
       </c>
-      <c r="P56" s="16">
+      <c r="Q56" s="16">
         <v>0.124093842936</v>
       </c>
-      <c r="Q56" s="17">
+      <c r="R56" s="17">
         <v>6.3932943295208657</v>
       </c>
-      <c r="R56" s="18">
+      <c r="S56" s="18">
         <v>8.646821086875001E-3</v>
       </c>
-      <c r="S56" s="17">
+      <c r="T56" s="17">
         <v>0.44548279685085013</v>
       </c>
     </row>
-    <row r="57" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A57" s="127" t="s">
         <v>66</v>
       </c>
@@ -35728,26 +35810,27 @@
       <c r="M57" s="13" t="s">
         <v>80</v>
       </c>
-      <c r="N57" s="35">
+      <c r="N57" s="13"/>
+      <c r="O57" s="35">
         <v>45146</v>
       </c>
-      <c r="O57" s="18">
+      <c r="P57" s="18">
         <v>5.3229190612098028E-2</v>
       </c>
-      <c r="P57" s="16">
+      <c r="Q57" s="16">
         <v>0.102625879500125</v>
       </c>
-      <c r="Q57" s="17">
+      <c r="R57" s="17">
         <v>5.3229190612098032</v>
       </c>
-      <c r="R57" s="18">
+      <c r="S57" s="18">
         <v>4.3786440464062496E-3</v>
       </c>
-      <c r="S57" s="17">
+      <c r="T57" s="17">
         <v>0.2271080936932702</v>
       </c>
     </row>
-    <row r="58" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A58" s="124" t="s">
         <v>67</v>
       </c>
@@ -35789,26 +35872,27 @@
       <c r="M58" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="N58" s="31" t="s">
+      <c r="N58" s="31"/>
+      <c r="O58" s="31" t="s">
         <v>73</v>
       </c>
-      <c r="O58" s="31" t="s">
+      <c r="P58" s="31" t="s">
         <v>74</v>
       </c>
-      <c r="P58" s="20" t="s">
+      <c r="Q58" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="Q58" s="1" t="s">
+      <c r="R58" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="R58" s="1" t="s">
+      <c r="S58" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="S58" s="1" t="s">
+      <c r="T58" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="59" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A59" s="148" t="s">
         <v>68</v>
       </c>
@@ -35850,26 +35934,27 @@
       <c r="M59" s="73" t="s">
         <v>10</v>
       </c>
-      <c r="N59" s="37">
+      <c r="N59" s="73"/>
+      <c r="O59" s="37">
         <v>44406</v>
       </c>
-      <c r="O59" s="27">
+      <c r="P59" s="27">
         <v>1.4761361997822069E-2</v>
       </c>
-      <c r="P59" s="68">
+      <c r="Q59" s="68">
         <v>2.7958019623874997E-2</v>
       </c>
-      <c r="Q59" s="69">
+      <c r="R59" s="69">
         <v>1.4761361997822069</v>
       </c>
-      <c r="R59" s="70">
+      <c r="S59" s="70">
         <v>2.1961429373375002E-2</v>
       </c>
-      <c r="S59" s="69">
+      <c r="T59" s="69">
         <v>1.1595263660704858</v>
       </c>
     </row>
-    <row r="60" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A60" s="39" t="s">
         <v>60</v>
       </c>
@@ -35911,26 +35996,27 @@
       <c r="M60" s="73" t="s">
         <v>21</v>
       </c>
-      <c r="N60" s="37">
+      <c r="N60" s="73"/>
+      <c r="O60" s="37">
         <v>44413</v>
       </c>
-      <c r="O60" s="27">
+      <c r="P60" s="27">
         <v>1.5058361144762035E-2</v>
       </c>
-      <c r="P60" s="68">
+      <c r="Q60" s="68">
         <v>2.7526684172625E-2</v>
       </c>
-      <c r="Q60" s="69">
+      <c r="R60" s="69">
         <v>1.5058361144762036</v>
       </c>
-      <c r="R60" s="70">
+      <c r="S60" s="70">
         <v>1.2599044099375015E-3</v>
       </c>
-      <c r="S60" s="69">
+      <c r="T60" s="69">
         <v>6.8922560718681705E-2</v>
       </c>
     </row>
-    <row r="61" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A61" s="21" t="s">
         <v>61</v>
       </c>
@@ -35972,26 +36058,27 @@
       <c r="M61" s="73" t="s">
         <v>27</v>
       </c>
-      <c r="N61" s="37">
+      <c r="N61" s="73"/>
+      <c r="O61" s="37">
         <v>44421</v>
       </c>
-      <c r="O61" s="27">
+      <c r="P61" s="27">
         <v>2.8185368694723621E-2</v>
       </c>
-      <c r="P61" s="68">
+      <c r="Q61" s="68">
         <v>6.7306660443000002E-2</v>
       </c>
-      <c r="Q61" s="69">
+      <c r="R61" s="69">
         <v>2.818536869472362</v>
       </c>
-      <c r="R61" s="70">
+      <c r="S61" s="70">
         <v>4.0108938467499997E-3</v>
       </c>
-      <c r="S61" s="69">
+      <c r="T61" s="69">
         <v>0.16796037884212731</v>
       </c>
     </row>
-    <row r="62" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A62" s="22" t="s">
         <v>43</v>
       </c>
@@ -36033,26 +36120,27 @@
       <c r="M62" s="28" t="s">
         <v>72</v>
       </c>
-      <c r="N62" s="37">
+      <c r="N62" s="28"/>
+      <c r="O62" s="37">
         <v>44754</v>
       </c>
-      <c r="O62" s="27">
+      <c r="P62" s="27">
         <v>2.1222551780676606E-2</v>
       </c>
-      <c r="P62" s="25">
+      <c r="Q62" s="25">
         <v>4.6265162881875002E-2</v>
       </c>
-      <c r="Q62" s="26">
+      <c r="R62" s="26">
         <v>2.1222551780676606</v>
       </c>
-      <c r="R62" s="27">
+      <c r="S62" s="27">
         <v>6.8615382543749997E-3</v>
       </c>
-      <c r="S62" s="26">
+      <c r="T62" s="26">
         <v>0.31474946120986236</v>
       </c>
     </row>
-    <row r="63" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A63" s="127" t="s">
         <v>62</v>
       </c>
@@ -36094,26 +36182,27 @@
       <c r="M63" s="28" t="s">
         <v>33</v>
       </c>
-      <c r="N63" s="37">
+      <c r="N63" s="28"/>
+      <c r="O63" s="37">
         <v>45004</v>
       </c>
-      <c r="O63" s="27">
+      <c r="P63" s="27">
         <v>2.7976898447768763E-2</v>
       </c>
-      <c r="P63" s="25">
+      <c r="Q63" s="25">
         <v>5.5170443739E-2</v>
       </c>
-      <c r="Q63" s="26">
+      <c r="R63" s="26">
         <v>2.7976898447768761</v>
       </c>
-      <c r="R63" s="27">
+      <c r="S63" s="27">
         <v>1.4501068387500001E-2</v>
       </c>
-      <c r="S63" s="26">
+      <c r="T63" s="26">
         <v>0.7353482955121704</v>
       </c>
     </row>
-    <row r="64" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A64" s="124" t="s">
         <v>44</v>
       </c>
@@ -36155,26 +36244,27 @@
       <c r="M64" s="28" t="s">
         <v>37</v>
       </c>
-      <c r="N64" s="37">
+      <c r="N64" s="28"/>
+      <c r="O64" s="37">
         <v>45045</v>
       </c>
-      <c r="O64" s="27">
+      <c r="P64" s="27">
         <v>3.8450563674918829E-2</v>
       </c>
-      <c r="P64" s="25">
+      <c r="Q64" s="25">
         <v>7.1056641671250004E-2</v>
       </c>
-      <c r="Q64" s="26">
+      <c r="R64" s="26">
         <v>3.8450563674918827</v>
       </c>
-      <c r="R64" s="27">
+      <c r="S64" s="27">
         <v>9.1419326221874996E-3</v>
       </c>
-      <c r="S64" s="26">
+      <c r="T64" s="26">
         <v>0.49469332371144475</v>
       </c>
     </row>
-    <row r="65" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A65" s="148" t="s">
         <v>45</v>
       </c>
@@ -36216,26 +36306,27 @@
       <c r="M65" s="28" t="s">
         <v>56</v>
       </c>
-      <c r="N65" s="37">
+      <c r="N65" s="28"/>
+      <c r="O65" s="37">
         <v>45100</v>
       </c>
-      <c r="O65" s="27">
+      <c r="P65" s="27">
         <v>1.7886653884458457E-2</v>
       </c>
-      <c r="P65" s="25">
+      <c r="Q65" s="25">
         <v>4.2194616513437498E-2</v>
       </c>
-      <c r="Q65" s="26">
+      <c r="R65" s="26">
         <v>1.7886653884458457</v>
       </c>
-      <c r="R65" s="27">
+      <c r="S65" s="27">
         <v>8.2568382809062486E-3</v>
       </c>
-      <c r="S65" s="26">
+      <c r="T65" s="26">
         <v>0.35001434001298215</v>
       </c>
     </row>
-    <row r="66" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A66" s="39" t="s">
         <v>76</v>
       </c>
@@ -36277,26 +36368,27 @@
       <c r="M66" s="28" t="s">
         <v>65</v>
       </c>
-      <c r="N66" s="37">
+      <c r="N66" s="28"/>
+      <c r="O66" s="37">
         <v>45120</v>
       </c>
-      <c r="O66" s="27">
+      <c r="P66" s="27">
         <v>1.6280268144578312E-2</v>
       </c>
-      <c r="P66" s="25">
+      <c r="Q66" s="25">
         <v>3.2430294143999998E-2</v>
       </c>
-      <c r="Q66" s="26">
+      <c r="R66" s="26">
         <v>1.6280268144578312</v>
       </c>
-      <c r="R66" s="27">
+      <c r="S66" s="27">
         <v>1.3134819616875E-2</v>
       </c>
-      <c r="S66" s="26">
+      <c r="T66" s="26">
         <v>0.65937849482304212</v>
       </c>
     </row>
-    <row r="67" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A67" s="21" t="s">
         <v>80</v>
       </c>
@@ -36338,26 +36430,27 @@
       <c r="M67" s="28" t="s">
         <v>43</v>
       </c>
-      <c r="N67" s="37">
+      <c r="N67" s="28"/>
+      <c r="O67" s="37">
         <v>45134</v>
       </c>
-      <c r="O67" s="27">
+      <c r="P67" s="27">
         <v>1.9121543922762271E-2</v>
       </c>
-      <c r="P67" s="25">
+      <c r="Q67" s="25">
         <v>3.9734568271499994E-2</v>
       </c>
-      <c r="Q67" s="26">
+      <c r="R67" s="26">
         <v>1.912154392276227</v>
       </c>
-      <c r="R67" s="27">
+      <c r="S67" s="27">
         <v>6.7338353981250005E-3</v>
       </c>
-      <c r="S67" s="26">
+      <c r="T67" s="26">
         <v>0.32405367652189609</v>
       </c>
     </row>
-    <row r="68" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A68" s="22" t="s">
         <v>77</v>
       </c>
@@ -36399,24 +36492,25 @@
       <c r="M68" s="28" t="s">
         <v>77</v>
       </c>
-      <c r="N68" s="37">
+      <c r="N68" s="28"/>
+      <c r="O68" s="37">
         <v>45146</v>
       </c>
-      <c r="O68" s="27">
+      <c r="P68" s="27">
         <v>0.1477072933292011</v>
       </c>
-      <c r="P68" s="25">
+      <c r="Q68" s="25">
         <v>0.32170648487100001</v>
       </c>
-      <c r="Q68" s="26"/>
-      <c r="R68" s="27">
+      <c r="R68" s="26"/>
+      <c r="S68" s="27">
         <v>1.763577148875E-2</v>
       </c>
-      <c r="S68" s="26">
+      <c r="T68" s="26">
         <v>0.80972320884986226</v>
       </c>
     </row>
-    <row r="69" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A69" s="127" t="s">
         <v>78</v>
       </c>
@@ -36456,7 +36550,7 @@
         <v>1.6948198261392141E-3</v>
       </c>
     </row>
-    <row r="70" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A70" s="131" t="s">
         <v>79</v>
       </c>
@@ -36498,827 +36592,863 @@
       <c r="M70" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="N70" s="1" t="s">
+      <c r="N70" s="1"/>
+      <c r="O70" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="O70" s="1" t="s">
+      <c r="P70" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="P70" s="1" t="s">
+      <c r="Q70" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="Q70" s="1" t="s">
+      <c r="R70" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="R70" s="1" t="s">
+      <c r="S70" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="S70" s="1" t="s">
+      <c r="T70" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="71" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:20" x14ac:dyDescent="0.3">
       <c r="M71" s="75" t="s">
         <v>19</v>
       </c>
-      <c r="N71" s="82">
+      <c r="N71" s="75"/>
+      <c r="O71" s="82">
         <v>44413</v>
       </c>
-      <c r="O71" s="83">
+      <c r="P71" s="83">
         <v>3.4816069629649893E-2</v>
       </c>
-      <c r="P71" s="78">
+      <c r="Q71" s="78">
         <v>7.9554719103750005E-2</v>
       </c>
-      <c r="Q71" s="79">
+      <c r="R71" s="79">
         <v>3.4816069629649902</v>
       </c>
-      <c r="R71" s="80">
+      <c r="S71" s="80">
         <v>2.4910599382875001E-2</v>
       </c>
-      <c r="S71" s="79">
+      <c r="T71" s="79">
         <v>1.0901794040645514</v>
       </c>
     </row>
-    <row r="72" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:20" x14ac:dyDescent="0.3">
       <c r="M72" s="84" t="s">
         <v>53</v>
       </c>
-      <c r="N72" s="82">
+      <c r="N72" s="84"/>
+      <c r="O72" s="82">
         <v>44777</v>
       </c>
-      <c r="O72" s="83">
+      <c r="P72" s="83">
         <v>6.4307165637578411E-3</v>
       </c>
-      <c r="P72" s="86">
+      <c r="Q72" s="86">
         <v>1.230196078646875E-2</v>
       </c>
-      <c r="Q72" s="87">
+      <c r="R72" s="87">
         <v>0.64307165637578412</v>
       </c>
-      <c r="R72" s="83">
+      <c r="S72" s="83">
         <v>2.31156921825E-3</v>
       </c>
-      <c r="S72" s="87">
+      <c r="T72" s="87">
         <v>0.12083477356246732</v>
       </c>
     </row>
-    <row r="73" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:20" x14ac:dyDescent="0.3">
       <c r="M73" s="84" t="s">
         <v>31</v>
       </c>
-      <c r="N73" s="82">
+      <c r="N73" s="84"/>
+      <c r="O73" s="82">
         <v>45004</v>
       </c>
-      <c r="O73" s="83">
+      <c r="P73" s="83">
         <v>4.5796617339119383E-2</v>
       </c>
-      <c r="P73" s="86">
+      <c r="Q73" s="86">
         <v>5.4085805077499993E-2</v>
       </c>
-      <c r="Q73" s="87">
+      <c r="R73" s="87">
         <v>4.5796617339119381</v>
       </c>
-      <c r="R73" s="83">
+      <c r="S73" s="83">
         <v>6.8162937900000005E-3</v>
       </c>
-      <c r="S73" s="87">
+      <c r="T73" s="87">
         <v>0.57716289500423379</v>
       </c>
     </row>
-    <row r="74" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:20" x14ac:dyDescent="0.3">
       <c r="M74" s="84" t="s">
         <v>38</v>
       </c>
-      <c r="N74" s="82">
+      <c r="N74" s="84"/>
+      <c r="O74" s="82">
         <v>45045</v>
       </c>
-      <c r="O74" s="83">
+      <c r="P74" s="83">
         <v>4.792294697998508E-2</v>
       </c>
-      <c r="P74" s="86">
+      <c r="Q74" s="86">
         <v>9.6373046376749996E-2</v>
       </c>
-      <c r="Q74" s="87">
+      <c r="R74" s="87">
         <v>4.7922946979985079</v>
       </c>
-      <c r="R74" s="83">
+      <c r="S74" s="83">
         <v>8.4232530806250018E-3</v>
       </c>
-      <c r="S74" s="87">
+      <c r="T74" s="87">
         <v>0.4188589299167082</v>
       </c>
     </row>
-    <row r="75" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:20" x14ac:dyDescent="0.3">
       <c r="M75" s="84" t="s">
         <v>57</v>
       </c>
-      <c r="N75" s="82">
+      <c r="N75" s="84"/>
+      <c r="O75" s="82">
         <v>45100</v>
       </c>
-      <c r="O75" s="83">
+      <c r="P75" s="83">
         <v>4.1712511737339225E-2</v>
       </c>
-      <c r="P75" s="86">
+      <c r="Q75" s="86">
         <v>7.7835546901874997E-2</v>
       </c>
-      <c r="Q75" s="87">
+      <c r="R75" s="87">
         <v>4.1712511737339222</v>
       </c>
-      <c r="R75" s="83">
+      <c r="S75" s="83">
         <v>6.2214054598124999E-3</v>
       </c>
-      <c r="S75" s="87">
+      <c r="T75" s="87">
         <v>0.33340865272307069</v>
       </c>
     </row>
-    <row r="76" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:20" x14ac:dyDescent="0.3">
       <c r="M76" s="84" t="s">
         <v>66</v>
       </c>
-      <c r="N76" s="82">
+      <c r="N76" s="84"/>
+      <c r="O76" s="82">
         <v>45120</v>
       </c>
-      <c r="O76" s="83">
+      <c r="P76" s="83">
         <v>4.8377718971910101E-2</v>
       </c>
-      <c r="P76" s="86">
+      <c r="Q76" s="86">
         <v>0.10333480772399999</v>
       </c>
-      <c r="Q76" s="87">
+      <c r="R76" s="87">
         <v>4.8377718971910104</v>
       </c>
-      <c r="R76" s="83">
+      <c r="S76" s="83">
         <v>8.0501506481250006E-3</v>
       </c>
-      <c r="S76" s="87">
+      <c r="T76" s="87">
         <v>0.37687971199087078</v>
       </c>
     </row>
-    <row r="77" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:20" x14ac:dyDescent="0.3">
       <c r="M77" s="84" t="s">
         <v>62</v>
       </c>
-      <c r="N77" s="82">
+      <c r="N77" s="84"/>
+      <c r="O77" s="82">
         <v>45134</v>
       </c>
-      <c r="O77" s="83">
+      <c r="P77" s="83">
         <v>4.2561740354097384E-2</v>
       </c>
-      <c r="P77" s="86">
+      <c r="Q77" s="86">
         <v>8.9592463445374998E-2</v>
       </c>
-      <c r="Q77" s="87">
+      <c r="R77" s="87">
         <v>4.2561740354097388</v>
       </c>
-      <c r="R77" s="83">
+      <c r="S77" s="83">
         <v>4.0582605854531254E-3</v>
       </c>
-      <c r="S77" s="87">
+      <c r="T77" s="87">
         <v>0.19279147674361641</v>
       </c>
     </row>
-    <row r="78" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:20" x14ac:dyDescent="0.3">
       <c r="M78" s="84" t="s">
         <v>78</v>
       </c>
-      <c r="N78" s="82">
+      <c r="N78" s="84"/>
+      <c r="O78" s="82">
         <v>45146</v>
       </c>
-      <c r="O78" s="83">
+      <c r="P78" s="83">
         <v>3.1173460359890111E-2</v>
       </c>
-      <c r="P78" s="86">
+      <c r="Q78" s="86">
         <v>6.5246052533249999E-2</v>
       </c>
-      <c r="Q78" s="87">
+      <c r="R78" s="87">
         <v>3.1173460359890113</v>
       </c>
-      <c r="R78" s="83">
+      <c r="S78" s="83">
         <v>3.5472578961093749E-3</v>
       </c>
-      <c r="S78" s="87">
+      <c r="T78" s="87">
         <v>0.16948198261392142</v>
       </c>
     </row>
-    <row r="79" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:20" x14ac:dyDescent="0.3">
       <c r="M79" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="N79" s="1" t="s">
+      <c r="N79" s="1"/>
+      <c r="O79" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="O79" s="1" t="s">
+      <c r="P79" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="P79" s="1" t="s">
+      <c r="Q79" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="Q79" s="1" t="s">
+      <c r="R79" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="R79" s="1" t="s">
+      <c r="S79" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="S79" s="1" t="s">
+      <c r="T79" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="80" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:20" x14ac:dyDescent="0.3">
       <c r="M80" s="90" t="s">
         <v>12</v>
       </c>
-      <c r="N80" s="97">
+      <c r="N80" s="90"/>
+      <c r="O80" s="97">
         <v>44406</v>
       </c>
-      <c r="O80" s="98">
+      <c r="P80" s="98">
         <v>2.8522095944787992E-2</v>
       </c>
-      <c r="P80" s="93">
+      <c r="Q80" s="93">
         <v>3.2287012609500003E-2</v>
       </c>
-      <c r="Q80" s="94">
+      <c r="R80" s="94">
         <v>2.8522095944787993</v>
       </c>
-      <c r="R80" s="95">
+      <c r="S80" s="95">
         <v>1.9758253396875008E-3</v>
       </c>
-      <c r="S80" s="94">
+      <c r="T80" s="94">
         <v>0.17454287453069797</v>
       </c>
     </row>
-    <row r="81" spans="13:19" x14ac:dyDescent="0.3">
+    <row r="81" spans="13:20" x14ac:dyDescent="0.3">
       <c r="M81" s="90" t="s">
         <v>23</v>
       </c>
-      <c r="N81" s="97">
+      <c r="N81" s="90"/>
+      <c r="O81" s="97">
         <v>44413</v>
       </c>
-      <c r="O81" s="98">
+      <c r="P81" s="98">
         <v>1.4504291018941295E-2</v>
       </c>
-      <c r="P81" s="93">
+      <c r="Q81" s="93">
         <v>2.8907052000750003E-2</v>
       </c>
-      <c r="Q81" s="94">
+      <c r="R81" s="94">
         <v>1.4504291018941295</v>
       </c>
-      <c r="R81" s="95">
+      <c r="S81" s="95">
         <v>1.8592905670312514E-3</v>
       </c>
-      <c r="S81" s="94">
+      <c r="T81" s="94">
         <v>9.3291047016118983E-2</v>
       </c>
     </row>
-    <row r="82" spans="13:19" x14ac:dyDescent="0.3">
+    <row r="82" spans="13:20" x14ac:dyDescent="0.3">
       <c r="M82" s="90" t="s">
         <v>29</v>
       </c>
-      <c r="N82" s="97">
+      <c r="N82" s="90"/>
+      <c r="O82" s="97">
         <v>44421</v>
       </c>
-      <c r="O82" s="98">
+      <c r="P82" s="98">
         <v>2.2718415220178003E-2</v>
       </c>
-      <c r="P82" s="93">
+      <c r="Q82" s="93">
         <v>4.2756057444375002E-2</v>
       </c>
-      <c r="Q82" s="94">
+      <c r="R82" s="94">
         <v>2.2718415220178003</v>
       </c>
-      <c r="R82" s="95">
+      <c r="S82" s="95">
         <v>-3.5690677587812492E-3</v>
       </c>
-      <c r="S82" s="94">
+      <c r="T82" s="94">
         <v>-0.18964228261324384</v>
       </c>
     </row>
-    <row r="83" spans="13:19" x14ac:dyDescent="0.3">
+    <row r="83" spans="13:20" x14ac:dyDescent="0.3">
       <c r="M83" s="99" t="s">
         <v>41</v>
       </c>
-      <c r="N83" s="97">
+      <c r="N83" s="99"/>
+      <c r="O83" s="97">
         <v>44754</v>
       </c>
-      <c r="O83" s="98">
+      <c r="P83" s="98">
         <v>2.7760354085790886E-2</v>
       </c>
-      <c r="P83" s="102">
+      <c r="Q83" s="102">
         <v>5.1773060369999999E-2</v>
       </c>
-      <c r="Q83" s="103">
+      <c r="R83" s="103">
         <v>2.7760354085790886</v>
       </c>
-      <c r="R83" s="98">
+      <c r="S83" s="98">
         <v>6.6006929550000001E-3</v>
       </c>
-      <c r="S83" s="103">
+      <c r="T83" s="103">
         <v>0.35392455522788208</v>
       </c>
     </row>
-    <row r="84" spans="13:19" x14ac:dyDescent="0.3">
+    <row r="84" spans="13:20" x14ac:dyDescent="0.3">
       <c r="M84" s="99" t="s">
         <v>46</v>
       </c>
-      <c r="N84" s="97">
+      <c r="N84" s="99"/>
+      <c r="O84" s="97">
         <v>44777</v>
       </c>
-      <c r="O84" s="98">
+      <c r="P84" s="98">
         <v>1.8748977215822783E-2</v>
       </c>
-      <c r="P84" s="102">
+      <c r="Q84" s="102">
         <v>4.4435076001499998E-2</v>
       </c>
-      <c r="Q84" s="103">
+      <c r="R84" s="103">
         <v>1.8748977215822784</v>
       </c>
-      <c r="R84" s="98">
+      <c r="S84" s="98">
         <v>5.6025787518750002E-3</v>
       </c>
-      <c r="S84" s="103">
+      <c r="T84" s="103">
         <v>0.23639572792721517</v>
       </c>
     </row>
-    <row r="85" spans="13:19" x14ac:dyDescent="0.3">
+    <row r="85" spans="13:20" x14ac:dyDescent="0.3">
       <c r="M85" s="99" t="s">
         <v>50</v>
       </c>
-      <c r="N85" s="97">
+      <c r="N85" s="99"/>
+      <c r="O85" s="97">
         <v>44783</v>
       </c>
-      <c r="O85" s="98">
+      <c r="P85" s="98">
         <v>3.1779787840978201E-2</v>
       </c>
-      <c r="P85" s="102">
+      <c r="Q85" s="102">
         <v>6.2701521410249997E-2</v>
       </c>
-      <c r="Q85" s="103">
+      <c r="R85" s="103">
         <v>3.17797878409782</v>
       </c>
-      <c r="R85" s="98">
+      <c r="S85" s="98">
         <v>7.1228235928125008E-3</v>
       </c>
-      <c r="S85" s="103">
+      <c r="T85" s="103">
         <v>0.3610148805277496</v>
       </c>
     </row>
-    <row r="86" spans="13:19" x14ac:dyDescent="0.3">
+    <row r="86" spans="13:20" x14ac:dyDescent="0.3">
       <c r="M86" s="99" t="s">
         <v>52</v>
       </c>
-      <c r="N86" s="97">
+      <c r="N86" s="99"/>
+      <c r="O86" s="97">
         <v>44796</v>
       </c>
-      <c r="O86" s="98">
+      <c r="P86" s="98">
         <v>1.9971370823819133E-2</v>
       </c>
-      <c r="P86" s="102">
+      <c r="Q86" s="102">
         <v>4.0801510593062494E-2</v>
       </c>
-      <c r="Q86" s="103">
+      <c r="R86" s="103">
         <v>1.9971370823819132</v>
       </c>
-      <c r="R86" s="98">
+      <c r="S86" s="98">
         <v>4.6139380924218746E-3</v>
       </c>
-      <c r="S86" s="103">
+      <c r="T86" s="103">
         <v>0.22584131632020921</v>
       </c>
     </row>
-    <row r="87" spans="13:19" x14ac:dyDescent="0.3">
+    <row r="87" spans="13:20" x14ac:dyDescent="0.3">
       <c r="M87" s="99" t="s">
         <v>32</v>
       </c>
-      <c r="N87" s="97">
+      <c r="N87" s="99"/>
+      <c r="O87" s="97">
         <v>45004</v>
       </c>
-      <c r="O87" s="98">
+      <c r="P87" s="98">
         <v>3.2583484975625902E-2</v>
       </c>
-      <c r="P87" s="102">
+      <c r="Q87" s="102">
         <v>6.7675898294374995E-2</v>
       </c>
-      <c r="Q87" s="103">
+      <c r="R87" s="103">
         <v>3.25834849756259</v>
       </c>
-      <c r="R87" s="98">
+      <c r="S87" s="98">
         <v>3.540156143484375E-3</v>
       </c>
-      <c r="S87" s="103">
+      <c r="T87" s="103">
         <v>0.17044564966222317</v>
       </c>
     </row>
-    <row r="88" spans="13:19" x14ac:dyDescent="0.3">
+    <row r="88" spans="13:20" x14ac:dyDescent="0.3">
       <c r="M88" s="99" t="s">
         <v>39</v>
       </c>
-      <c r="N88" s="97">
+      <c r="N88" s="99"/>
+      <c r="O88" s="97">
         <v>45045</v>
       </c>
-      <c r="O88" s="98">
+      <c r="P88" s="98">
         <v>1.0746867809774435E-2</v>
       </c>
-      <c r="P88" s="102">
+      <c r="Q88" s="102">
         <v>2.1440001280499998E-2</v>
       </c>
-      <c r="Q88" s="103">
+      <c r="R88" s="103">
         <v>1.0746867809774434</v>
       </c>
-      <c r="R88" s="98">
+      <c r="S88" s="98">
         <v>5.5995181921874998E-3</v>
       </c>
-      <c r="S88" s="103">
+      <c r="T88" s="103">
         <v>0.28067760361842103</v>
       </c>
     </row>
-    <row r="89" spans="13:19" x14ac:dyDescent="0.3">
+    <row r="89" spans="13:20" x14ac:dyDescent="0.3">
       <c r="M89" s="99" t="s">
         <v>58</v>
       </c>
-      <c r="N89" s="97">
+      <c r="N89" s="99"/>
+      <c r="O89" s="97">
         <v>45100</v>
       </c>
-      <c r="O89" s="98">
+      <c r="P89" s="98">
         <v>4.8660426133989146E-2</v>
       </c>
-      <c r="P89" s="102">
+      <c r="Q89" s="102">
         <v>0.10758820218224999</v>
       </c>
-      <c r="Q89" s="103">
+      <c r="R89" s="103">
         <v>4.866042613398915</v>
       </c>
-      <c r="R89" s="98">
+      <c r="S89" s="98">
         <v>1.4330423351250001E-2</v>
       </c>
-      <c r="S89" s="103">
+      <c r="T89" s="103">
         <v>0.64814216875848041</v>
       </c>
     </row>
-    <row r="90" spans="13:19" x14ac:dyDescent="0.3">
+    <row r="90" spans="13:20" x14ac:dyDescent="0.3">
       <c r="M90" s="99" t="s">
         <v>67</v>
       </c>
-      <c r="N90" s="97">
+      <c r="N90" s="99"/>
+      <c r="O90" s="97">
         <v>45120</v>
       </c>
-      <c r="O90" s="98">
+      <c r="P90" s="98">
         <v>7.8753014642203526E-3</v>
       </c>
-      <c r="P90" s="102">
+      <c r="Q90" s="102">
         <v>1.6136492700187501E-2</v>
       </c>
-      <c r="Q90" s="103">
+      <c r="R90" s="103">
         <v>0.78753014642203523</v>
       </c>
-      <c r="R90" s="98">
+      <c r="S90" s="98">
         <v>5.5636888035937504E-3</v>
       </c>
-      <c r="S90" s="103">
+      <c r="T90" s="103">
         <v>0.27153190842331631</v>
       </c>
     </row>
-    <row r="91" spans="13:19" x14ac:dyDescent="0.3">
+    <row r="91" spans="13:20" x14ac:dyDescent="0.3">
       <c r="M91" s="99" t="s">
         <v>44</v>
       </c>
-      <c r="N91" s="97">
+      <c r="N91" s="99"/>
+      <c r="O91" s="97">
         <v>45134</v>
       </c>
-      <c r="O91" s="98">
+      <c r="P91" s="98">
         <v>3.8038774552472371E-2</v>
       </c>
-      <c r="P91" s="102">
+      <c r="Q91" s="102">
         <v>7.2311710424249984E-2</v>
       </c>
-      <c r="Q91" s="103">
+      <c r="R91" s="103">
         <v>3.8038774552472372</v>
       </c>
-      <c r="R91" s="98">
+      <c r="S91" s="98">
         <v>7.4870013290625004E-3</v>
       </c>
-      <c r="S91" s="103">
+      <c r="T91" s="103">
         <v>0.39384541446935828</v>
       </c>
     </row>
-    <row r="92" spans="13:19" x14ac:dyDescent="0.3">
+    <row r="92" spans="13:20" x14ac:dyDescent="0.3">
       <c r="M92" s="99" t="s">
         <v>79</v>
       </c>
-      <c r="N92" s="97">
+      <c r="N92" s="99"/>
+      <c r="O92" s="97">
         <v>45146</v>
       </c>
-      <c r="O92" s="98">
+      <c r="P92" s="98">
         <v>3.0115005225647792E-2</v>
       </c>
-      <c r="P92" s="102">
+      <c r="Q92" s="102">
         <v>6.2759670890250002E-2</v>
       </c>
-      <c r="Q92" s="103">
+      <c r="R92" s="103">
         <v>3.0115005225647793</v>
       </c>
-      <c r="R92" s="98">
+      <c r="S92" s="98">
         <v>7.5660358650000009E-3</v>
       </c>
-      <c r="S92" s="103">
+      <c r="T92" s="103">
         <v>0.36305354438579657</v>
       </c>
     </row>
-    <row r="93" spans="13:19" x14ac:dyDescent="0.3">
+    <row r="93" spans="13:20" x14ac:dyDescent="0.3">
       <c r="M93" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="N93" s="1" t="s">
+      <c r="N93" s="1"/>
+      <c r="O93" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="O93" s="1" t="s">
+      <c r="P93" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="P93" s="1" t="s">
+      <c r="Q93" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="Q93" s="1" t="s">
+      <c r="R93" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="R93" s="1" t="s">
+      <c r="S93" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="S93" s="1" t="s">
+      <c r="T93" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="94" spans="13:19" x14ac:dyDescent="0.3">
+    <row r="94" spans="13:20" x14ac:dyDescent="0.3">
       <c r="M94" s="165" t="s">
         <v>14</v>
       </c>
-      <c r="N94" s="162">
+      <c r="N94" s="165"/>
+      <c r="O94" s="162">
         <v>44406</v>
       </c>
-      <c r="O94" s="161">
+      <c r="P94" s="161">
         <v>2.627872287701041E-2</v>
       </c>
-      <c r="P94" s="166">
+      <c r="Q94" s="166">
         <v>5.5553220162000004E-2</v>
       </c>
-      <c r="Q94" s="167">
+      <c r="R94" s="167">
         <v>2.6278722877010408</v>
       </c>
-      <c r="R94" s="168">
+      <c r="S94" s="168">
         <v>3.3154236167500014E-3</v>
       </c>
-      <c r="S94" s="167">
+      <c r="T94" s="167">
         <v>0.15683176995033121</v>
       </c>
     </row>
-    <row r="95" spans="13:19" x14ac:dyDescent="0.3">
+    <row r="95" spans="13:20" x14ac:dyDescent="0.3">
       <c r="M95" s="165" t="s">
         <v>22</v>
       </c>
-      <c r="N95" s="162">
+      <c r="N95" s="165"/>
+      <c r="O95" s="162">
         <v>44413</v>
       </c>
-      <c r="O95" s="161">
+      <c r="P95" s="161">
         <v>2.8779592972922853E-2</v>
       </c>
-      <c r="P95" s="166">
+      <c r="Q95" s="166">
         <v>5.8192336991250003E-2</v>
       </c>
-      <c r="Q95" s="167">
+      <c r="R95" s="167">
         <v>2.8779592972922852</v>
       </c>
-      <c r="R95" s="168">
+      <c r="S95" s="168">
         <v>3.8464701644374995E-3</v>
       </c>
-      <c r="S95" s="167">
+      <c r="T95" s="167">
         <v>0.19023096757851138</v>
       </c>
     </row>
-    <row r="96" spans="13:19" x14ac:dyDescent="0.3">
+    <row r="96" spans="13:20" x14ac:dyDescent="0.3">
       <c r="M96" s="165" t="s">
         <v>28</v>
       </c>
-      <c r="N96" s="162">
+      <c r="N96" s="165"/>
+      <c r="O96" s="162">
         <v>44421</v>
       </c>
-      <c r="O96" s="161">
+      <c r="P96" s="161">
         <v>1.9648530039748393E-2</v>
       </c>
-      <c r="P96" s="166">
+      <c r="Q96" s="166">
         <v>3.6703454114250002E-2</v>
       </c>
-      <c r="Q96" s="167">
+      <c r="R96" s="167">
         <v>1.9648530039748393</v>
       </c>
-      <c r="R96" s="168">
+      <c r="S96" s="168">
         <v>-2.9938866249988594E-6</v>
       </c>
-      <c r="S96" s="167">
+      <c r="T96" s="167">
         <v>-1.6027230326546356E-4</v>
       </c>
     </row>
-    <row r="97" spans="13:19" x14ac:dyDescent="0.3">
+    <row r="97" spans="13:20" x14ac:dyDescent="0.3">
       <c r="M97" s="157" t="s">
         <v>42</v>
       </c>
-      <c r="N97" s="162">
+      <c r="N97" s="157"/>
+      <c r="O97" s="162">
         <v>44754</v>
       </c>
-      <c r="O97" s="161">
+      <c r="P97" s="161">
         <v>4.5967234306436171E-2</v>
       </c>
-      <c r="P97" s="159">
+      <c r="Q97" s="159">
         <v>0.108023000620125</v>
       </c>
-      <c r="Q97" s="160">
+      <c r="R97" s="160">
         <v>4.5967234306436167</v>
       </c>
-      <c r="R97" s="161">
+      <c r="S97" s="161">
         <v>5.165935184671875E-3</v>
       </c>
-      <c r="S97" s="160">
+      <c r="T97" s="160">
         <v>0.21982702913497337</v>
       </c>
     </row>
-    <row r="98" spans="13:19" x14ac:dyDescent="0.3">
+    <row r="98" spans="13:20" x14ac:dyDescent="0.3">
       <c r="M98" s="157" t="s">
         <v>47</v>
       </c>
-      <c r="N98" s="162">
+      <c r="N98" s="157"/>
+      <c r="O98" s="162">
         <v>44777</v>
       </c>
-      <c r="O98" s="161">
+      <c r="P98" s="161">
         <v>2.7707459234450341E-2</v>
       </c>
-      <c r="P98" s="159">
+      <c r="Q98" s="159">
         <v>5.746527045225E-2</v>
       </c>
-      <c r="Q98" s="160">
+      <c r="R98" s="160">
         <v>2.770745923445034</v>
       </c>
-      <c r="R98" s="161">
+      <c r="S98" s="161">
         <v>1.35361422825E-2</v>
       </c>
-      <c r="S98" s="160">
+      <c r="T98" s="160">
         <v>0.65265874071841856</v>
       </c>
     </row>
-    <row r="99" spans="13:19" x14ac:dyDescent="0.3">
+    <row r="99" spans="13:20" x14ac:dyDescent="0.3">
       <c r="M99" s="157" t="s">
         <v>81</v>
       </c>
-      <c r="N99" s="162">
+      <c r="N99" s="157"/>
+      <c r="O99" s="162">
         <v>44783</v>
       </c>
-      <c r="O99" s="161">
+      <c r="P99" s="161">
         <v>2.9518101311857652E-2</v>
       </c>
-      <c r="P99" s="159">
+      <c r="Q99" s="159">
         <v>5.744222515287499E-2</v>
       </c>
-      <c r="Q99" s="160">
+      <c r="R99" s="160">
         <v>2.9518101311857654</v>
       </c>
-      <c r="R99" s="161">
+      <c r="S99" s="161">
         <v>2.8879100059921873E-3</v>
       </c>
-      <c r="S99" s="160">
+      <c r="T99" s="160">
         <v>0.14840236413115043</v>
       </c>
     </row>
-    <row r="100" spans="13:19" x14ac:dyDescent="0.3">
+    <row r="100" spans="13:20" x14ac:dyDescent="0.3">
       <c r="M100" s="157" t="s">
         <v>70</v>
       </c>
-      <c r="N100" s="162">
+      <c r="N100" s="157"/>
+      <c r="O100" s="162">
         <v>44796</v>
       </c>
-      <c r="O100" s="161">
+      <c r="P100" s="161">
         <v>3.7780468660844627E-2</v>
       </c>
-      <c r="P100" s="159">
+      <c r="Q100" s="159">
         <v>7.2462938891499989E-2</v>
       </c>
-      <c r="Q100" s="160">
+      <c r="R100" s="160">
         <v>3.7780468660844626</v>
       </c>
-      <c r="R100" s="161">
+      <c r="S100" s="161">
         <v>5.5426792822031255E-3</v>
       </c>
-      <c r="S100" s="160">
+      <c r="T100" s="160">
         <v>0.28898223577701382</v>
       </c>
     </row>
-    <row r="101" spans="13:19" x14ac:dyDescent="0.3">
+    <row r="101" spans="13:20" x14ac:dyDescent="0.3">
       <c r="M101" s="157" t="s">
         <v>34</v>
       </c>
-      <c r="N101" s="162">
+      <c r="N101" s="157"/>
+      <c r="O101" s="162">
         <v>45004</v>
       </c>
-      <c r="O101" s="161">
+      <c r="P101" s="161">
         <v>2.4416330404311126E-2</v>
       </c>
-      <c r="P101" s="159">
+      <c r="Q101" s="159">
         <v>5.3520596246249996E-2</v>
       </c>
-      <c r="Q101" s="160">
+      <c r="R101" s="160">
         <v>2.4416330404311126</v>
       </c>
-      <c r="R101" s="161">
+      <c r="S101" s="161">
         <v>1.4081816066250001E-2</v>
       </c>
-      <c r="S101" s="160">
+      <c r="T101" s="160">
         <v>0.64241861616104012</v>
       </c>
     </row>
-    <row r="102" spans="13:19" x14ac:dyDescent="0.3">
+    <row r="102" spans="13:20" x14ac:dyDescent="0.3">
       <c r="M102" s="157" t="s">
         <v>40</v>
       </c>
-      <c r="N102" s="162">
+      <c r="N102" s="157"/>
+      <c r="O102" s="162">
         <v>45045</v>
       </c>
-      <c r="O102" s="161">
+      <c r="P102" s="161">
         <v>3.0669633617302388E-2</v>
       </c>
-      <c r="P102" s="159">
+      <c r="Q102" s="159">
         <v>6.6737122751250003E-2</v>
       </c>
-      <c r="Q102" s="160">
+      <c r="R102" s="160">
         <v>3.066963361730239</v>
       </c>
-      <c r="R102" s="161">
+      <c r="S102" s="161">
         <v>1.13404762040625E-2</v>
       </c>
-      <c r="S102" s="160">
+      <c r="T102" s="160">
         <v>0.52116159026022513</v>
       </c>
     </row>
-    <row r="103" spans="13:19" x14ac:dyDescent="0.3">
+    <row r="103" spans="13:20" x14ac:dyDescent="0.3">
       <c r="M103" s="157" t="s">
         <v>59</v>
       </c>
-      <c r="N103" s="162">
+      <c r="N103" s="157"/>
+      <c r="O103" s="162">
         <v>45100</v>
       </c>
-      <c r="O103" s="161">
+      <c r="P103" s="161">
         <v>2.2105599118509095E-2</v>
       </c>
-      <c r="P103" s="159">
+      <c r="Q103" s="159">
         <v>4.1293259153374992E-2</v>
       </c>
-      <c r="Q103" s="160">
+      <c r="R103" s="160">
         <v>2.2105599118509094</v>
       </c>
-      <c r="R103" s="161">
+      <c r="S103" s="161">
         <v>3.2440670218124995E-3</v>
       </c>
-      <c r="S103" s="160">
+      <c r="T103" s="160">
         <v>0.17366525812700745</v>
       </c>
     </row>
-    <row r="104" spans="13:19" x14ac:dyDescent="0.3">
+    <row r="104" spans="13:20" x14ac:dyDescent="0.3">
       <c r="M104" s="157" t="s">
         <v>68</v>
       </c>
-      <c r="N104" s="162">
+      <c r="N104" s="157"/>
+      <c r="O104" s="162">
         <v>45120</v>
       </c>
-      <c r="O104" s="161">
+      <c r="P104" s="161">
         <v>1.2289907989089242E-2</v>
       </c>
-      <c r="P104" s="159">
+      <c r="Q104" s="159">
         <v>2.5132861837687499E-2</v>
       </c>
-      <c r="Q104" s="160">
+      <c r="R104" s="160">
         <v>1.2289907989089242</v>
       </c>
-      <c r="R104" s="161">
+      <c r="S104" s="161">
         <v>6.0400620675000009E-3</v>
       </c>
-      <c r="S104" s="160">
+      <c r="T104" s="160">
         <v>0.29535755831295851</v>
       </c>
     </row>
-    <row r="105" spans="13:19" x14ac:dyDescent="0.3">
+    <row r="105" spans="13:20" x14ac:dyDescent="0.3">
       <c r="M105" s="157" t="s">
         <v>45</v>
       </c>
-      <c r="N105" s="162">
+      <c r="N105" s="157"/>
+      <c r="O105" s="162">
         <v>45134</v>
       </c>
-      <c r="O105" s="161">
+      <c r="P105" s="161">
         <v>4.1529324627726745E-2</v>
       </c>
-      <c r="P105" s="159">
+      <c r="Q105" s="159">
         <v>7.2344083501499984E-2</v>
       </c>
-      <c r="Q105" s="160">
+      <c r="R105" s="160">
         <v>4.1529324627726742</v>
       </c>
-      <c r="R105" s="161">
+      <c r="S105" s="161">
         <v>1.59767045325E-2</v>
       </c>
-      <c r="S105" s="160">
+      <c r="T105" s="160">
         <v>0.91714721770952934</v>
       </c>
     </row>
@@ -37332,7 +37462,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{83E4E41D-CCD8-4B95-AB4C-B35F3B4D4374}">
   <dimension ref="A1:AA149"/>
   <sheetViews>
-    <sheetView topLeftCell="O46" zoomScale="83" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="J1" zoomScale="83" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="AI60" sqref="AI60"/>
     </sheetView>
   </sheetViews>
@@ -45157,7 +45287,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B9518CF0-901B-4257-8749-E67B3F2BB51B}">
   <dimension ref="B1:AP76"/>
   <sheetViews>
-    <sheetView topLeftCell="S1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView topLeftCell="A52" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="AS22" sqref="AS22"/>
     </sheetView>
   </sheetViews>
@@ -48033,7 +48163,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C9262DC-E5B7-49F4-A43F-DEF8C5BFDEDE}">
   <dimension ref="A1:V48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C27" workbookViewId="0">
+    <sheetView topLeftCell="A11" workbookViewId="0">
       <selection activeCell="Q37" sqref="Q37"/>
     </sheetView>
   </sheetViews>

</xml_diff>